<commit_message>
Test with optimx and nlminb
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\R_working_dir\CKMR\LemonSharkCKMR_GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swens\Documents\R\R_working_dir\LemonSharkCKMR_GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B3846-3DE6-4257-84D8-81FD38E7E339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB080EE-D3C0-4078-B00B-3D37345AE2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Date run</t>
   </si>
@@ -270,6 +270,15 @@
   <si>
     <t>Setting the seed to a random number each loop.;
 Also, change the location of the Truth calculation so it's after mating but before mortality</t>
+  </si>
+  <si>
+    <t>CKMR_DoviIBS_Lemon_sharks_AvgN_6yrs_06.07.2021_Lemon_CB_rmvTry.R</t>
+  </si>
+  <si>
+    <t>Dovi_IBS_model_validation\Lemon_sharks\results\testing</t>
+  </si>
+  <si>
+    <t>Charlotte fixed the script! But she included a "try" section because errors were popping up occasionally. Here, I removed the "try" clause and saved each seed to see if the code runs and if it doesn't, then I can use the seed to trace the error back and figure out what happened.</t>
   </si>
 </sst>
 </file>
@@ -894,9 +903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,14 +1266,28 @@
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12">
+        <v>44354</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Add script to test successful breeding
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\R_working_dir\CKMR\LemonSharkCKMR_GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6C667F-D408-436B-95BE-5D6A691020DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD99426-4590-41C9-9A1F-203432EB594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Script_tracking" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="94">
   <si>
     <t>Date run</t>
   </si>
@@ -396,10 +396,25 @@
     <t>021_DoviIBS_LS_07.06.2021_neutral_lambda_SB_TM.R</t>
   </si>
   <si>
-    <t>TM</t>
-  </si>
-  <si>
-    <t>Tailored model. Means the CKMR model (with lambda parameter) was adapted to account for the process being tested with simulation (e.g. skipped-breeding)</t>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>Adapted model. Means the CKMR model (with lambda parameter) was adapted to account for the process being tested with simulation (e.g. skipped-breeding)</t>
+  </si>
+  <si>
+    <t>022_DoviIBS_LS_08.11.2021_SB_AM_estimate_lambda</t>
+  </si>
+  <si>
+    <t>This script attempts to estimate lambda along with abundance, while accounting for skipped breeding.</t>
+  </si>
+  <si>
+    <t>Couldn't estimate lambda; it was confounded by the abundance estimate.</t>
+  </si>
+  <si>
+    <t>023_DoviIBS_LS_10.11.2021_neutral_lambda_SB_AM_failed_breeders</t>
+  </si>
+  <si>
+    <t>What happens when a certain percentage of females fail to breed? Will the model still work?</t>
   </si>
 </sst>
 </file>
@@ -1095,9 +1110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1120,7 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.7109375" customWidth="1"/>
@@ -1605,25 +1620,51 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="34">
+        <v>44419</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>89</v>
+      </c>
       <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="G21" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="37" t="s">
+        <v>91</v>
+      </c>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="34">
+        <v>44480</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
+      <c r="G22" s="37" t="s">
+        <v>93</v>
+      </c>
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
     </row>
@@ -1670,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reorganize file structure for Bayesian framework.
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\R_working_dir\CKMR\LemonSharkCKMR_GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\CKMR\LemonSharkCKMR_GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD99426-4590-41C9-9A1F-203432EB594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6FEC4B-7E2E-44BD-8C97-D22B11B2B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Script_tracking" sheetId="1" r:id="rId1"/>
-    <sheet name="Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
+    <sheet name="Frequentist_scripts" sheetId="1" r:id="rId2"/>
+    <sheet name="Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="130">
   <si>
     <t>Date run</t>
   </si>
@@ -297,10 +298,6 @@
     <t>skipped-breeding</t>
   </si>
   <si>
-    <t>The naming of the scripts has evolved as I've been keeping this doucment, so some of the names have changed.
-In newer (~07/06/2021) scripts, I started using abbreviations (see right)</t>
-  </si>
-  <si>
     <t>NM</t>
   </si>
   <si>
@@ -415,6 +412,119 @@
   </si>
   <si>
     <t>What happens when a certain percentage of females fail to breed? Will the model still work?</t>
+  </si>
+  <si>
+    <t>The naming of the scripts has evolved as I've been keeping this document, so some of the names have changed.
+In newer (~07/06/2021) scripts, I started using abbreviations (see right)</t>
+  </si>
+  <si>
+    <t>Years sampled</t>
+  </si>
+  <si>
+    <t>Fixed parameters</t>
+  </si>
+  <si>
+    <t>Estimated parameters</t>
+  </si>
+  <si>
+    <t>skipped-breeding?</t>
+  </si>
+  <si>
+    <t>Overall Outcome</t>
+  </si>
+  <si>
+    <t>Priors</t>
+  </si>
+  <si>
+    <t>% pop sampled 1</t>
+  </si>
+  <si>
+    <t>% pop sampled 2</t>
+  </si>
+  <si>
+    <t>% pop sampled 3</t>
+  </si>
+  <si>
+    <t>% in posterior predictive interval 3</t>
+  </si>
+  <si>
+    <t>% in posterior predictive interval 2</t>
+  </si>
+  <si>
+    <t>% in posterior predictive interval 1</t>
+  </si>
+  <si>
+    <t>Script run</t>
+  </si>
+  <si>
+    <t>001_neutralGrowth_estN_2021.10.20.R</t>
+  </si>
+  <si>
+    <t>001_negGrowth_estN_2021.10.20.R</t>
+  </si>
+  <si>
+    <t>001_posGrowth_estN_2021.10.20.R</t>
+  </si>
+  <si>
+    <t>01_IBS\results\Lemon_Shark_life_history\model_validation</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>survival,lambda</t>
+  </si>
+  <si>
+    <t>Nf,Nm</t>
+  </si>
+  <si>
+    <t>dnorm(0, 1.0E-6),dnorm(0, 1.0E-6)</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Test whether the Bayesian framework works</t>
+  </si>
+  <si>
+    <t>002_neutralGrowth_estN_2021.10.27.R</t>
+  </si>
+  <si>
+    <t>003_neutralGrowth_estNSurv_2021.11.04</t>
+  </si>
+  <si>
+    <t>004_neutralGrowth_estNSurvLam_2021.11.04</t>
+  </si>
+  <si>
+    <t>Export functions to streamline script</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Nf,Nm,survival</t>
+  </si>
+  <si>
+    <t>Nf,Nm,survival,lambda</t>
+  </si>
+  <si>
+    <t>dnorm(0, 1.0E-6),dnorm(0, 1.0E-6),dbeta(1 ,1)</t>
+  </si>
+  <si>
+    <t>dnorm(0, 1.0E-6),dnorm(0, 1.0E-6),dbeta(1 ,1),dnorm(0, 1.0E-6)</t>
+  </si>
+  <si>
+    <t>Test whether the model can estimate survival jointly with abundance</t>
+  </si>
+  <si>
+    <t>It can!</t>
+  </si>
+  <si>
+    <t>This is the fundamental model I will be working from.
+Copied to a script called "base_model" in the main directory.</t>
   </si>
 </sst>
 </file>
@@ -446,7 +556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,8 +569,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -719,11 +853,463 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -792,6 +1378,177 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1107,11 +1864,1055 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
+  <dimension ref="A1:R43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="9" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="39.7109375" customWidth="1"/>
+    <col min="18" max="18" width="49.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="116" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="122" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="134" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="116" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q1" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" s="46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="139" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="50">
+        <v>44489</v>
+      </c>
+      <c r="D2" s="111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="98">
+        <v>6</v>
+      </c>
+      <c r="F2" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="129"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="135" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+    </row>
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="50">
+        <v>44489</v>
+      </c>
+      <c r="D3" s="111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="99">
+        <v>6</v>
+      </c>
+      <c r="F3" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="130"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="135" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="50">
+        <v>44489</v>
+      </c>
+      <c r="D4" s="111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="99">
+        <v>6</v>
+      </c>
+      <c r="F4" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="130"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="135" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="15"/>
+    </row>
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53">
+        <v>44496</v>
+      </c>
+      <c r="D5" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="99">
+        <v>3</v>
+      </c>
+      <c r="F5" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="130"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="136" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53">
+        <v>44504</v>
+      </c>
+      <c r="D6" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="99">
+        <v>1</v>
+      </c>
+      <c r="F6" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="118" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="123" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="130"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="136" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53">
+        <v>44504</v>
+      </c>
+      <c r="D7" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="99">
+        <v>1</v>
+      </c>
+      <c r="F7" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="118" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="123" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="130"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="15"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="136"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="91"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="131"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="136"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="15"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="131"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="136"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="131"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="91"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="136"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="136"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="15"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="56"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="132"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="94"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="38"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="132"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="82"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="137"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="38"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="132"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="137"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="38"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="137"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="38"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="38"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="114"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="94"/>
+      <c r="P20" s="137"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="38"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="132"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="137"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="38"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="126"/>
+      <c r="J22" s="132"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="93"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="137"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="38"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="132"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="93"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="137"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="126"/>
+      <c r="J24" s="132"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="93"/>
+      <c r="O24" s="94"/>
+      <c r="P24" s="137"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="38"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="120"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="132"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="94"/>
+      <c r="P25" s="137"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="38"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="120"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="132"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="83"/>
+      <c r="N26" s="93"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="137"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="38"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="132"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="93"/>
+      <c r="O27" s="94"/>
+      <c r="P27" s="137"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="38"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="114"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="120"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="132"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="83"/>
+      <c r="N28" s="93"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="137"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="38"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="120"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="132"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="83"/>
+      <c r="N29" s="93"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="137"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="38"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="126"/>
+      <c r="J30" s="132"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="83"/>
+      <c r="N30" s="93"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="137"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="38"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="120"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="126"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="137"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="38"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="120"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="126"/>
+      <c r="J32" s="132"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="83"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="137"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="38"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="59"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="120"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="137"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="38"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="126"/>
+      <c r="J34" s="132"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="137"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="38"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="59"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="114"/>
+      <c r="E35" s="101"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="126"/>
+      <c r="J35" s="132"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="93"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="137"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="38"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="59"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="132"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="83"/>
+      <c r="N36" s="93"/>
+      <c r="O36" s="94"/>
+      <c r="P36" s="137"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="38"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="59"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="114"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="126"/>
+      <c r="J37" s="132"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="94"/>
+      <c r="P37" s="137"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="38"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="114"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="126"/>
+      <c r="J38" s="132"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
+      <c r="N38" s="93"/>
+      <c r="O38" s="94"/>
+      <c r="P38" s="137"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="38"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="59"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="120"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="126"/>
+      <c r="J39" s="132"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="83"/>
+      <c r="N39" s="93"/>
+      <c r="O39" s="94"/>
+      <c r="P39" s="137"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="38"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="59"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="114"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="126"/>
+      <c r="J40" s="132"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="83"/>
+      <c r="N40" s="93"/>
+      <c r="O40" s="94"/>
+      <c r="P40" s="137"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="38"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="59"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="126"/>
+      <c r="J41" s="132"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="83"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="94"/>
+      <c r="P41" s="137"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="38"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="59"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="126"/>
+      <c r="J42" s="132"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="83"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="94"/>
+      <c r="P42" s="137"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="38"/>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="60"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="109"/>
+      <c r="G43" s="121"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="127"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="84"/>
+      <c r="M43" s="85"/>
+      <c r="N43" s="95"/>
+      <c r="O43" s="96"/>
+      <c r="P43" s="138"/>
+      <c r="Q43" s="140"/>
+      <c r="R43" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1238,7 +3039,7 @@
         <v>44328</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>31</v>
@@ -1265,7 +3066,7 @@
         <v>44328</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>32</v>
@@ -1290,7 +3091,7 @@
         <v>44330</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>23</v>
@@ -1315,7 +3116,7 @@
         <v>44333</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>33</v>
@@ -1344,7 +3145,7 @@
         <v>44336</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>41</v>
@@ -1371,7 +3172,7 @@
         <v>44341</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>44</v>
@@ -1394,7 +3195,7 @@
         <v>44342</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="14" t="s">
@@ -1417,7 +3218,7 @@
         <v>44342</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="14" t="s">
@@ -1453,7 +3254,7 @@
         <v>44354</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>48</v>
@@ -1478,7 +3279,7 @@
         <v>44356</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>50</v>
@@ -1505,7 +3306,7 @@
         <v>44356</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>50</v>
@@ -1532,7 +3333,7 @@
         <v>44368</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>55</v>
@@ -1557,16 +3358,16 @@
         <v>44369</v>
       </c>
       <c r="E18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>79</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>80</v>
       </c>
       <c r="G18" s="37" t="s">
         <v>57</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" s="38"/>
     </row>
@@ -1584,16 +3385,16 @@
         <v>44383</v>
       </c>
       <c r="E19" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="G19" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="37" t="s">
-        <v>83</v>
-      </c>
       <c r="H19" s="37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I19" s="38"/>
     </row>
@@ -1611,10 +3412,10 @@
         <v>44384</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
@@ -1634,14 +3435,14 @@
         <v>44419</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="36"/>
       <c r="G21" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="37" t="s">
         <v>90</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>91</v>
       </c>
       <c r="I21" s="38"/>
     </row>
@@ -1659,11 +3460,11 @@
         <v>44480</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
@@ -1707,12 +3508,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +3536,7 @@
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -1754,18 +3555,18 @@
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update file structure 3
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\CKMR\LemonSharkCKMR_GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6FEC4B-7E2E-44BD-8C97-D22B11B2B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC5DE7-73CF-4605-8E54-954505AEADE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   </si>
   <si>
     <t>This is the fundamental model I will be working from.
-Copied to a script called "base_model" in the main directory.</t>
+Copied to a script called "base_model" in the MAIN_scripts folder</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1869,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add POP pairwise comparison matrix
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E47047-D5F4-4EF9-942F-E18812E3CD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612859D9-DC51-4CD0-B99B-9762977B6089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="3645" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="142">
   <si>
     <t>Date run</t>
   </si>
@@ -537,6 +537,30 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>base_simulation_and_model_UPDATED_HS.PO</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Start incorporating POP likelihood into framework</t>
+  </si>
+  <si>
+    <t>First, adjusting pairwise comparison matrix to exclude comparisons that cannot produce a PO match.</t>
+  </si>
+  <si>
+    <t>TBD (as of 12/19/2021)</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1414,7 +1438,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1881,7 +1904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,46 +1935,46 @@
       <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="115" t="s">
         <v>95</v>
       </c>
       <c r="I1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="122" t="s">
+      <c r="J1" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="128" t="s">
+      <c r="K1" s="127" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="75" t="s">
+      <c r="N1" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="86" t="s">
+      <c r="O1" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="134" t="s">
+      <c r="P1" s="133" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="116" t="s">
+      <c r="Q1" s="115" t="s">
         <v>115</v>
       </c>
       <c r="R1" s="42" t="s">
@@ -1962,8 +1985,8 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="139"/>
-      <c r="B2" s="139" t="s">
+      <c r="A2" s="138"/>
+      <c r="B2" s="138" t="s">
         <v>107</v>
       </c>
       <c r="C2" s="49" t="s">
@@ -1972,31 +1995,31 @@
       <c r="D2" s="50">
         <v>44489</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="98">
+      <c r="F2" s="97">
         <v>6</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="117" t="s">
+      <c r="H2" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="123" t="s">
+      <c r="J2" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="129"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="135" t="s">
+      <c r="K2" s="128"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="134" t="s">
         <v>116</v>
       </c>
       <c r="R2" s="40"/>
@@ -2013,31 +2036,31 @@
       <c r="D3" s="50">
         <v>44489</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="99">
+      <c r="F3" s="98">
         <v>6</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="G3" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="117" t="s">
+      <c r="H3" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="123" t="s">
+      <c r="J3" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="K3" s="130"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="135" t="s">
+      <c r="K3" s="129"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="134" t="s">
         <v>116</v>
       </c>
       <c r="R3" s="28"/>
@@ -2054,31 +2077,31 @@
       <c r="D4" s="50">
         <v>44489</v>
       </c>
-      <c r="E4" s="111" t="s">
+      <c r="E4" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="98">
         <v>6</v>
       </c>
-      <c r="G4" s="106" t="s">
+      <c r="G4" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="117" t="s">
+      <c r="H4" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="123" t="s">
+      <c r="J4" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="K4" s="130"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="135" t="s">
+      <c r="K4" s="129"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="134" t="s">
         <v>116</v>
       </c>
       <c r="R4" s="28"/>
@@ -2093,31 +2116,31 @@
       <c r="D5" s="53">
         <v>44496</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="98">
         <v>3</v>
       </c>
-      <c r="G5" s="106" t="s">
+      <c r="G5" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="117" t="s">
+      <c r="H5" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="123" t="s">
+      <c r="J5" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="K5" s="130"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="136" t="s">
+      <c r="K5" s="129"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="135" t="s">
         <v>120</v>
       </c>
       <c r="R5" s="28"/>
@@ -2132,31 +2155,31 @@
       <c r="D6" s="53">
         <v>44504</v>
       </c>
-      <c r="E6" s="112" t="s">
+      <c r="E6" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="99">
+      <c r="F6" s="98">
         <v>1</v>
       </c>
-      <c r="G6" s="106" t="s">
+      <c r="G6" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="118" t="s">
+      <c r="H6" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="70" t="s">
+      <c r="I6" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="123" t="s">
+      <c r="J6" s="122" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="130"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="89"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="136" t="s">
+      <c r="K6" s="129"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="135" t="s">
         <v>127</v>
       </c>
       <c r="R6" s="28" t="s">
@@ -2175,31 +2198,31 @@
       <c r="D7" s="53">
         <v>44504</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="99">
+      <c r="F7" s="98">
         <v>1</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="70" t="s">
+      <c r="I7" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="J7" s="123" t="s">
+      <c r="J7" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="K7" s="130"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="136"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="135"/>
       <c r="R7" s="28"/>
       <c r="S7" s="15"/>
     </row>
@@ -2210,19 +2233,19 @@
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="130"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="136"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="89"/>
+      <c r="Q8" s="135"/>
       <c r="R8" s="28"/>
       <c r="S8" s="15"/>
     </row>
@@ -2235,73 +2258,93 @@
       <c r="D9" s="53">
         <v>44545</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="100">
+      <c r="F9" s="99">
         <v>1</v>
       </c>
-      <c r="G9" s="107" t="s">
+      <c r="G9" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="119" t="s">
+      <c r="H9" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="I9" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="J9" s="123" t="s">
+      <c r="J9" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="131"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="92"/>
-      <c r="Q9" s="136"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="91"/>
+      <c r="Q9" s="135"/>
       <c r="R9" s="28"/>
       <c r="S9" s="15"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
+      <c r="B10" s="52" t="s">
+        <v>134</v>
+      </c>
       <c r="C10" s="52"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="91"/>
-      <c r="P10" s="92"/>
-      <c r="Q10" s="136"/>
+      <c r="D10" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="99">
+        <v>1</v>
+      </c>
+      <c r="G10" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="118" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="122" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="130"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="135" t="s">
+        <v>139</v>
+      </c>
       <c r="R10" s="28"/>
-      <c r="S10" s="15"/>
+      <c r="S10" s="15" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="52"/>
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
       <c r="D11" s="53"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="125"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="91"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="136"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="130"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="135"/>
       <c r="R11" s="28"/>
       <c r="S11" s="15"/>
     </row>
@@ -2310,19 +2353,19 @@
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="53"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="125"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="91"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="136"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="130"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="91"/>
+      <c r="Q12" s="135"/>
       <c r="R12" s="28"/>
       <c r="S12" s="15"/>
     </row>
@@ -2331,650 +2374,650 @@
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
       <c r="D13" s="53"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="125"/>
-      <c r="K13" s="131"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="91"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="136"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="90"/>
+      <c r="P13" s="91"/>
+      <c r="Q13" s="135"/>
       <c r="R13" s="28"/>
       <c r="S13" s="15"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="52"/>
       <c r="D14" s="53"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="125"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="92"/>
-      <c r="Q14" s="136"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="130"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="135"/>
       <c r="R14" s="28"/>
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="56"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="126"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="137"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="125"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="136"/>
       <c r="R15" s="43"/>
       <c r="S15" s="38"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="126"/>
-      <c r="K16" s="132"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="83"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="94"/>
-      <c r="Q16" s="137"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="125"/>
+      <c r="K16" s="131"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="136"/>
       <c r="R16" s="43"/>
       <c r="S16" s="38"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="126"/>
-      <c r="K17" s="132"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="83"/>
-      <c r="O17" s="93"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="137"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="125"/>
+      <c r="K17" s="131"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="136"/>
       <c r="R17" s="43"/>
       <c r="S17" s="38"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="126"/>
-      <c r="K18" s="132"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="93"/>
-      <c r="P18" s="94"/>
-      <c r="Q18" s="137"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="125"/>
+      <c r="K18" s="131"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="92"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="136"/>
       <c r="R18" s="43"/>
       <c r="S18" s="38"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="126"/>
-      <c r="K19" s="132"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="93"/>
-      <c r="P19" s="94"/>
-      <c r="Q19" s="137"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="136"/>
       <c r="R19" s="43"/>
       <c r="S19" s="38"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="108"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="126"/>
-      <c r="K20" s="132"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="93"/>
-      <c r="P20" s="94"/>
-      <c r="Q20" s="137"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="119"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="125"/>
+      <c r="K20" s="131"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="92"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="136"/>
       <c r="R20" s="43"/>
       <c r="S20" s="38"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="126"/>
-      <c r="K21" s="132"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="94"/>
-      <c r="Q21" s="137"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="119"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="131"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="81"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="92"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="136"/>
       <c r="R21" s="43"/>
       <c r="S21" s="38"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="126"/>
-      <c r="K22" s="132"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="93"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="137"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="125"/>
+      <c r="K22" s="131"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="92"/>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="136"/>
       <c r="R22" s="43"/>
       <c r="S22" s="38"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="126"/>
-      <c r="K23" s="132"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="93"/>
-      <c r="P23" s="94"/>
-      <c r="Q23" s="137"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="131"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="81"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="92"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="136"/>
       <c r="R23" s="43"/>
       <c r="S23" s="38"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="108"/>
-      <c r="H24" s="120"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="132"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="82"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="93"/>
-      <c r="P24" s="94"/>
-      <c r="Q24" s="137"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="125"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="92"/>
+      <c r="P24" s="93"/>
+      <c r="Q24" s="136"/>
       <c r="R24" s="43"/>
       <c r="S24" s="38"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="120"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="126"/>
-      <c r="K25" s="132"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="93"/>
-      <c r="P25" s="94"/>
-      <c r="Q25" s="137"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="119"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="131"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="81"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="92"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="136"/>
       <c r="R25" s="43"/>
       <c r="S25" s="38"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="108"/>
-      <c r="H26" s="120"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="132"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="82"/>
-      <c r="N26" s="83"/>
-      <c r="O26" s="93"/>
-      <c r="P26" s="94"/>
-      <c r="Q26" s="137"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="125"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="66"/>
+      <c r="M26" s="81"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="92"/>
+      <c r="P26" s="93"/>
+      <c r="Q26" s="136"/>
       <c r="R26" s="43"/>
       <c r="S26" s="38"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="120"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="126"/>
-      <c r="K27" s="132"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="82"/>
-      <c r="N27" s="83"/>
-      <c r="O27" s="93"/>
-      <c r="P27" s="94"/>
-      <c r="Q27" s="137"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="119"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="81"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="92"/>
+      <c r="P27" s="93"/>
+      <c r="Q27" s="136"/>
       <c r="R27" s="43"/>
       <c r="S27" s="38"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="108"/>
-      <c r="H28" s="120"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="126"/>
-      <c r="K28" s="132"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="82"/>
-      <c r="N28" s="83"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="94"/>
-      <c r="Q28" s="137"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="92"/>
+      <c r="P28" s="93"/>
+      <c r="Q28" s="136"/>
       <c r="R28" s="43"/>
       <c r="S28" s="38"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="114"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="120"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="126"/>
-      <c r="K29" s="132"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="82"/>
-      <c r="N29" s="83"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="94"/>
-      <c r="Q29" s="137"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="107"/>
+      <c r="H29" s="119"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="125"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="92"/>
+      <c r="P29" s="93"/>
+      <c r="Q29" s="136"/>
       <c r="R29" s="43"/>
       <c r="S29" s="38"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="108"/>
-      <c r="H30" s="120"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="126"/>
-      <c r="K30" s="132"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="83"/>
-      <c r="O30" s="93"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="137"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="100"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="125"/>
+      <c r="K30" s="131"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="92"/>
+      <c r="P30" s="93"/>
+      <c r="Q30" s="136"/>
       <c r="R30" s="43"/>
       <c r="S30" s="38"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="108"/>
-      <c r="H31" s="120"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="126"/>
-      <c r="K31" s="132"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="82"/>
-      <c r="N31" s="83"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="94"/>
-      <c r="Q31" s="137"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="107"/>
+      <c r="H31" s="119"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="125"/>
+      <c r="K31" s="131"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="81"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="136"/>
       <c r="R31" s="43"/>
       <c r="S31" s="38"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="108"/>
-      <c r="H32" s="120"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="126"/>
-      <c r="K32" s="132"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="83"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="94"/>
-      <c r="Q32" s="137"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="107"/>
+      <c r="H32" s="119"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="125"/>
+      <c r="K32" s="131"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="81"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="92"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="136"/>
       <c r="R32" s="43"/>
       <c r="S32" s="38"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="108"/>
-      <c r="H33" s="120"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="126"/>
-      <c r="K33" s="132"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="82"/>
-      <c r="N33" s="83"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="137"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="113"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="119"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="125"/>
+      <c r="K33" s="131"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="81"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="92"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="136"/>
       <c r="R33" s="43"/>
       <c r="S33" s="38"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="108"/>
-      <c r="H34" s="120"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="126"/>
-      <c r="K34" s="132"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="83"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="94"/>
-      <c r="Q34" s="137"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="107"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="131"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="82"/>
+      <c r="O34" s="92"/>
+      <c r="P34" s="93"/>
+      <c r="Q34" s="136"/>
       <c r="R34" s="43"/>
       <c r="S34" s="38"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="59"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="120"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="126"/>
-      <c r="K35" s="132"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="82"/>
-      <c r="N35" s="83"/>
-      <c r="O35" s="93"/>
-      <c r="P35" s="94"/>
-      <c r="Q35" s="137"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="131"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="82"/>
+      <c r="O35" s="92"/>
+      <c r="P35" s="93"/>
+      <c r="Q35" s="136"/>
       <c r="R35" s="43"/>
       <c r="S35" s="38"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="59"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="108"/>
-      <c r="H36" s="120"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="126"/>
-      <c r="K36" s="132"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="82"/>
-      <c r="N36" s="83"/>
-      <c r="O36" s="93"/>
-      <c r="P36" s="94"/>
-      <c r="Q36" s="137"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="100"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="125"/>
+      <c r="K36" s="131"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="81"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="92"/>
+      <c r="P36" s="93"/>
+      <c r="Q36" s="136"/>
       <c r="R36" s="43"/>
       <c r="S36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="59"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="114"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="120"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="126"/>
-      <c r="K37" s="132"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="82"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="93"/>
-      <c r="P37" s="94"/>
-      <c r="Q37" s="137"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="107"/>
+      <c r="H37" s="119"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="131"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="92"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="136"/>
       <c r="R37" s="43"/>
       <c r="S37" s="38"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38" s="59"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="114"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="108"/>
-      <c r="H38" s="120"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="126"/>
-      <c r="K38" s="132"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="83"/>
-      <c r="O38" s="93"/>
-      <c r="P38" s="94"/>
-      <c r="Q38" s="137"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="107"/>
+      <c r="H38" s="119"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="125"/>
+      <c r="K38" s="131"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="81"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="92"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="136"/>
       <c r="R38" s="43"/>
       <c r="S38" s="38"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" s="59"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="114"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="108"/>
-      <c r="H39" s="120"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="126"/>
-      <c r="K39" s="132"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="82"/>
-      <c r="N39" s="83"/>
-      <c r="O39" s="93"/>
-      <c r="P39" s="94"/>
-      <c r="Q39" s="137"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="100"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="119"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="125"/>
+      <c r="K39" s="131"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="81"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="92"/>
+      <c r="P39" s="93"/>
+      <c r="Q39" s="136"/>
       <c r="R39" s="43"/>
       <c r="S39" s="38"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" s="59"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="114"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="108"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="126"/>
-      <c r="K40" s="132"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="82"/>
-      <c r="N40" s="83"/>
-      <c r="O40" s="93"/>
-      <c r="P40" s="94"/>
-      <c r="Q40" s="137"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="107"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="125"/>
+      <c r="K40" s="131"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="81"/>
+      <c r="N40" s="82"/>
+      <c r="O40" s="92"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="136"/>
       <c r="R40" s="43"/>
       <c r="S40" s="38"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="59"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="101"/>
-      <c r="G41" s="108"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="126"/>
-      <c r="K41" s="132"/>
-      <c r="L41" s="67"/>
-      <c r="M41" s="82"/>
-      <c r="N41" s="83"/>
-      <c r="O41" s="93"/>
-      <c r="P41" s="94"/>
-      <c r="Q41" s="137"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="92"/>
+      <c r="P41" s="93"/>
+      <c r="Q41" s="136"/>
       <c r="R41" s="43"/>
       <c r="S41" s="38"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="59"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="114"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="108"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="126"/>
-      <c r="K42" s="132"/>
-      <c r="L42" s="67"/>
-      <c r="M42" s="82"/>
-      <c r="N42" s="83"/>
-      <c r="O42" s="93"/>
-      <c r="P42" s="94"/>
-      <c r="Q42" s="137"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="107"/>
+      <c r="H42" s="119"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="125"/>
+      <c r="K42" s="131"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="82"/>
+      <c r="O42" s="92"/>
+      <c r="P42" s="93"/>
+      <c r="Q42" s="136"/>
       <c r="R42" s="43"/>
       <c r="S42" s="38"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="115"/>
-      <c r="F43" s="102"/>
-      <c r="G43" s="109"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="73"/>
-      <c r="J43" s="127"/>
-      <c r="K43" s="133"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="84"/>
-      <c r="N43" s="85"/>
-      <c r="O43" s="95"/>
-      <c r="P43" s="96"/>
-      <c r="Q43" s="138"/>
-      <c r="R43" s="140"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="101"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="120"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="126"/>
+      <c r="K43" s="132"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="83"/>
+      <c r="N43" s="84"/>
+      <c r="O43" s="94"/>
+      <c r="P43" s="95"/>
+      <c r="Q43" s="137"/>
+      <c r="R43" s="139"/>
       <c r="S43" s="44"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HS/PO yearly model -- doesn't work
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612859D9-DC51-4CD0-B99B-9762977B6089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2B363-1720-400B-B13D-02D99B739814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
   <si>
     <t>Date run</t>
   </si>
@@ -542,25 +542,41 @@
     <t>base_simulation_and_model_UPDATED_HS.PO</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Start incorporating POP likelihood into framework</t>
-  </si>
-  <si>
     <t>First, adjusting pairwise comparison matrix to exclude comparisons that cannot produce a PO match.</t>
   </si>
   <si>
     <t>TBD (as of 12/19/2021)</t>
+  </si>
+  <si>
+    <t>base_simulation_and_model_UPDATED</t>
+  </si>
+  <si>
+    <t>Run completed?</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>run but not analyzed</t>
+  </si>
+  <si>
+    <t>analysis complete</t>
+  </si>
+  <si>
+    <t>Results prefix</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Results heavily biased</t>
+  </si>
+  <si>
+    <t>Start incorporating POP likelihood into framework; first try just excluding comparisons that cannot produce a match.</t>
+  </si>
+  <si>
+    <t>Use new seeds and save additional output files (e.g. dataframes of samples and #of offspring per parent per year).
+Everything else was the same (e.g. sample size, sample years)</t>
   </si>
 </sst>
 </file>
@@ -630,7 +646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -925,17 +941,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="dashed">
         <color indexed="64"/>
       </left>
@@ -967,17 +972,6 @@
       <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1040,8 +1034,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1053,7 +1049,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="hair">
@@ -1068,10 +1064,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1083,12 +1079,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1098,25 +1092,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
+      <right style="dashed">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1126,41 +1105,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="dashed">
         <color indexed="64"/>
       </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="dashed">
         <color indexed="64"/>
       </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="hair">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1172,7 +1151,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="dashed">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1184,156 +1163,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1345,7 +1194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1416,41 +1265,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1460,130 +1283,121 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1900,11 +1714,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,1115 +1726,1244 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="8" width="19.5546875" customWidth="1"/>
-    <col min="9" max="10" width="25.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="39.6640625" customWidth="1"/>
-    <col min="19" max="19" width="49.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" customWidth="1"/>
+    <col min="8" max="8" width="39.6640625" customWidth="1"/>
+    <col min="9" max="9" width="49.6640625" style="39" customWidth="1"/>
+    <col min="10" max="13" width="19.5546875" customWidth="1"/>
+    <col min="14" max="15" width="25.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="106" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="91" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="119" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="106" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" s="81" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="107"/>
+      <c r="B2" s="108" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="110">
+        <v>44489</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="89"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="103" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="104">
+        <v>6</v>
+      </c>
+      <c r="L2" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="104" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="104" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="66"/>
+    </row>
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="111"/>
+      <c r="B3" s="112" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="112">
+        <v>44489</v>
+      </c>
+      <c r="E3" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="83"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="97">
+        <v>6</v>
+      </c>
+      <c r="L3" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="M3" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="68"/>
+    </row>
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="111"/>
+      <c r="B4" s="112" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="112">
+        <v>44489</v>
+      </c>
+      <c r="E4" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="83"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="97">
+        <v>6</v>
+      </c>
+      <c r="L4" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="68"/>
+    </row>
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="113"/>
+      <c r="B5" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="98"/>
+      <c r="D5" s="112">
+        <v>44496</v>
+      </c>
+      <c r="E5" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="84"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="97">
+        <v>3</v>
+      </c>
+      <c r="L5" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="O5" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="68"/>
+    </row>
+    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="113"/>
+      <c r="B6" s="98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="98"/>
+      <c r="D6" s="112">
+        <v>44504</v>
+      </c>
+      <c r="E6" s="94" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="84"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="121" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="97">
         <v>1</v>
       </c>
-      <c r="D1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="109" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="96" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="103" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="115" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="121" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="127" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" s="73" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="74" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="133" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="115" t="s">
-        <v>115</v>
-      </c>
-      <c r="R1" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" s="46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="138"/>
-      <c r="B2" s="138" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="50">
-        <v>44489</v>
-      </c>
-      <c r="E2" s="110" t="s">
+      <c r="L6" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="O6" s="94" t="s">
+        <v>125</v>
+      </c>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="68"/>
+    </row>
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="113"/>
+      <c r="B7" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="98"/>
+      <c r="D7" s="112">
+        <v>44504</v>
+      </c>
+      <c r="E7" s="94"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="97">
-        <v>6</v>
-      </c>
-      <c r="G2" s="104" t="s">
+      <c r="K7" s="97">
+        <v>1</v>
+      </c>
+      <c r="L7" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="116" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="122" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="128"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="134" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="41"/>
-    </row>
-    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="50">
-        <v>44489</v>
-      </c>
-      <c r="E3" s="110" t="s">
+      <c r="M7" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="O7" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="68"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="113"/>
+      <c r="B8" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="98"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="68"/>
+    </row>
+    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="113"/>
+      <c r="B9" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="98"/>
+      <c r="D9" s="112">
+        <v>44545</v>
+      </c>
+      <c r="E9" s="94"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="98">
-        <v>6</v>
-      </c>
-      <c r="G3" s="105" t="s">
+      <c r="K9" s="98">
+        <v>1</v>
+      </c>
+      <c r="L9" s="98" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="N9" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="70"/>
+    </row>
+    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="113"/>
+      <c r="B10" s="98" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="98"/>
+      <c r="D10" s="112" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="94" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" s="121" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="98">
+        <v>1</v>
+      </c>
+      <c r="L10" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="116" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="122" t="s">
-        <v>114</v>
-      </c>
-      <c r="K3" s="129"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="134" t="s">
-        <v>116</v>
-      </c>
-      <c r="R3" s="28"/>
-      <c r="S3" s="15"/>
-    </row>
-    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="50">
-        <v>44489</v>
-      </c>
-      <c r="E4" s="110" t="s">
+      <c r="M10" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="70"/>
+    </row>
+    <row r="11" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="113"/>
+      <c r="B11" s="98" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="98"/>
+      <c r="D11" s="112">
+        <v>44558</v>
+      </c>
+      <c r="E11" s="94" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="98">
-        <v>6</v>
-      </c>
-      <c r="G4" s="105" t="s">
+      <c r="K11" s="98">
+        <v>1</v>
+      </c>
+      <c r="L11" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="116" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="J4" s="122" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" s="129"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="134" t="s">
-        <v>116</v>
-      </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="15"/>
-    </row>
-    <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53">
-        <v>44496</v>
-      </c>
-      <c r="E5" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="98">
-        <v>3</v>
-      </c>
-      <c r="G5" s="105" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="116" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="J5" s="122" t="s">
-        <v>114</v>
-      </c>
-      <c r="K5" s="129"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="135" t="s">
-        <v>120</v>
-      </c>
-      <c r="R5" s="28"/>
-      <c r="S5" s="15"/>
-    </row>
-    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53">
-        <v>44504</v>
-      </c>
-      <c r="E6" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="98">
-        <v>1</v>
-      </c>
-      <c r="G6" s="105" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="117" t="s">
+      <c r="M11" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="69" t="s">
+      <c r="N11" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="122" t="s">
-        <v>125</v>
-      </c>
-      <c r="K6" s="129"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="135" t="s">
-        <v>127</v>
-      </c>
-      <c r="R6" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53">
-        <v>44504</v>
-      </c>
-      <c r="E7" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="98">
-        <v>1</v>
-      </c>
-      <c r="G7" s="105" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="117" t="s">
-        <v>122</v>
-      </c>
-      <c r="I7" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" s="122" t="s">
+      <c r="O11" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="K7" s="129"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="15"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="117"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="135"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="15"/>
-    </row>
-    <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53">
-        <v>44545</v>
-      </c>
-      <c r="E9" s="112" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="99">
-        <v>1</v>
-      </c>
-      <c r="G9" s="106" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="118" t="s">
-        <v>121</v>
-      </c>
-      <c r="I9" s="70" t="s">
-        <v>123</v>
-      </c>
-      <c r="J9" s="122" t="s">
-        <v>126</v>
-      </c>
-      <c r="K9" s="130"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="135"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="15"/>
-    </row>
-    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="112" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="99">
-        <v>1</v>
-      </c>
-      <c r="G10" s="106" t="s">
-        <v>111</v>
-      </c>
-      <c r="H10" s="118" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" s="70" t="s">
-        <v>123</v>
-      </c>
-      <c r="J10" s="122" t="s">
-        <v>126</v>
-      </c>
-      <c r="K10" s="130"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="80"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="R10" s="28"/>
-      <c r="S10" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="91"/>
-      <c r="Q11" s="135"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="15"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="130"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="91"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="15"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="135"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="15"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="130"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="15"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="92"/>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="136"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="38"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="119"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="125"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="136"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="38"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="119"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="125"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="92"/>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="38"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="131"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="92"/>
-      <c r="P18" s="93"/>
-      <c r="Q18" s="136"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="38"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="119"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="136"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="38"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="58"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="119"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="125"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="92"/>
-      <c r="P20" s="93"/>
-      <c r="Q20" s="136"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="38"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="119"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="125"/>
-      <c r="K21" s="131"/>
-      <c r="L21" s="66"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="92"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="136"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="38"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="58"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="125"/>
-      <c r="K22" s="131"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="92"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="136"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="38"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="58"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="119"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="125"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="92"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="136"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="38"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="58"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="119"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="125"/>
-      <c r="K24" s="131"/>
-      <c r="L24" s="66"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="82"/>
-      <c r="O24" s="92"/>
-      <c r="P24" s="93"/>
-      <c r="Q24" s="136"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="38"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="58"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="119"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="131"/>
-      <c r="L25" s="66"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="93"/>
-      <c r="Q25" s="136"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="38"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="119"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="125"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="82"/>
-      <c r="O26" s="92"/>
-      <c r="P26" s="93"/>
-      <c r="Q26" s="136"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="38"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="58"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="125"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="81"/>
-      <c r="N27" s="82"/>
-      <c r="O27" s="92"/>
-      <c r="P27" s="93"/>
-      <c r="Q27" s="136"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="38"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="58"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="131"/>
-      <c r="L28" s="66"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="82"/>
-      <c r="O28" s="92"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="136"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="38"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="58"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="119"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="131"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="82"/>
-      <c r="O29" s="92"/>
-      <c r="P29" s="93"/>
-      <c r="Q29" s="136"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="38"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="58"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="113"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="107"/>
-      <c r="H30" s="119"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="131"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="82"/>
-      <c r="O30" s="92"/>
-      <c r="P30" s="93"/>
-      <c r="Q30" s="136"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="38"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="58"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="125"/>
-      <c r="K31" s="131"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="82"/>
-      <c r="O31" s="92"/>
-      <c r="P31" s="93"/>
-      <c r="Q31" s="136"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="38"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="58"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="113"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="119"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="125"/>
-      <c r="K32" s="131"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="81"/>
-      <c r="N32" s="82"/>
-      <c r="O32" s="92"/>
-      <c r="P32" s="93"/>
-      <c r="Q32" s="136"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="38"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="58"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="119"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="125"/>
-      <c r="K33" s="131"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="82"/>
-      <c r="O33" s="92"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="136"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="38"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="131"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="82"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="136"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="38"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="119"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="131"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="82"/>
-      <c r="O35" s="92"/>
-      <c r="P35" s="93"/>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="38"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="58"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="125"/>
-      <c r="K36" s="131"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="81"/>
-      <c r="N36" s="82"/>
-      <c r="O36" s="92"/>
-      <c r="P36" s="93"/>
-      <c r="Q36" s="136"/>
-      <c r="R36" s="43"/>
-      <c r="S36" s="38"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="119"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="125"/>
-      <c r="K37" s="131"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="81"/>
-      <c r="N37" s="82"/>
-      <c r="O37" s="92"/>
-      <c r="P37" s="93"/>
-      <c r="Q37" s="136"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="38"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="100"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="131"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="81"/>
-      <c r="N38" s="82"/>
-      <c r="O38" s="92"/>
-      <c r="P38" s="93"/>
-      <c r="Q38" s="136"/>
-      <c r="R38" s="43"/>
-      <c r="S38" s="38"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" s="58"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="113"/>
-      <c r="F39" s="100"/>
-      <c r="G39" s="107"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="125"/>
-      <c r="K39" s="131"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="82"/>
-      <c r="O39" s="92"/>
-      <c r="P39" s="93"/>
-      <c r="Q39" s="136"/>
-      <c r="R39" s="43"/>
-      <c r="S39" s="38"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" s="58"/>
-      <c r="B40" s="58"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="113"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="125"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="81"/>
-      <c r="N40" s="82"/>
-      <c r="O40" s="92"/>
-      <c r="P40" s="93"/>
-      <c r="Q40" s="136"/>
-      <c r="R40" s="43"/>
-      <c r="S40" s="38"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="58"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="119"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="125"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="81"/>
-      <c r="N41" s="82"/>
-      <c r="O41" s="92"/>
-      <c r="P41" s="93"/>
-      <c r="Q41" s="136"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="38"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="58"/>
-      <c r="B42" s="58"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="107"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="125"/>
-      <c r="K42" s="131"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="81"/>
-      <c r="N42" s="82"/>
-      <c r="O42" s="92"/>
-      <c r="P42" s="93"/>
-      <c r="Q42" s="136"/>
-      <c r="R42" s="43"/>
-      <c r="S42" s="38"/>
-    </row>
-    <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="108"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="132"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="83"/>
-      <c r="N43" s="84"/>
-      <c r="O43" s="94"/>
-      <c r="P43" s="95"/>
-      <c r="Q43" s="137"/>
-      <c r="R43" s="139"/>
-      <c r="S43" s="44"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="70"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="113"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="99"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="70"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="113"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="99"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="70"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="96"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="69"/>
+      <c r="U14" s="70"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="96"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="99"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="72"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="96"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="72"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="114"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="72"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="114"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="99"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="71"/>
+      <c r="U18" s="72"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="114"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="99"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="72"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="114"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="98"/>
+      <c r="O20" s="99"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="60"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="71"/>
+      <c r="U20" s="72"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="114"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="121"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="72"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="114"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="121"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="98"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="98"/>
+      <c r="O22" s="99"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="61"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="72"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="114"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="98"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="99"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="61"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="72"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="114"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="72"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="114"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="96"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="99"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="61"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="72"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="114"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
+      <c r="M26" s="98"/>
+      <c r="N26" s="98"/>
+      <c r="O26" s="99"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="60"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="72"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="114"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="98"/>
+      <c r="N27" s="98"/>
+      <c r="O27" s="99"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="72"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" s="114"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="79"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="61"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="72"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29" s="114"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="98"/>
+      <c r="N29" s="98"/>
+      <c r="O29" s="99"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="61"/>
+      <c r="T29" s="71"/>
+      <c r="U29" s="72"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="114"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="98"/>
+      <c r="O30" s="99"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="71"/>
+      <c r="U30" s="72"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="114"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="121"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="98"/>
+      <c r="L31" s="98"/>
+      <c r="M31" s="98"/>
+      <c r="N31" s="98"/>
+      <c r="O31" s="99"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="61"/>
+      <c r="T31" s="71"/>
+      <c r="U31" s="72"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="114"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="121"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="98"/>
+      <c r="O32" s="99"/>
+      <c r="P32" s="79"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="71"/>
+      <c r="U32" s="72"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33" s="114"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="121"/>
+      <c r="J33" s="96"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="98"/>
+      <c r="N33" s="98"/>
+      <c r="O33" s="99"/>
+      <c r="P33" s="79"/>
+      <c r="Q33" s="50"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="71"/>
+      <c r="U33" s="72"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A34" s="114"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+      <c r="O34" s="99"/>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="61"/>
+      <c r="T34" s="71"/>
+      <c r="U34" s="72"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="114"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="99"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="61"/>
+      <c r="T35" s="71"/>
+      <c r="U35" s="72"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36" s="114"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="98"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="98"/>
+      <c r="O36" s="99"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="71"/>
+      <c r="U36" s="72"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" s="114"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="121"/>
+      <c r="J37" s="96"/>
+      <c r="K37" s="98"/>
+      <c r="L37" s="98"/>
+      <c r="M37" s="98"/>
+      <c r="N37" s="98"/>
+      <c r="O37" s="99"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="61"/>
+      <c r="T37" s="71"/>
+      <c r="U37" s="72"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="114"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="98"/>
+      <c r="L38" s="98"/>
+      <c r="M38" s="98"/>
+      <c r="N38" s="98"/>
+      <c r="O38" s="99"/>
+      <c r="P38" s="79"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="61"/>
+      <c r="T38" s="71"/>
+      <c r="U38" s="72"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39" s="114"/>
+      <c r="B39" s="115"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="121"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="98"/>
+      <c r="O39" s="99"/>
+      <c r="P39" s="79"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="60"/>
+      <c r="S39" s="61"/>
+      <c r="T39" s="71"/>
+      <c r="U39" s="72"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40" s="114"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="121"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="99"/>
+      <c r="P40" s="79"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="60"/>
+      <c r="S40" s="61"/>
+      <c r="T40" s="71"/>
+      <c r="U40" s="72"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41" s="114"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="96"/>
+      <c r="K41" s="98"/>
+      <c r="L41" s="98"/>
+      <c r="M41" s="98"/>
+      <c r="N41" s="98"/>
+      <c r="O41" s="99"/>
+      <c r="P41" s="79"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="60"/>
+      <c r="S41" s="61"/>
+      <c r="T41" s="71"/>
+      <c r="U41" s="72"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="114"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="121"/>
+      <c r="J42" s="96"/>
+      <c r="K42" s="98"/>
+      <c r="L42" s="98"/>
+      <c r="M42" s="98"/>
+      <c r="N42" s="98"/>
+      <c r="O42" s="99"/>
+      <c r="P42" s="79"/>
+      <c r="Q42" s="50"/>
+      <c r="R42" s="60"/>
+      <c r="S42" s="61"/>
+      <c r="T42" s="71"/>
+      <c r="U42" s="72"/>
+    </row>
+    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="116"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="95"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="100"/>
+      <c r="K43" s="101"/>
+      <c r="L43" s="101"/>
+      <c r="M43" s="101"/>
+      <c r="N43" s="101"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="80"/>
+      <c r="Q43" s="51"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="63"/>
+      <c r="T43" s="73"/>
+      <c r="U43" s="74"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43 E2:E4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
+      <formula1>"not run, run but not analyzed, analysis complete"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
+      <formula1>"yes, no"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data analysis and viz; run tests of different priors.
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2B363-1720-400B-B13D-02D99B739814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10B0AE-AB04-4067-BF6A-BB81C57464B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="154">
   <si>
     <t>Date run</t>
   </si>
@@ -577,6 +577,27 @@
   <si>
     <t>Use new seeds and save additional output files (e.g. dataframes of samples and #of offspring per parent per year).
 Everything else was the same (e.g. sample size, sample years)</t>
+  </si>
+  <si>
+    <t>base_simulation_and_model_UPDATED_estimate_survival_only</t>
+  </si>
+  <si>
+    <t>It works!!!! Setting an informative prior for lambda seems to work similar to setting bounds. The abundance estimates remain solid as well.</t>
+  </si>
+  <si>
+    <t>Try including lambda as an estimable parameter, with a prior informed from a Leslie matrix.</t>
+  </si>
+  <si>
+    <t>base_simulation_and_model_UPDATED_estimateLambda_testPriors_2022.01.01</t>
+  </si>
+  <si>
+    <t>Try different priors. Specifically, a uniform distribution from 0:prior.max, varying prior.max from 1000 to 3000. 1000 is roughly double the real N; 3000 is much higher. As we increase we could be increasing the bias as well.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>running</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1738,8 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2177,7 +2198,7 @@
     <row r="11" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="113"/>
       <c r="B11" s="98" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="112">
@@ -2219,15 +2240,27 @@
       <c r="T11" s="69"/>
       <c r="U11" s="70"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="113"/>
-      <c r="B12" s="98"/>
+      <c r="B12" s="98" t="s">
+        <v>137</v>
+      </c>
       <c r="C12" s="98"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="D12" s="112">
+        <v>44562</v>
+      </c>
+      <c r="E12" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>148</v>
+      </c>
       <c r="I12" s="121"/>
       <c r="J12" s="96"/>
       <c r="K12" s="98"/>
@@ -2242,15 +2275,25 @@
       <c r="T12" s="69"/>
       <c r="U12" s="70"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="113"/>
-      <c r="B13" s="98"/>
+      <c r="B13" s="98" t="s">
+        <v>150</v>
+      </c>
       <c r="C13" s="98"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="D13" s="112">
+        <v>44564</v>
+      </c>
+      <c r="E13" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" s="43"/>
       <c r="I13" s="121"/>
       <c r="J13" s="96"/>
       <c r="K13" s="98"/>
@@ -2956,12 +2999,15 @@
       <c r="U43" s="74"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43 E2:E4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
       <formula1>"not run, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
       <formula1>"yes, no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43" xr:uid="{F77A9EEE-A581-42E3-8103-D2264E3EEDD5}">
+      <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test priors and update log and scripts
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10B0AE-AB04-4067-BF6A-BB81C57464B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47238CF-6BE4-4B91-B786-4150730972A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
-    <sheet name="Frequentist_scripts" sheetId="1" r:id="rId2"/>
-    <sheet name="Notes" sheetId="2" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId2"/>
+    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="185">
   <si>
     <t>Date run</t>
   </si>
@@ -430,9 +432,6 @@
     <t>skipped-breeding?</t>
   </si>
   <si>
-    <t>Overall Outcome</t>
-  </si>
-  <si>
     <t>Priors</t>
   </si>
   <si>
@@ -479,9 +478,6 @@
   </si>
   <si>
     <t>dnorm(0, 1.0E-6),dnorm(0, 1.0E-6)</t>
-  </si>
-  <si>
-    <t>Purpose</t>
   </si>
   <si>
     <t>Test whether the Bayesian framework works</t>
@@ -530,9 +526,6 @@
     <t>005_neutralGrowth_estNSurv_2021.11.04</t>
   </si>
   <si>
-    <t>Abbrev</t>
-  </si>
-  <si>
     <t>006_neutralGrowth_skippedBreed_2021.12.15</t>
   </si>
   <si>
@@ -594,10 +587,114 @@
     <t>Try different priors. Specifically, a uniform distribution from 0:prior.max, varying prior.max from 1000 to 3000. 1000 is roughly double the real N; 3000 is much higher. As we increase we could be increasing the bias as well.</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>running</t>
+    <t>Purpose details</t>
+  </si>
+  <si>
+    <t>Purpose (file label)</t>
+  </si>
+  <si>
+    <t>See if the hierarchical model works and how it compares to the others.</t>
+  </si>
+  <si>
+    <t>testHierarchical</t>
+  </si>
+  <si>
+    <t>base_simulation_and_hierarchical_model</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>Thinning rate</t>
+  </si>
+  <si>
+    <t>Burn-in</t>
+  </si>
+  <si>
+    <t>Posterior samples</t>
+  </si>
+  <si>
+    <t>estSurvLam</t>
+  </si>
+  <si>
+    <t>testUniformPriors</t>
+  </si>
+  <si>
+    <t>Seeds12.27</t>
+  </si>
+  <si>
+    <t>Passed diagnostics?</t>
+  </si>
+  <si>
+    <t>What does "Passed diagnostics" mean?</t>
+  </si>
+  <si>
+    <t>If yes, then convergence was good within and between the MCMC chains, there is little autocorrelation among the posterior draws (&lt; ~0.05), the cross-correlation among parameters is &lt; .8, and the gelman statistic suggests that the draws come from a stationary distribution.</t>
+  </si>
+  <si>
+    <t>Trace Plot notes</t>
+  </si>
+  <si>
+    <t>Autocorrelation notes</t>
+  </si>
+  <si>
+    <t>Gelman notes</t>
+  </si>
+  <si>
+    <t>Convergence was achieved each time, but sometimes the posterior distributions of the two chains were staggered a little bit, or had a little hump.</t>
+  </si>
+  <si>
+    <t>Plots look good!</t>
+  </si>
+  <si>
+    <t>Had issues for a number of the runs; sometimes didn't flatten out until 40k. If we use the uniform prior, I may want to increase the burn-in</t>
+  </si>
+  <si>
+    <t>Results: Notes on statistical coverage</t>
+  </si>
+  <si>
+    <t>Results: Other notes</t>
+  </si>
+  <si>
+    <t>convergence assessed</t>
+  </si>
+  <si>
+    <t>Had issues for a number of the runs; sometimes didn't flatten out until 40k. If we use the normal prior, I may want to increase the burn-in</t>
+  </si>
+  <si>
+    <t>Not quite. Should increase the burn-in for normal priors. Seems like things changed once lambda was introduced as a parameter … may need to run the chain out longer.</t>
+  </si>
+  <si>
+    <t>Not quite. Should increase the burn-in for uniform priors.  Seems like things changed once lambda was introduced as a parameter … may need to run the chain out longer.</t>
+  </si>
+  <si>
+    <t>Looks good overall BUT could still benefit from a burn-in of 40k.</t>
+  </si>
+  <si>
+    <t>I mean … probably. Still should increase the burn-in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seems to struggle with 200 samples - some estimates are wildly biased - but does much better with 300 and 400.
+Think I'm gonna need to do some work if I want to use this … </t>
+  </si>
+  <si>
+    <t>base_simulation_and_hierarchical_model2</t>
+  </si>
+  <si>
+    <t>testHierarchical2</t>
+  </si>
+  <si>
+    <t>Use the combination of uninformative priors that Charlotte recommended in her email.
+Set the sd to 1000 (arbitrary)</t>
+  </si>
+  <si>
+    <t>Convergence looks good, and the plots look better with the burn-in of 40,000</t>
+  </si>
+  <si>
+    <t>Generally looks good, but still seems like a longer burn-in? Might not be fixable by increasing the burn-in</t>
+  </si>
+  <si>
+    <t>Yes. Gelman plot is a bit funny, but I'd say overall it passes diagnostics.</t>
   </si>
 </sst>
 </file>
@@ -667,7 +764,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1211,11 +1308,209 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1286,14 +1581,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1355,15 +1648,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1373,9 +1662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1397,16 +1683,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1419,6 +1700,62 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1735,1279 +2072,1741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5546875" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" style="39" customWidth="1"/>
-    <col min="10" max="13" width="19.5546875" customWidth="1"/>
-    <col min="14" max="15" width="25.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5546875" customWidth="1"/>
+    <col min="16" max="16" width="51" customWidth="1"/>
+    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
+    <col min="18" max="21" width="19.5546875" customWidth="1"/>
+    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="118" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="126" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="126" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="126" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="126" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="111" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="85" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="O1" s="131" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="R1" s="98" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" s="79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="102">
+        <v>44489</v>
+      </c>
+      <c r="D2" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="97">
+        <v>6</v>
+      </c>
+      <c r="T2" s="97" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="V2" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="W2" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="64"/>
+    </row>
+    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="103" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="103">
+        <v>44489</v>
+      </c>
+      <c r="D3" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="90">
+        <v>6</v>
+      </c>
+      <c r="T3" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="U3" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="V3" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" s="88" t="s">
+        <v>113</v>
+      </c>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="66"/>
+    </row>
+    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="103">
+        <v>44489</v>
+      </c>
+      <c r="D4" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="90">
+        <v>6</v>
+      </c>
+      <c r="T4" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="U4" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="V4" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="W4" s="88" t="s">
+        <v>113</v>
+      </c>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="66"/>
+    </row>
+    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="91" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="103">
+        <v>44496</v>
+      </c>
+      <c r="D5" s="120" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="90">
+        <v>3</v>
+      </c>
+      <c r="T5" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="U5" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="V5" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="W5" s="88" t="s">
+        <v>113</v>
+      </c>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="66"/>
+    </row>
+    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="91"/>
+      <c r="C6" s="103">
+        <v>44504</v>
+      </c>
+      <c r="D6" s="120" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q6" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="R6" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S6" s="90">
+        <v>1</v>
+      </c>
+      <c r="T6" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="U6" s="90" t="s">
+        <v>119</v>
+      </c>
+      <c r="V6" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="W6" s="88" t="s">
+        <v>123</v>
+      </c>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="66"/>
+    </row>
+    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="91" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="91"/>
+      <c r="C7" s="103">
+        <v>44504</v>
+      </c>
+      <c r="D7" s="120"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" s="90">
+        <v>1</v>
+      </c>
+      <c r="T7" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="U7" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="V7" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="W7" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="66"/>
+    </row>
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="91"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="88"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="66"/>
+    </row>
+    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="91" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="91"/>
+      <c r="C9" s="103">
+        <v>44545</v>
+      </c>
+      <c r="D9" s="120"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="134"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="91">
+        <v>1</v>
+      </c>
+      <c r="T9" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="U9" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="V9" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="W9" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="X9" s="76"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="57"/>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="68"/>
+    </row>
+    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="106" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="106" t="s">
+      <c r="B10" s="91"/>
+      <c r="C10" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="120"/>
+      <c r="E10" s="128" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="92" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="90" t="s">
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="114" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="91" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="119" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="106" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="106" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="106" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" s="106" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="75" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q1" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="T1" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="U1" s="81" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="108" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="109" t="s">
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q10" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="R10" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="S10" s="91">
+        <v>1</v>
+      </c>
+      <c r="T10" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="110">
-        <v>44489</v>
-      </c>
-      <c r="E2" s="93" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="103" t="s">
+      <c r="U10" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="V10" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="W10" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="X10" s="76"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="68"/>
+    </row>
+    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="91" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="91"/>
+      <c r="C11" s="103">
+        <v>44558</v>
+      </c>
+      <c r="D11" s="120"/>
+      <c r="E11" s="128" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="114" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="134"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="104">
-        <v>6</v>
-      </c>
-      <c r="L2" s="104" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="104" t="s">
-        <v>113</v>
-      </c>
-      <c r="O2" s="93" t="s">
-        <v>114</v>
-      </c>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="66"/>
-    </row>
-    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="98" t="s">
+      <c r="S11" s="91">
+        <v>1</v>
+      </c>
+      <c r="T11" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="112">
-        <v>44489</v>
-      </c>
-      <c r="E3" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="97">
-        <v>6</v>
-      </c>
-      <c r="L3" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="M3" s="97" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="97" t="s">
-        <v>113</v>
-      </c>
-      <c r="O3" s="94" t="s">
-        <v>114</v>
-      </c>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="68"/>
-    </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="98" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="112">
-        <v>44489</v>
-      </c>
-      <c r="E4" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="97">
-        <v>6</v>
-      </c>
-      <c r="L4" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" s="97" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="97" t="s">
-        <v>113</v>
-      </c>
-      <c r="O4" s="94" t="s">
-        <v>114</v>
-      </c>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
-    </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="113"/>
-      <c r="B5" s="98" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="112">
-        <v>44496</v>
-      </c>
-      <c r="E5" s="94" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="97">
-        <v>3</v>
-      </c>
-      <c r="L5" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="M5" s="97" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="97" t="s">
-        <v>113</v>
-      </c>
-      <c r="O5" s="94" t="s">
-        <v>114</v>
-      </c>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="68"/>
-    </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="113"/>
-      <c r="B6" s="98" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="112">
-        <v>44504</v>
-      </c>
-      <c r="E6" s="94" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" s="121" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="97">
-        <v>1</v>
-      </c>
-      <c r="L6" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="M6" s="97" t="s">
+      <c r="U11" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="V11" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="N6" s="97" t="s">
-        <v>123</v>
-      </c>
-      <c r="O6" s="94" t="s">
-        <v>125</v>
-      </c>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="68"/>
-    </row>
-    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
-      <c r="B7" s="98" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="112">
-        <v>44504</v>
-      </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" s="97">
-        <v>1</v>
-      </c>
-      <c r="L7" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="97" t="s">
-        <v>122</v>
-      </c>
-      <c r="N7" s="97" t="s">
+      <c r="W11" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="O7" s="94" t="s">
-        <v>126</v>
-      </c>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="68"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="113"/>
-      <c r="B8" s="98" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="67"/>
-      <c r="U8" s="68"/>
-    </row>
-    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="113"/>
-      <c r="B9" s="98" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="112">
-        <v>44545</v>
-      </c>
-      <c r="E9" s="94"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="98">
-        <v>1</v>
-      </c>
-      <c r="L9" s="98" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="98" t="s">
-        <v>121</v>
-      </c>
-      <c r="N9" s="98" t="s">
-        <v>123</v>
-      </c>
-      <c r="O9" s="94" t="s">
-        <v>126</v>
-      </c>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="59"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="70"/>
-    </row>
-    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="113"/>
-      <c r="B10" s="98" t="s">
+      <c r="X11" s="76"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="68"/>
+    </row>
+    <row r="12" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="112" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="94" t="s">
+      <c r="B12" s="91"/>
+      <c r="C12" s="103">
+        <v>44562</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="128" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="128">
+        <v>15</v>
+      </c>
+      <c r="H12" s="128">
+        <v>15000</v>
+      </c>
+      <c r="I12" s="124">
+        <v>20000</v>
+      </c>
+      <c r="J12" s="114" t="s">
+        <v>140</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="L12" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="M12" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="O12" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="P12" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" s="121" t="s">
-        <v>135</v>
-      </c>
-      <c r="J10" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="98">
-        <v>1</v>
-      </c>
-      <c r="L10" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="M10" s="98" t="s">
-        <v>121</v>
-      </c>
-      <c r="N10" s="98" t="s">
-        <v>123</v>
-      </c>
-      <c r="O10" s="94" t="s">
-        <v>126</v>
-      </c>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="70"/>
-    </row>
-    <row r="11" spans="1:21" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
-      <c r="B11" s="98" t="s">
+      <c r="Q12" s="109"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="91"/>
+      <c r="T12" s="91"/>
+      <c r="U12" s="91"/>
+      <c r="V12" s="91"/>
+      <c r="W12" s="92"/>
+      <c r="X12" s="76"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="68"/>
+    </row>
+    <row r="13" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="112">
-        <v>44558</v>
-      </c>
-      <c r="E11" s="94" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="42" t="s">
+      <c r="B13" s="91"/>
+      <c r="C13" s="103">
+        <v>44564</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="128" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="128">
+        <v>15</v>
+      </c>
+      <c r="H13" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I13" s="124">
+        <v>20000</v>
+      </c>
+      <c r="J13" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="121"/>
-      <c r="J11" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="98">
-        <v>1</v>
-      </c>
-      <c r="L11" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="M11" s="98" t="s">
-        <v>121</v>
-      </c>
-      <c r="N11" s="98" t="s">
-        <v>123</v>
-      </c>
-      <c r="O11" s="94" t="s">
-        <v>126</v>
-      </c>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="70"/>
-    </row>
-    <row r="12" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="98" t="s">
+      <c r="K13" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="M13" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="N13" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="O13" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="91"/>
+      <c r="T13" s="91"/>
+      <c r="U13" s="91"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="92"/>
+      <c r="X13" s="76"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="57"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="68"/>
+    </row>
+    <row r="14" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="91"/>
+      <c r="C14" s="103">
+        <v>44565</v>
+      </c>
+      <c r="D14" s="120" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="128" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="128">
+        <v>15</v>
+      </c>
+      <c r="H14" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I14" s="124">
+        <v>20000</v>
+      </c>
+      <c r="J14" s="115" t="s">
+        <v>140</v>
+      </c>
+      <c r="K14" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="98"/>
-      <c r="D12" s="112">
-        <v>44562</v>
-      </c>
-      <c r="E12" s="94" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="I12" s="121"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="99"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="69"/>
-      <c r="U12" s="70"/>
-    </row>
-    <row r="13" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-      <c r="B13" s="98" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="112">
-        <v>44564</v>
-      </c>
-      <c r="E13" s="94" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="84" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="121"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="70"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="96"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="121"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="99"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="59"/>
-      <c r="T14" s="69"/>
-      <c r="U14" s="70"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="96"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="71"/>
-      <c r="U15" s="72"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="96"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="61"/>
-      <c r="T16" s="71"/>
-      <c r="U16" s="72"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="98"/>
-      <c r="N17" s="98"/>
-      <c r="O17" s="99"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="71"/>
-      <c r="U17" s="72"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="114"/>
-      <c r="B18" s="115"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="71"/>
-      <c r="U18" s="72"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="114"/>
-      <c r="B19" s="115"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="71"/>
-      <c r="U19" s="72"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="114"/>
-      <c r="B20" s="115"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="96"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="98"/>
-      <c r="N20" s="98"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="61"/>
-      <c r="T20" s="71"/>
-      <c r="U20" s="72"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" s="114"/>
-      <c r="B21" s="115"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="121"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="61"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="72"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="114"/>
-      <c r="B22" s="115"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="121"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="98"/>
-      <c r="N22" s="98"/>
-      <c r="O22" s="99"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="61"/>
-      <c r="T22" s="71"/>
-      <c r="U22" s="72"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="114"/>
-      <c r="B23" s="115"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
-      <c r="N23" s="98"/>
-      <c r="O23" s="99"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="61"/>
-      <c r="T23" s="71"/>
-      <c r="U23" s="72"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="114"/>
-      <c r="B24" s="115"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="96"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="98"/>
-      <c r="N24" s="98"/>
-      <c r="O24" s="99"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="61"/>
-      <c r="T24" s="71"/>
-      <c r="U24" s="72"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="114"/>
-      <c r="B25" s="115"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="96"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-      <c r="O25" s="99"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="61"/>
-      <c r="T25" s="71"/>
-      <c r="U25" s="72"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" s="114"/>
-      <c r="B26" s="115"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="121"/>
-      <c r="J26" s="96"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
-      <c r="M26" s="98"/>
-      <c r="N26" s="98"/>
-      <c r="O26" s="99"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="61"/>
-      <c r="T26" s="71"/>
-      <c r="U26" s="72"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="96"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
-      <c r="M27" s="98"/>
-      <c r="N27" s="98"/>
-      <c r="O27" s="99"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="71"/>
-      <c r="U27" s="72"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A28" s="114"/>
-      <c r="B28" s="115"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="121"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="98"/>
-      <c r="M28" s="98"/>
-      <c r="N28" s="98"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="61"/>
-      <c r="T28" s="71"/>
-      <c r="U28" s="72"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A29" s="114"/>
-      <c r="B29" s="115"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="121"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="98"/>
-      <c r="L29" s="98"/>
-      <c r="M29" s="98"/>
-      <c r="N29" s="98"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="50"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="71"/>
-      <c r="U29" s="72"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="114"/>
-      <c r="B30" s="115"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="121"/>
-      <c r="J30" s="96"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="98"/>
-      <c r="M30" s="98"/>
-      <c r="N30" s="98"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="79"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="61"/>
-      <c r="T30" s="71"/>
-      <c r="U30" s="72"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="114"/>
-      <c r="B31" s="115"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="121"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="98"/>
-      <c r="L31" s="98"/>
-      <c r="M31" s="98"/>
-      <c r="N31" s="98"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="61"/>
-      <c r="T31" s="71"/>
-      <c r="U31" s="72"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A32" s="114"/>
-      <c r="B32" s="115"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="121"/>
-      <c r="J32" s="96"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
-      <c r="N32" s="98"/>
-      <c r="O32" s="99"/>
-      <c r="P32" s="79"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="60"/>
-      <c r="S32" s="61"/>
-      <c r="T32" s="71"/>
-      <c r="U32" s="72"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="114"/>
-      <c r="B33" s="115"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="121"/>
-      <c r="J33" s="96"/>
-      <c r="K33" s="98"/>
-      <c r="L33" s="98"/>
-      <c r="M33" s="98"/>
-      <c r="N33" s="98"/>
-      <c r="O33" s="99"/>
-      <c r="P33" s="79"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="61"/>
-      <c r="T33" s="71"/>
-      <c r="U33" s="72"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="114"/>
-      <c r="B34" s="115"/>
-      <c r="C34" s="98"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="96"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="98"/>
-      <c r="M34" s="98"/>
-      <c r="N34" s="98"/>
-      <c r="O34" s="99"/>
-      <c r="P34" s="79"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="61"/>
-      <c r="T34" s="71"/>
-      <c r="U34" s="72"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="114"/>
-      <c r="B35" s="115"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="98"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="98"/>
-      <c r="N35" s="98"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="61"/>
-      <c r="T35" s="71"/>
-      <c r="U35" s="72"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="114"/>
-      <c r="B36" s="115"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="96"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
-      <c r="M36" s="98"/>
-      <c r="N36" s="98"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="61"/>
-      <c r="T36" s="71"/>
-      <c r="U36" s="72"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="114"/>
-      <c r="B37" s="115"/>
-      <c r="C37" s="98"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="121"/>
-      <c r="J37" s="96"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="98"/>
-      <c r="M37" s="98"/>
-      <c r="N37" s="98"/>
-      <c r="O37" s="99"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="61"/>
-      <c r="T37" s="71"/>
-      <c r="U37" s="72"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="114"/>
-      <c r="B38" s="115"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="96"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="98"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="98"/>
-      <c r="O38" s="99"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="61"/>
-      <c r="T38" s="71"/>
-      <c r="U38" s="72"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="114"/>
-      <c r="B39" s="115"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="121"/>
-      <c r="J39" s="96"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="98"/>
-      <c r="M39" s="98"/>
-      <c r="N39" s="98"/>
-      <c r="O39" s="99"/>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="60"/>
-      <c r="S39" s="61"/>
-      <c r="T39" s="71"/>
-      <c r="U39" s="72"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="114"/>
-      <c r="B40" s="115"/>
-      <c r="C40" s="98"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="121"/>
-      <c r="J40" s="96"/>
-      <c r="K40" s="98"/>
-      <c r="L40" s="98"/>
-      <c r="M40" s="98"/>
-      <c r="N40" s="98"/>
-      <c r="O40" s="99"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="60"/>
-      <c r="S40" s="61"/>
-      <c r="T40" s="71"/>
-      <c r="U40" s="72"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="114"/>
-      <c r="B41" s="115"/>
-      <c r="C41" s="98"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="121"/>
-      <c r="J41" s="96"/>
-      <c r="K41" s="98"/>
-      <c r="L41" s="98"/>
-      <c r="M41" s="98"/>
-      <c r="N41" s="98"/>
-      <c r="O41" s="99"/>
-      <c r="P41" s="79"/>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="60"/>
-      <c r="S41" s="61"/>
-      <c r="T41" s="71"/>
-      <c r="U41" s="72"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="114"/>
-      <c r="B42" s="115"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="94"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="121"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="98"/>
-      <c r="L42" s="98"/>
-      <c r="M42" s="98"/>
-      <c r="N42" s="98"/>
-      <c r="O42" s="99"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="60"/>
-      <c r="S42" s="61"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="72"/>
-    </row>
-    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="116"/>
-      <c r="B43" s="117"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="118"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="88"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="122"/>
-      <c r="J43" s="100"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="101"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="101"/>
-      <c r="O43" s="102"/>
-      <c r="P43" s="80"/>
-      <c r="Q43" s="51"/>
-      <c r="R43" s="62"/>
-      <c r="S43" s="63"/>
-      <c r="T43" s="73"/>
-      <c r="U43" s="74"/>
+      <c r="L14" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="M14" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="N14" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="O14" s="135" t="s">
+        <v>177</v>
+      </c>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="109" t="s">
+        <v>178</v>
+      </c>
+      <c r="R14" s="89"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="91"/>
+      <c r="V14" s="91"/>
+      <c r="W14" s="92"/>
+      <c r="X14" s="76"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="57"/>
+      <c r="AB14" s="67"/>
+      <c r="AC14" s="68"/>
+    </row>
+    <row r="15" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="91"/>
+      <c r="C15" s="103">
+        <v>44570</v>
+      </c>
+      <c r="D15" s="120" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="128" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="128">
+        <v>15</v>
+      </c>
+      <c r="H15" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I15" s="124">
+        <v>40000</v>
+      </c>
+      <c r="J15" s="115" t="s">
+        <v>140</v>
+      </c>
+      <c r="K15" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="L15" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="M15" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="N15" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="O15" s="135" t="s">
+        <v>184</v>
+      </c>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="109"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="77"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="59"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="70"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="135"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="91"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="91"/>
+      <c r="V16" s="91"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="77"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="128"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="116"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="135"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="109"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="91"/>
+      <c r="T17" s="91"/>
+      <c r="U17" s="91"/>
+      <c r="V17" s="91"/>
+      <c r="W17" s="92"/>
+      <c r="X17" s="77"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="70"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="135"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="109"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="91"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="92"/>
+      <c r="X18" s="77"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="69"/>
+      <c r="AC18" s="70"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="116"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="135"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="109"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="91"/>
+      <c r="T19" s="91"/>
+      <c r="U19" s="91"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="92"/>
+      <c r="X19" s="77"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="70"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="116"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="135"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="109"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="91"/>
+      <c r="U20" s="91"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="70"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="135"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="89"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="91"/>
+      <c r="U21" s="91"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="77"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="70"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="135"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="91"/>
+      <c r="T22" s="91"/>
+      <c r="U22" s="91"/>
+      <c r="V22" s="91"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="77"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="58"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="69"/>
+      <c r="AC22" s="70"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="116"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="135"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="109"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="91"/>
+      <c r="T23" s="91"/>
+      <c r="U23" s="91"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="92"/>
+      <c r="X23" s="77"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="59"/>
+      <c r="AB23" s="69"/>
+      <c r="AC23" s="70"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="109"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="91"/>
+      <c r="T24" s="91"/>
+      <c r="U24" s="91"/>
+      <c r="V24" s="91"/>
+      <c r="W24" s="92"/>
+      <c r="X24" s="77"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="58"/>
+      <c r="AA24" s="59"/>
+      <c r="AB24" s="69"/>
+      <c r="AC24" s="70"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="124"/>
+      <c r="J25" s="116"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="135"/>
+      <c r="P25" s="82"/>
+      <c r="Q25" s="109"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="91"/>
+      <c r="T25" s="91"/>
+      <c r="U25" s="91"/>
+      <c r="V25" s="91"/>
+      <c r="W25" s="92"/>
+      <c r="X25" s="77"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="69"/>
+      <c r="AC25" s="70"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A26" s="91"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="116"/>
+      <c r="K26" s="83"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="135"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="109"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="91"/>
+      <c r="T26" s="91"/>
+      <c r="U26" s="91"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="92"/>
+      <c r="X26" s="77"/>
+      <c r="Y26" s="48"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="59"/>
+      <c r="AB26" s="69"/>
+      <c r="AC26" s="70"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A27" s="91"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="116"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="135"/>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="109"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="92"/>
+      <c r="X27" s="77"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="59"/>
+      <c r="AB27" s="69"/>
+      <c r="AC27" s="70"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="124"/>
+      <c r="J28" s="116"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="135"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="109"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="91"/>
+      <c r="T28" s="91"/>
+      <c r="U28" s="91"/>
+      <c r="V28" s="91"/>
+      <c r="W28" s="92"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="59"/>
+      <c r="AB28" s="69"/>
+      <c r="AC28" s="70"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="124"/>
+      <c r="J29" s="116"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="135"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="109"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="91"/>
+      <c r="T29" s="91"/>
+      <c r="U29" s="91"/>
+      <c r="V29" s="91"/>
+      <c r="W29" s="92"/>
+      <c r="X29" s="77"/>
+      <c r="Y29" s="48"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="59"/>
+      <c r="AB29" s="69"/>
+      <c r="AC29" s="70"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" s="91"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="124"/>
+      <c r="J30" s="116"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="135"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="109"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="92"/>
+      <c r="X30" s="77"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="69"/>
+      <c r="AC30" s="70"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A31" s="91"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="124"/>
+      <c r="J31" s="116"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="135"/>
+      <c r="P31" s="82"/>
+      <c r="Q31" s="109"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="91"/>
+      <c r="T31" s="91"/>
+      <c r="U31" s="91"/>
+      <c r="V31" s="91"/>
+      <c r="W31" s="92"/>
+      <c r="X31" s="77"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="59"/>
+      <c r="AB31" s="69"/>
+      <c r="AC31" s="70"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="128"/>
+      <c r="I32" s="124"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="83"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="135"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="109"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="91"/>
+      <c r="T32" s="91"/>
+      <c r="U32" s="91"/>
+      <c r="V32" s="91"/>
+      <c r="W32" s="92"/>
+      <c r="X32" s="77"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="58"/>
+      <c r="AA32" s="59"/>
+      <c r="AB32" s="69"/>
+      <c r="AC32" s="70"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A33" s="91"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="116"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="135"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="109"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="91"/>
+      <c r="T33" s="91"/>
+      <c r="U33" s="91"/>
+      <c r="V33" s="91"/>
+      <c r="W33" s="92"/>
+      <c r="X33" s="77"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="58"/>
+      <c r="AA33" s="59"/>
+      <c r="AB33" s="69"/>
+      <c r="AC33" s="70"/>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A34" s="91"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="135"/>
+      <c r="P34" s="82"/>
+      <c r="Q34" s="109"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="91"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="91"/>
+      <c r="V34" s="91"/>
+      <c r="W34" s="92"/>
+      <c r="X34" s="77"/>
+      <c r="Y34" s="48"/>
+      <c r="Z34" s="58"/>
+      <c r="AA34" s="59"/>
+      <c r="AB34" s="69"/>
+      <c r="AC34" s="70"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A35" s="91"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="116"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="135"/>
+      <c r="P35" s="82"/>
+      <c r="Q35" s="109"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
+      <c r="V35" s="91"/>
+      <c r="W35" s="92"/>
+      <c r="X35" s="77"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="58"/>
+      <c r="AA35" s="59"/>
+      <c r="AB35" s="69"/>
+      <c r="AC35" s="70"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A36" s="91"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="116"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="135"/>
+      <c r="P36" s="82"/>
+      <c r="Q36" s="109"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="91"/>
+      <c r="T36" s="91"/>
+      <c r="U36" s="91"/>
+      <c r="V36" s="91"/>
+      <c r="W36" s="92"/>
+      <c r="X36" s="77"/>
+      <c r="Y36" s="48"/>
+      <c r="Z36" s="58"/>
+      <c r="AA36" s="59"/>
+      <c r="AB36" s="69"/>
+      <c r="AC36" s="70"/>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="128"/>
+      <c r="F37" s="128"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="116"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="135"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="109"/>
+      <c r="R37" s="89"/>
+      <c r="S37" s="91"/>
+      <c r="T37" s="91"/>
+      <c r="U37" s="91"/>
+      <c r="V37" s="91"/>
+      <c r="W37" s="92"/>
+      <c r="X37" s="77"/>
+      <c r="Y37" s="48"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="59"/>
+      <c r="AB37" s="69"/>
+      <c r="AC37" s="70"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" s="104"/>
+      <c r="B38" s="91"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="128"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="128"/>
+      <c r="H38" s="128"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="116"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="135"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="109"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="91"/>
+      <c r="T38" s="91"/>
+      <c r="U38" s="91"/>
+      <c r="V38" s="91"/>
+      <c r="W38" s="92"/>
+      <c r="X38" s="77"/>
+      <c r="Y38" s="48"/>
+      <c r="Z38" s="58"/>
+      <c r="AA38" s="59"/>
+      <c r="AB38" s="69"/>
+      <c r="AC38" s="70"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A39" s="104"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
+      <c r="H39" s="128"/>
+      <c r="I39" s="124"/>
+      <c r="J39" s="116"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="135"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="109"/>
+      <c r="R39" s="89"/>
+      <c r="S39" s="91"/>
+      <c r="T39" s="91"/>
+      <c r="U39" s="91"/>
+      <c r="V39" s="91"/>
+      <c r="W39" s="92"/>
+      <c r="X39" s="77"/>
+      <c r="Y39" s="48"/>
+      <c r="Z39" s="58"/>
+      <c r="AA39" s="59"/>
+      <c r="AB39" s="69"/>
+      <c r="AC39" s="70"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A40" s="104"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="128"/>
+      <c r="G40" s="128"/>
+      <c r="H40" s="128"/>
+      <c r="I40" s="124"/>
+      <c r="J40" s="116"/>
+      <c r="K40" s="83"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="135"/>
+      <c r="P40" s="82"/>
+      <c r="Q40" s="109"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="91"/>
+      <c r="T40" s="91"/>
+      <c r="U40" s="91"/>
+      <c r="V40" s="91"/>
+      <c r="W40" s="92"/>
+      <c r="X40" s="77"/>
+      <c r="Y40" s="48"/>
+      <c r="Z40" s="58"/>
+      <c r="AA40" s="59"/>
+      <c r="AB40" s="69"/>
+      <c r="AC40" s="70"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A41" s="104"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="103"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="128"/>
+      <c r="F41" s="128"/>
+      <c r="G41" s="128"/>
+      <c r="H41" s="128"/>
+      <c r="I41" s="124"/>
+      <c r="J41" s="116"/>
+      <c r="K41" s="83"/>
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="135"/>
+      <c r="P41" s="82"/>
+      <c r="Q41" s="109"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="91"/>
+      <c r="T41" s="91"/>
+      <c r="U41" s="91"/>
+      <c r="V41" s="91"/>
+      <c r="W41" s="92"/>
+      <c r="X41" s="77"/>
+      <c r="Y41" s="48"/>
+      <c r="Z41" s="58"/>
+      <c r="AA41" s="59"/>
+      <c r="AB41" s="69"/>
+      <c r="AC41" s="70"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A42" s="104"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="128"/>
+      <c r="F42" s="128"/>
+      <c r="G42" s="128"/>
+      <c r="H42" s="128"/>
+      <c r="I42" s="124"/>
+      <c r="J42" s="116"/>
+      <c r="K42" s="83"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="135"/>
+      <c r="P42" s="82"/>
+      <c r="Q42" s="109"/>
+      <c r="R42" s="89"/>
+      <c r="S42" s="91"/>
+      <c r="T42" s="91"/>
+      <c r="U42" s="91"/>
+      <c r="V42" s="91"/>
+      <c r="W42" s="92"/>
+      <c r="X42" s="77"/>
+      <c r="Y42" s="48"/>
+      <c r="Z42" s="58"/>
+      <c r="AA42" s="59"/>
+      <c r="AB42" s="69"/>
+      <c r="AC42" s="70"/>
+    </row>
+    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="105"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="125"/>
+      <c r="J43" s="117"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="130"/>
+      <c r="N43" s="130"/>
+      <c r="O43" s="136"/>
+      <c r="P43" s="138"/>
+      <c r="Q43" s="110"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="94"/>
+      <c r="T43" s="94"/>
+      <c r="U43" s="94"/>
+      <c r="V43" s="94"/>
+      <c r="W43" s="95"/>
+      <c r="X43" s="78"/>
+      <c r="Y43" s="49"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="61"/>
+      <c r="AB43" s="71"/>
+      <c r="AC43" s="72"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
       <formula1>"not run, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
       <formula1>"yes, no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43" xr:uid="{F77A9EEE-A581-42E3-8103-D2264E3EEDD5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:O11" xr:uid="{F77A9EEE-A581-42E3-8103-D2264E3EEDD5}">
       <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:K43" xr:uid="{53ECF302-A855-4FB9-844A-C7CE01367649}">
+      <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3016,12 +3815,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E03EF-3489-4384-AA19-0C78DA3254C7}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3616,12 +4443,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update Leslie matrix visualization
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47238CF-6BE4-4B91-B786-4150730972A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0737D7D3-FF93-4BBF-8C22-898AE96A8522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bayesian_scripts" sheetId="3" r:id="rId1"/>
-    <sheet name="Notes" sheetId="4" r:id="rId2"/>
-    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId3"/>
-    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Bayesian_model_validation" sheetId="3" r:id="rId1"/>
+    <sheet name="Prior_sensitivity" sheetId="5" r:id="rId2"/>
+    <sheet name="Notes" sheetId="4" r:id="rId3"/>
+    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId4"/>
+    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="191">
   <si>
     <t>Date run</t>
   </si>
@@ -695,6 +695,25 @@
   </si>
   <si>
     <t>Yes. Gelman plot is a bit funny, but I'd say overall it passes diagnostics.</t>
+  </si>
+  <si>
+    <t>test_CV_on_fecundity_and_survival</t>
+  </si>
+  <si>
+    <t>When using CKMR and incorporating lambda, researchers will have varying degrees of confidence in the numbers they use for fecundity and survival. To set a prior on lambda, I want to see what happens if I play with those values (i.e. the CV on fecundity and survival, and a potential correlation between the two) and see what sort of range of values I get for lambda.</t>
+  </si>
+  <si>
+    <t>Mean value of lambda is very near to 1, regardless,
+standard deviation across all cv and correlation values is .02277. Good enough for now, but may want to change this once I decide which values to move forward with for fecundity and survival.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Uniform_10kMax</t>
+  </si>
+  <si>
+    <t>Trying to re-think the priors. What kind of information would we actually have available? Maybe for a small population we would estimate the population size is 10k or less. The previous simulations just looked at a max value up to 3k with a uniform prior.</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1756,6 +1775,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2074,9 +2096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2926,17 +2948,35 @@
       <c r="AB15" s="69"/>
       <c r="AC15" s="70"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" s="91"/>
+    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="90" t="s">
+        <v>134</v>
+      </c>
       <c r="B16" s="91"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="128"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="115"/>
+      <c r="C16" s="103">
+        <v>44578</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="128" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="128">
+        <v>15</v>
+      </c>
+      <c r="H16" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I16" s="124">
+        <v>40000</v>
+      </c>
+      <c r="J16" s="115" t="s">
+        <v>188</v>
+      </c>
       <c r="K16" s="42"/>
       <c r="L16" s="42"/>
       <c r="M16" s="42"/>
@@ -3815,6 +3855,301 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD7D549-C187-4DCD-8DD0-20217DC34E3E}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="118" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="126" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="102">
+        <v>44578</v>
+      </c>
+      <c r="B2" s="119" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="127" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="139" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="103"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="103"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="103"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="41"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="103"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="41"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="103"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="41"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="103"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="103"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="103"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="103"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="41"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="103"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="42"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="103"/>
+      <c r="B13" s="120"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="42"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="103"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="42"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="103"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="42"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="103"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="42"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="103"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="42"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="103"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="42"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="103"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="42"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="103"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="42"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="103"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="42"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="103"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="42"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="103"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="42"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="103"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="42"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="103"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="42"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="103"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="42"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="103"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="42"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="103"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="42"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="103"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="42"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="103"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="42"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="103"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="42"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="103"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="42"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="103"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="42"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="103"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="42"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="103"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="42"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="103"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="42"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="103"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="42"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="103"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="42"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="103"/>
+      <c r="B39" s="120"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="42"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="103"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="128"/>
+      <c r="D40" s="42"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="103"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="42"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="103"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="42"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="106"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="130"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E03EF-3489-4384-AA19-0C78DA3254C7}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -3841,7 +4176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -4443,7 +4778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update and test hierarchical model
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0737D7D3-FF93-4BBF-8C22-898AE96A8522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA83A872-9F27-4E6C-A25D-1DA40EBD1ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="197">
   <si>
     <t>Date run</t>
   </si>
@@ -714,6 +714,25 @@
   </si>
   <si>
     <t>Trying to re-think the priors. What kind of information would we actually have available? Maybe for a small population we would estimate the population size is 10k or less. The previous simulations just looked at a max value up to 3k with a uniform prior.</t>
+  </si>
+  <si>
+    <t>Generally looks good, but seems like a burn-in of 50,000 might be best. Another 10,000 iterations would improve the shrink factor near the beginning of the sampling period.</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Coverage looks good! Males at higher sample size struggle a bit, perhaps due to uneven sampling. Should continue for now with a uniform prior on abundance with max 10,000.</t>
+  </si>
+  <si>
+    <t>base_simulation_and_hierarchical_model_calculatePriorFirst.R</t>
+  </si>
+  <si>
+    <t>testHierarchical_calculatePriorsFirst</t>
+  </si>
+  <si>
+    <t>I want to use an informed prior on abundance, but not sure how to integrate it into the model fully (due to survival being estimated as a parameter). SO, here I use the simple N=Y/R *C from Waples &amp; Feutry to calculate a mean and sd on abundance outside the model, then use these as the parameters of a normal distribution.
+Note that I increased the burn-in by 10000 relative to previous runs.</t>
   </si>
 </sst>
 </file>
@@ -2096,7 +2115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
@@ -2708,7 +2727,7 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
         <v>134</v>
       </c>
@@ -2769,7 +2788,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
         <v>147</v>
       </c>
@@ -2828,7 +2847,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
         <v>153</v>
       </c>
@@ -2889,7 +2908,7 @@
       <c r="AB14" s="67"/>
       <c r="AC14" s="68"/>
     </row>
-    <row r="15" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="90" t="s">
         <v>179</v>
       </c>
@@ -2975,14 +2994,26 @@
         <v>40000</v>
       </c>
       <c r="J16" s="115" t="s">
-        <v>188</v>
-      </c>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="135"/>
-      <c r="P16" s="82"/>
+        <v>140</v>
+      </c>
+      <c r="K16" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="L16" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="M16" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="N16" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="O16" s="135" t="s">
+        <v>192</v>
+      </c>
+      <c r="P16" s="82" t="s">
+        <v>193</v>
+      </c>
       <c r="Q16" s="109"/>
       <c r="R16" s="89"/>
       <c r="S16" s="91"/>
@@ -2997,17 +3028,35 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
+    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="91" t="s">
+        <v>194</v>
+      </c>
       <c r="B17" s="91"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="124"/>
-      <c r="J17" s="116"/>
+      <c r="C17" s="103">
+        <v>44579</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="128" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="128">
+        <v>15</v>
+      </c>
+      <c r="H17" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I17" s="124">
+        <v>50000</v>
+      </c>
+      <c r="J17" s="116" t="s">
+        <v>188</v>
+      </c>
       <c r="K17" s="83"/>
       <c r="L17" s="42"/>
       <c r="M17" s="42"/>

</xml_diff>

<commit_message>
Update data analysis script and skipped-breeding simulation
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA83A872-9F27-4E6C-A25D-1DA40EBD1ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51C4F8F-46D3-4B97-BB09-1F79F1EB3FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="205">
   <si>
     <t>Date run</t>
   </si>
@@ -578,9 +578,6 @@
     <t>It works!!!! Setting an informative prior for lambda seems to work similar to setting bounds. The abundance estimates remain solid as well.</t>
   </si>
   <si>
-    <t>Try including lambda as an estimable parameter, with a prior informed from a Leslie matrix.</t>
-  </si>
-  <si>
     <t>base_simulation_and_model_UPDATED_estimateLambda_testPriors_2022.01.01</t>
   </si>
   <si>
@@ -733,6 +730,35 @@
   <si>
     <t>I want to use an informed prior on abundance, but not sure how to integrate it into the model fully (due to survival being estimated as a parameter). SO, here I use the simple N=Y/R *C from Waples &amp; Feutry to calculate a mean and sd on abundance outside the model, then use these as the parameters of a normal distribution.
 Note that I increased the burn-in by 10000 relative to previous runs.</t>
+  </si>
+  <si>
+    <t>Convergence looks great</t>
+  </si>
+  <si>
+    <t>Looks good!</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Try including lambda as an estimable parameter, with a prior informed from a Leslie matrix. Prior is uninformative Normal</t>
+  </si>
+  <si>
+    <t>Looks good overall. Similar to the uniform prior, also struggles with males, moreso as sample size increases. But nothing alarming.</t>
+  </si>
+  <si>
+    <t>Median relative bias is much much lower than with the uninformative priors!</t>
+  </si>
+  <si>
+    <t>base_simulation_and_model_SB.R</t>
+  </si>
+  <si>
+    <t>Added skipped-breeding to simulation.
+Accounted for it in the model by multiplying the numerator by 0.5 for females.
+Also sampled over two years to make sure we're sampling females evenly -- seemed like the equivalent to sampling one year with annual breeding.</t>
+  </si>
+  <si>
+    <t>SB_w_uninformativePrior</t>
   </si>
 </sst>
 </file>
@@ -2116,8 +2142,8 @@
   <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E17" sqref="E17"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2157,22 +2183,22 @@
         <v>0</v>
       </c>
       <c r="D1" s="118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E1" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F1" s="126" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="126" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="126" t="s">
+      <c r="H1" s="126" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="122" t="s">
         <v>155</v>
-      </c>
-      <c r="H1" s="126" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="122" t="s">
-        <v>156</v>
       </c>
       <c r="J1" s="111" t="s">
         <v>135</v>
@@ -2181,22 +2207,22 @@
         <v>136</v>
       </c>
       <c r="L1" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="M1" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="M1" s="85" t="s">
+      <c r="N1" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="N1" s="85" t="s">
-        <v>166</v>
-      </c>
       <c r="O1" s="131" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P1" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q1" s="107" t="s">
         <v>170</v>
-      </c>
-      <c r="Q1" s="107" t="s">
-        <v>171</v>
       </c>
       <c r="R1" s="98" t="s">
         <v>24</v>
@@ -2727,28 +2753,28 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B12" s="91"/>
       <c r="C12" s="103">
-        <v>44562</v>
+        <v>44564</v>
       </c>
       <c r="D12" s="120" t="s">
         <v>158</v>
       </c>
       <c r="E12" s="128" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F12" s="128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" s="128">
         <v>15</v>
       </c>
       <c r="H12" s="128">
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="I12" s="124">
         <v>20000</v>
@@ -2757,23 +2783,21 @@
         <v>140</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="L12" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="M12" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="M12" s="42" t="s">
+      <c r="N12" s="42" t="s">
         <v>168</v>
-      </c>
-      <c r="N12" s="42" t="s">
-        <v>173</v>
       </c>
       <c r="O12" s="135" t="s">
         <v>174</v>
       </c>
-      <c r="P12" s="82" t="s">
-        <v>145</v>
-      </c>
+      <c r="P12" s="82"/>
       <c r="Q12" s="109"/>
       <c r="R12" s="89"/>
       <c r="S12" s="91"/>
@@ -2788,22 +2812,22 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B13" s="91"/>
       <c r="C13" s="103">
-        <v>44564</v>
+        <v>44565</v>
       </c>
       <c r="D13" s="120" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="128" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="128" t="s">
         <v>159</v>
-      </c>
-      <c r="E13" s="128" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="128" t="s">
-        <v>160</v>
       </c>
       <c r="G13" s="128">
         <v>15</v>
@@ -2814,26 +2838,28 @@
       <c r="I13" s="124">
         <v>20000</v>
       </c>
-      <c r="J13" s="114" t="s">
+      <c r="J13" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="K13" s="41" t="s">
-        <v>172</v>
+      <c r="K13" s="42" t="s">
+        <v>137</v>
       </c>
       <c r="L13" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="M13" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="M13" s="42" t="s">
-        <v>168</v>
-      </c>
       <c r="N13" s="42" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="O13" s="135" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P13" s="82"/>
-      <c r="Q13" s="109"/>
+      <c r="Q13" s="109" t="s">
+        <v>177</v>
+      </c>
       <c r="R13" s="89"/>
       <c r="S13" s="91"/>
       <c r="T13" s="91"/>
@@ -2847,22 +2873,22 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="B14" s="91"/>
       <c r="C14" s="103">
-        <v>44565</v>
+        <v>44570</v>
       </c>
       <c r="D14" s="120" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="E14" s="128" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="F14" s="128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G14" s="128">
         <v>15</v>
@@ -2871,7 +2897,7 @@
         <v>30000</v>
       </c>
       <c r="I14" s="124">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="J14" s="115" t="s">
         <v>140</v>
@@ -2880,79 +2906,79 @@
         <v>137</v>
       </c>
       <c r="L14" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="M14" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="M14" s="42" t="s">
-        <v>168</v>
-      </c>
       <c r="N14" s="42" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="O14" s="135" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="P14" s="82"/>
-      <c r="Q14" s="109" t="s">
-        <v>178</v>
-      </c>
+      <c r="Q14" s="109"/>
       <c r="R14" s="89"/>
       <c r="S14" s="91"/>
       <c r="T14" s="91"/>
       <c r="U14" s="91"/>
       <c r="V14" s="91"/>
       <c r="W14" s="92"/>
-      <c r="X14" s="76"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
-    </row>
-    <row r="15" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="X14" s="77"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="70"/>
+    </row>
+    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="90" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="B15" s="91"/>
       <c r="C15" s="103">
-        <v>44570</v>
+        <v>44562</v>
       </c>
       <c r="D15" s="120" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="E15" s="128" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="F15" s="128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G15" s="128">
         <v>15</v>
       </c>
       <c r="H15" s="128">
-        <v>30000</v>
+        <v>15000</v>
       </c>
       <c r="I15" s="124">
-        <v>40000</v>
-      </c>
-      <c r="J15" s="115" t="s">
+        <v>20000</v>
+      </c>
+      <c r="J15" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="K15" s="42" t="s">
-        <v>137</v>
+      <c r="K15" s="41" t="s">
+        <v>138</v>
       </c>
       <c r="L15" s="42" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="M15" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N15" s="42" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="O15" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="P15" s="82"/>
+        <v>173</v>
+      </c>
+      <c r="P15" s="82" t="s">
+        <v>145</v>
+      </c>
       <c r="Q15" s="109"/>
       <c r="R15" s="89"/>
       <c r="S15" s="91"/>
@@ -2960,12 +2986,12 @@
       <c r="U15" s="91"/>
       <c r="V15" s="91"/>
       <c r="W15" s="92"/>
-      <c r="X15" s="77"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="58"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="69"/>
-      <c r="AC15" s="70"/>
+      <c r="X15" s="76"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="57"/>
+      <c r="AB15" s="67"/>
+      <c r="AC15" s="68"/>
     </row>
     <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="90" t="s">
@@ -2976,13 +3002,13 @@
         <v>44578</v>
       </c>
       <c r="D16" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="128" t="s">
         <v>189</v>
       </c>
-      <c r="E16" s="128" t="s">
-        <v>190</v>
-      </c>
       <c r="F16" s="128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G16" s="128">
         <v>15</v>
@@ -3000,19 +3026,19 @@
         <v>138</v>
       </c>
       <c r="L16" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="M16" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="M16" s="42" t="s">
-        <v>168</v>
-      </c>
       <c r="N16" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="O16" s="135" t="s">
         <v>191</v>
       </c>
-      <c r="O16" s="135" t="s">
+      <c r="P16" s="82" t="s">
         <v>192</v>
-      </c>
-      <c r="P16" s="82" t="s">
-        <v>193</v>
       </c>
       <c r="Q16" s="109"/>
       <c r="R16" s="89"/>
@@ -3030,20 +3056,20 @@
     </row>
     <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A17" s="91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="91"/>
       <c r="C17" s="103">
         <v>44579</v>
       </c>
       <c r="D17" s="120" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="128" t="s">
         <v>195</v>
       </c>
-      <c r="E17" s="128" t="s">
-        <v>196</v>
-      </c>
       <c r="F17" s="128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G17" s="128">
         <v>15</v>
@@ -3055,15 +3081,29 @@
         <v>50000</v>
       </c>
       <c r="J17" s="116" t="s">
-        <v>188</v>
-      </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="135"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="109"/>
+        <v>140</v>
+      </c>
+      <c r="K17" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="M17" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="N17" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="O17" s="135" t="s">
+        <v>198</v>
+      </c>
+      <c r="P17" s="82" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q17" s="109" t="s">
+        <v>201</v>
+      </c>
       <c r="R17" s="89"/>
       <c r="S17" s="91"/>
       <c r="T17" s="91"/>
@@ -3077,17 +3117,35 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A18" s="91"/>
+    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="91" t="s">
+        <v>202</v>
+      </c>
       <c r="B18" s="91"/>
-      <c r="C18" s="103"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
-      <c r="I18" s="124"/>
-      <c r="J18" s="116"/>
+      <c r="C18" s="103">
+        <v>44581</v>
+      </c>
+      <c r="D18" s="120" t="s">
+        <v>204</v>
+      </c>
+      <c r="E18" s="128" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="128" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="128">
+        <v>15</v>
+      </c>
+      <c r="H18" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I18" s="124">
+        <v>50000</v>
+      </c>
+      <c r="J18" s="116" t="s">
+        <v>187</v>
+      </c>
       <c r="K18" s="83"/>
       <c r="L18" s="42"/>
       <c r="M18" s="42"/>
@@ -3888,11 +3946,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I4" xr:uid="{51E317E2-84C5-47D6-8404-EA880EC5DF80}">
       <formula1>"not run, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
-      <formula1>"yes, no"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:O11" xr:uid="{F77A9EEE-A581-42E3-8103-D2264E3EEDD5}">
       <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J11 J12:J43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
+      <formula1>"yes, no"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:K43" xr:uid="{53ECF302-A855-4FB9-844A-C7CE01367649}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
@@ -3924,10 +3982,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D1" s="85" t="s">
         <v>5</v>
@@ -3938,13 +3996,13 @@
         <v>44578</v>
       </c>
       <c r="B2" s="119" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="127" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="127" t="s">
+      <c r="D2" s="139" t="s">
         <v>186</v>
-      </c>
-      <c r="D2" s="139" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4214,10 +4272,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add skipped-breeding and test prior sensitivity.
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51C4F8F-46D3-4B97-BB09-1F79F1EB3FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602EC46-8C86-433E-B4E5-10797FFB5FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
   <si>
     <t>Date run</t>
   </si>
@@ -759,6 +759,27 @@
   </si>
   <si>
     <t>SB_w_uninformativePrior</t>
+  </si>
+  <si>
+    <t>base_simulation_and_hierarchical_model_SB.R</t>
+  </si>
+  <si>
+    <t>SB_w_uninformativePrior2</t>
+  </si>
+  <si>
+    <t>Same as above, except I moved the 0.5 to the denominator i.e. next to the Nf instead of multiplying the probability. i.e. instead of (surv*0.5)/N, it's surv/(N*0.5)</t>
+  </si>
+  <si>
+    <t>prior_posterior_density_SDMax</t>
+  </si>
+  <si>
+    <t>I want to be smart about how I set the noninformative prior, so I need to examine how the prior behaves at different values. The output shows a single iteration comparison of the priors and associated posteriors for diferent values of max in Uniform(min, max).</t>
+  </si>
+  <si>
+    <t>Seems like the priors for abundance (both sexes) and survival are quite uninformative.</t>
+  </si>
+  <si>
+    <t>Analyzed?</t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1823,6 +1844,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2139,40 +2163,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B74561-FEAE-4A63-A5C5-D46538C7187F}">
-  <dimension ref="A1:AC43"/>
+  <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5703125" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="17" max="17" width="49.7109375" style="39" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -2261,7 +2285,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>106</v>
       </c>
@@ -2312,7 +2336,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>107</v>
       </c>
@@ -2363,7 +2387,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
         <v>108</v>
       </c>
@@ -2414,7 +2438,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
@@ -2463,7 +2487,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
@@ -2516,7 +2540,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
@@ -2563,7 +2587,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91" t="s">
         <v>128</v>
       </c>
@@ -2596,7 +2620,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>129</v>
       </c>
@@ -2643,7 +2667,7 @@
       <c r="AB9" s="67"/>
       <c r="AC9" s="68"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
         <v>131</v>
       </c>
@@ -2700,7 +2724,7 @@
       <c r="AB10" s="67"/>
       <c r="AC10" s="68"/>
     </row>
-    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>144</v>
       </c>
@@ -2753,7 +2777,7 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="90" t="s">
         <v>146</v>
       </c>
@@ -2812,7 +2836,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
         <v>152</v>
       </c>
@@ -2873,7 +2897,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>178</v>
       </c>
@@ -2932,7 +2956,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>134</v>
       </c>
@@ -2993,7 +3017,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="90" t="s">
         <v>134</v>
       </c>
@@ -3054,7 +3078,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="91" t="s">
         <v>193</v>
       </c>
@@ -3117,7 +3141,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
         <v>202</v>
       </c>
@@ -3166,17 +3190,35 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="91"/>
+    <row r="19" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="91" t="s">
+        <v>202</v>
+      </c>
       <c r="B19" s="91"/>
-      <c r="C19" s="103"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="124"/>
-      <c r="J19" s="116"/>
+      <c r="C19" s="103">
+        <v>44581</v>
+      </c>
+      <c r="D19" s="120" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="128" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19" s="128" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="128">
+        <v>15</v>
+      </c>
+      <c r="H19" s="128">
+        <v>30000</v>
+      </c>
+      <c r="I19" s="124">
+        <v>50000</v>
+      </c>
+      <c r="J19" s="116" t="s">
+        <v>187</v>
+      </c>
       <c r="K19" s="83"/>
       <c r="L19" s="42"/>
       <c r="M19" s="42"/>
@@ -3197,10 +3239,14 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A20" s="91"/>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="91" t="s">
+        <v>205</v>
+      </c>
       <c r="B20" s="91"/>
-      <c r="C20" s="103"/>
+      <c r="C20" s="103">
+        <v>44581</v>
+      </c>
       <c r="D20" s="120"/>
       <c r="E20" s="128"/>
       <c r="F20" s="128"/>
@@ -3228,7 +3274,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -3259,7 +3305,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -3290,7 +3336,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -3321,7 +3367,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -3352,7 +3398,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -3383,7 +3429,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -3414,7 +3460,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -3445,7 +3491,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -3476,7 +3522,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -3507,7 +3553,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -3538,7 +3584,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -3569,7 +3615,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -3600,7 +3646,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -3631,7 +3677,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -3662,7 +3708,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -3693,7 +3739,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -3724,7 +3770,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -3755,8 +3801,8 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A38" s="104"/>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
       <c r="D38" s="120"/>
@@ -3786,7 +3832,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -3817,7 +3863,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -3848,7 +3894,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -3879,7 +3925,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -3910,36 +3956,67 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="105"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="106"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="129"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="125"/>
-      <c r="J43" s="117"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="130"/>
-      <c r="M43" s="130"/>
-      <c r="N43" s="130"/>
-      <c r="O43" s="136"/>
-      <c r="P43" s="138"/>
-      <c r="Q43" s="110"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="94"/>
-      <c r="T43" s="94"/>
-      <c r="U43" s="94"/>
-      <c r="V43" s="94"/>
-      <c r="W43" s="95"/>
-      <c r="X43" s="78"/>
-      <c r="Y43" s="49"/>
-      <c r="Z43" s="60"/>
-      <c r="AA43" s="61"/>
-      <c r="AB43" s="71"/>
-      <c r="AC43" s="72"/>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" s="104"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="128"/>
+      <c r="F43" s="128"/>
+      <c r="G43" s="128"/>
+      <c r="H43" s="128"/>
+      <c r="I43" s="124"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="83"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="135"/>
+      <c r="P43" s="82"/>
+      <c r="Q43" s="109"/>
+      <c r="R43" s="89"/>
+      <c r="S43" s="91"/>
+      <c r="T43" s="91"/>
+      <c r="U43" s="91"/>
+      <c r="V43" s="91"/>
+      <c r="W43" s="92"/>
+      <c r="X43" s="77"/>
+      <c r="Y43" s="48"/>
+      <c r="Z43" s="58"/>
+      <c r="AA43" s="59"/>
+      <c r="AB43" s="69"/>
+      <c r="AC43" s="70"/>
+    </row>
+    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="105"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="129"/>
+      <c r="I44" s="125"/>
+      <c r="J44" s="117"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="130"/>
+      <c r="M44" s="130"/>
+      <c r="N44" s="130"/>
+      <c r="O44" s="136"/>
+      <c r="P44" s="138"/>
+      <c r="Q44" s="110"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="94"/>
+      <c r="T44" s="94"/>
+      <c r="U44" s="94"/>
+      <c r="V44" s="94"/>
+      <c r="W44" s="95"/>
+      <c r="X44" s="78"/>
+      <c r="Y44" s="49"/>
+      <c r="Z44" s="60"/>
+      <c r="AA44" s="61"/>
+      <c r="AB44" s="71"/>
+      <c r="AC44" s="72"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3949,10 +4026,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:O11" xr:uid="{F77A9EEE-A581-42E3-8103-D2264E3EEDD5}">
       <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J11 J12:J43" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J44" xr:uid="{5B39EBA8-BE88-497B-9866-CC1AD5E7247C}">
       <formula1>"yes, no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:K43" xr:uid="{53ECF302-A855-4FB9-844A-C7CE01367649}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:K44" xr:uid="{53ECF302-A855-4FB9-844A-C7CE01367649}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3963,21 +4040,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD7D549-C187-4DCD-8DD0-20217DC34E3E}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
@@ -3990,8 +4067,11 @@
       <c r="D1" s="85" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="102">
         <v>44578</v>
       </c>
@@ -4005,247 +4085,258 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="103"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="40"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="103">
+        <v>44582</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="128" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="140" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="103"/>
       <c r="B4" s="120"/>
       <c r="C4" s="128"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="103"/>
       <c r="B5" s="120"/>
       <c r="C5" s="128"/>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="103"/>
       <c r="B6" s="120"/>
       <c r="C6" s="128"/>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="103"/>
       <c r="B7" s="120"/>
       <c r="C7" s="128"/>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="103"/>
       <c r="B8" s="120"/>
       <c r="C8" s="128"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="103"/>
       <c r="B9" s="120"/>
       <c r="C9" s="128"/>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="103"/>
       <c r="B10" s="120"/>
       <c r="C10" s="128"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="103"/>
       <c r="B11" s="120"/>
       <c r="C11" s="128"/>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="103"/>
       <c r="B12" s="120"/>
       <c r="C12" s="128"/>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="103"/>
       <c r="B13" s="120"/>
       <c r="C13" s="128"/>
       <c r="D13" s="42"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="103"/>
       <c r="B14" s="120"/>
       <c r="C14" s="128"/>
       <c r="D14" s="42"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="103"/>
       <c r="B15" s="120"/>
       <c r="C15" s="128"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="103"/>
       <c r="B16" s="120"/>
       <c r="C16" s="128"/>
       <c r="D16" s="42"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="103"/>
       <c r="B17" s="120"/>
       <c r="C17" s="128"/>
       <c r="D17" s="42"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="103"/>
       <c r="B18" s="120"/>
       <c r="C18" s="128"/>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="103"/>
       <c r="B19" s="120"/>
       <c r="C19" s="128"/>
       <c r="D19" s="42"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="103"/>
       <c r="B20" s="120"/>
       <c r="C20" s="128"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="103"/>
       <c r="B21" s="120"/>
       <c r="C21" s="128"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="103"/>
       <c r="B22" s="120"/>
       <c r="C22" s="128"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="103"/>
       <c r="B23" s="120"/>
       <c r="C23" s="128"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="103"/>
       <c r="B24" s="120"/>
       <c r="C24" s="128"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="103"/>
       <c r="B25" s="120"/>
       <c r="C25" s="128"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="103"/>
       <c r="B26" s="120"/>
       <c r="C26" s="128"/>
       <c r="D26" s="42"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="103"/>
       <c r="B27" s="120"/>
       <c r="C27" s="128"/>
       <c r="D27" s="42"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="103"/>
       <c r="B28" s="120"/>
       <c r="C28" s="128"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="103"/>
       <c r="B29" s="120"/>
       <c r="C29" s="128"/>
       <c r="D29" s="42"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="103"/>
       <c r="B30" s="120"/>
       <c r="C30" s="128"/>
       <c r="D30" s="42"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="103"/>
       <c r="B31" s="120"/>
       <c r="C31" s="128"/>
       <c r="D31" s="42"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="103"/>
       <c r="B32" s="120"/>
       <c r="C32" s="128"/>
       <c r="D32" s="42"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="103"/>
       <c r="B33" s="120"/>
       <c r="C33" s="128"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="103"/>
       <c r="B34" s="120"/>
       <c r="C34" s="128"/>
       <c r="D34" s="42"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="103"/>
       <c r="B35" s="120"/>
       <c r="C35" s="128"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="103"/>
       <c r="B36" s="120"/>
       <c r="C36" s="128"/>
       <c r="D36" s="42"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="103"/>
       <c r="B37" s="120"/>
       <c r="C37" s="128"/>
       <c r="D37" s="42"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="103"/>
       <c r="B38" s="120"/>
       <c r="C38" s="128"/>
       <c r="D38" s="42"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="103"/>
       <c r="B39" s="120"/>
       <c r="C39" s="128"/>
       <c r="D39" s="42"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="103"/>
       <c r="B40" s="120"/>
       <c r="C40" s="128"/>
       <c r="D40" s="42"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="103"/>
       <c r="B41" s="120"/>
       <c r="C41" s="128"/>
       <c r="D41" s="42"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="103"/>
       <c r="B42" s="120"/>
       <c r="C42" s="128"/>
       <c r="D42" s="42"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="106"/>
       <c r="B43" s="121"/>
       <c r="C43" s="129"/>
@@ -4253,6 +4344,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4264,13 +4356,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -4293,20 +4385,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
@@ -4335,7 +4427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="18" t="s">
@@ -4358,7 +4450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="19" t="s">
@@ -4381,7 +4473,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="19" t="s">
@@ -4402,7 +4494,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
@@ -4429,7 +4521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
@@ -4454,7 +4546,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
@@ -4479,7 +4571,7 @@
       </c>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>38</v>
       </c>
@@ -4508,7 +4600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
@@ -4535,7 +4627,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -4558,7 +4650,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>40</v>
       </c>
@@ -4581,7 +4673,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>38</v>
       </c>
@@ -4606,7 +4698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="29"/>
       <c r="C13" s="23"/>
@@ -4617,7 +4709,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>40</v>
       </c>
@@ -4642,7 +4734,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>40</v>
       </c>
@@ -4669,7 +4761,7 @@
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
@@ -4696,7 +4788,7 @@
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>40</v>
       </c>
@@ -4721,7 +4813,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
@@ -4748,7 +4840,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>40</v>
       </c>
@@ -4775,7 +4867,7 @@
       </c>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>40</v>
       </c>
@@ -4798,7 +4890,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>40</v>
       </c>
@@ -4823,7 +4915,7 @@
       </c>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -4846,7 +4938,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
@@ -4857,7 +4949,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
@@ -4868,7 +4960,7 @@
       <c r="H24" s="37"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="30"/>
       <c r="C25" s="25"/>
@@ -4893,14 +4985,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="1" max="1" width="105.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -4911,7 +5003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>93</v>
       </c>
@@ -4922,7 +5014,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -4930,7 +5022,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>64</v>
       </c>
@@ -4938,7 +5030,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -4946,19 +5038,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="39"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="39"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="39"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="39"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="39"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all major scripts
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC3B75-5ACA-4FF6-8E4F-02E84845F194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EADE40-4D24-47C8-9A71-6B4B7292D578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="249">
   <si>
     <t>Date run</t>
   </si>
@@ -789,9 +789,6 @@
     <t>base_simulation_and_model_HS.PO.R</t>
   </si>
   <si>
-    <t>Test_HS.PO_one.indv.per.parent</t>
-  </si>
-  <si>
     <t>First looped simulation running the combined HS and PO model.</t>
   </si>
   <si>
@@ -819,9 +816,6 @@
     <t>Test_HS.only</t>
   </si>
   <si>
-    <t>HSOnly_one.indv.per.parent</t>
-  </si>
-  <si>
     <t>Everything the same as with the HS/PO model, but only using HS relationships.</t>
   </si>
   <si>
@@ -832,6 +826,73 @@
   </si>
   <si>
     <t>running</t>
+  </si>
+  <si>
+    <t>Chains converged consistently.</t>
+  </si>
+  <si>
+    <t>Definitely get some funny results. Should bump burn-in period up to 50,000</t>
+  </si>
+  <si>
+    <t>Looks great</t>
+  </si>
+  <si>
+    <t>Yes, but could use some optimizing</t>
+  </si>
+  <si>
+    <t>Chains converged consistently. Didn't look too different from the HS|PO model.</t>
+  </si>
+  <si>
+    <t>Patterns are slightly different from the HS|PO model, but not particularly worse or better.</t>
+  </si>
+  <si>
+    <t>Plots look solid, but thinking I may want to bump thinning up to 20</t>
+  </si>
+  <si>
+    <t>Yes, but could use some optimizing. Nothing majorly different in diagnostics between this and the HS|PO model.</t>
+  </si>
+  <si>
+    <t>HS.PO_one.indv.per.parent</t>
+  </si>
+  <si>
+    <t>HS.only_one.indv.per.parent</t>
+  </si>
+  <si>
+    <t>Two instances failed to converge (Rhat &gt; 1.01). Otherwise looks great!</t>
+  </si>
+  <si>
+    <t>Looks a little different from the HS model w/ all samples, but not qualitatively better or worse.</t>
+  </si>
+  <si>
+    <t>Looks solid</t>
+  </si>
+  <si>
+    <t>Yes, but could use some optimizing.</t>
+  </si>
+  <si>
+    <t>Looks a little different from the HS|PO model w/ all samples. But not qualitatively better or worse.</t>
+  </si>
+  <si>
+    <t>HS.PO_surv.prior.R</t>
+  </si>
+  <si>
+    <t>HS.PO_surv.prior</t>
+  </si>
+  <si>
+    <t>HS.PO_new.compsDF</t>
+  </si>
+  <si>
+    <t>Discovered I had the wrong number of negative comparisons; my negative comparisons were only in reference to the parent of interest in the HS model, even though I removed the possibility of half-sibs. In other words, if one parent is positive, then I must discount the negative comparisons for the other parent as well BECAUSE I'm eliminating full siblings.</t>
+  </si>
+  <si>
+    <t>I've noticed that survival estimates vary quite a lot. What if I assume we have prior knowledge around this?
+Set prior on survival to normal distribution with mean of 0.825 and sd of 0.005</t>
+  </si>
+  <si>
+    <t>HS.only_new.compsDF</t>
+  </si>
+  <si>
+    <t>Run the HS only model with the correct number of comparisons to compare to the HS|PO model</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1899,6 +1960,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2222,33 +2286,33 @@
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5546875" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.7109375" style="39" customWidth="1"/>
-    <col min="18" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="23" width="25.28515625" customWidth="1"/>
+    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
+    <col min="18" max="21" width="19.5546875" customWidth="1"/>
+    <col min="22" max="23" width="25.33203125" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -2337,7 +2401,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="100" t="s">
         <v>106</v>
       </c>
@@ -2388,7 +2452,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="103" t="s">
         <v>107</v>
       </c>
@@ -2439,7 +2503,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="103" t="s">
         <v>108</v>
       </c>
@@ -2490,7 +2554,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
@@ -2539,7 +2603,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
@@ -2592,7 +2656,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
@@ -2639,7 +2703,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="91" t="s">
         <v>128</v>
       </c>
@@ -2672,7 +2736,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="91" t="s">
         <v>129</v>
       </c>
@@ -2719,7 +2783,7 @@
       <c r="AB9" s="67"/>
       <c r="AC9" s="68"/>
     </row>
-    <row r="10" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="91" t="s">
         <v>131</v>
       </c>
@@ -2776,7 +2840,7 @@
       <c r="AB10" s="67"/>
       <c r="AC10" s="68"/>
     </row>
-    <row r="11" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="91" t="s">
         <v>144</v>
       </c>
@@ -2829,7 +2893,7 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
         <v>146</v>
       </c>
@@ -2888,7 +2952,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
         <v>152</v>
       </c>
@@ -2949,7 +3013,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
         <v>178</v>
       </c>
@@ -3008,7 +3072,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="90" t="s">
         <v>134</v>
       </c>
@@ -3069,7 +3133,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="90" t="s">
         <v>134</v>
       </c>
@@ -3130,7 +3194,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A17" s="91" t="s">
         <v>193</v>
       </c>
@@ -3193,7 +3257,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="s">
         <v>202</v>
       </c>
@@ -3242,7 +3306,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="91" t="s">
         <v>202</v>
       </c>
@@ -3291,7 +3355,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="91" t="s">
         <v>205</v>
       </c>
@@ -3326,7 +3390,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -3357,7 +3421,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -3388,7 +3452,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -3419,7 +3483,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -3450,7 +3514,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -3481,7 +3545,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -3512,7 +3576,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -3543,7 +3607,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -3574,7 +3638,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -3605,7 +3669,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -3636,7 +3700,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -3667,7 +3731,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -3698,7 +3762,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -3729,7 +3793,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -3760,7 +3824,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -3791,7 +3855,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -3822,7 +3886,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -3853,7 +3917,7 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -3884,7 +3948,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -3915,7 +3979,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -3946,7 +4010,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -3977,7 +4041,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -4008,7 +4072,7 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="91"/>
       <c r="C43" s="103"/>
@@ -4039,7 +4103,7 @@
       <c r="AB43" s="69"/>
       <c r="AC43" s="70"/>
     </row>
-    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="105"/>
       <c r="B44" s="94"/>
       <c r="C44" s="106"/>
@@ -4092,37 +4156,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0949DA-C0C5-4F9C-B1C9-632432E72B29}">
-  <dimension ref="A1:AD44"/>
+  <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="6" width="39.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="6" width="39.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="31.5546875" customWidth="1"/>
     <col min="17" max="17" width="51" customWidth="1"/>
-    <col min="18" max="18" width="49.7109375" style="39" customWidth="1"/>
-    <col min="19" max="22" width="19.5703125" customWidth="1"/>
-    <col min="23" max="24" width="25.28515625" customWidth="1"/>
+    <col min="18" max="18" width="49.6640625" style="39" customWidth="1"/>
+    <col min="19" max="22" width="19.5546875" customWidth="1"/>
+    <col min="23" max="24" width="25.33203125" customWidth="1"/>
     <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -4139,7 +4206,7 @@
         <v>148</v>
       </c>
       <c r="F1" s="126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G1" s="126" t="s">
         <v>153</v>
@@ -4163,10 +4230,10 @@
         <v>163</v>
       </c>
       <c r="N1" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O1" s="85" t="s">
         <v>164</v>
-      </c>
-      <c r="O1" s="85" t="s">
-        <v>165</v>
       </c>
       <c r="P1" s="131" t="s">
         <v>160</v>
@@ -4214,7 +4281,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="100" t="s">
         <v>213</v>
       </c>
@@ -4226,13 +4293,13 @@
         <v>212</v>
       </c>
       <c r="E2" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" s="127" t="s">
         <v>215</v>
-      </c>
-      <c r="F2" s="127" t="s">
-        <v>218</v>
-      </c>
-      <c r="G2" s="127" t="s">
-        <v>216</v>
       </c>
       <c r="H2" s="127">
         <v>15</v>
@@ -4244,16 +4311,24 @@
         <v>40000</v>
       </c>
       <c r="K2" s="114" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="L2" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="139" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2" s="139" t="s">
         <v>228</v>
       </c>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="137"/>
+      <c r="O2" s="139" t="s">
+        <v>229</v>
+      </c>
+      <c r="P2" s="108" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="141"/>
       <c r="R2" s="108"/>
       <c r="S2" s="96"/>
       <c r="T2" s="97"/>
@@ -4268,25 +4343,25 @@
       <c r="AC2" s="63"/>
       <c r="AD2" s="64"/>
     </row>
-    <row r="3" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="103" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="91"/>
       <c r="C3" s="102">
         <v>44648</v>
       </c>
       <c r="D3" s="120" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="128" t="s">
-        <v>225</v>
-      </c>
       <c r="F3" s="128" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G3" s="127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H3" s="127">
         <v>15</v>
@@ -4298,16 +4373,24 @@
         <v>40000</v>
       </c>
       <c r="K3" s="114" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="L3" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="133"/>
-      <c r="Q3" s="81"/>
+        <v>138</v>
+      </c>
+      <c r="M3" s="139" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="140" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="P3" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q3" s="82"/>
       <c r="R3" s="109"/>
       <c r="S3" s="89"/>
       <c r="T3" s="90"/>
@@ -4322,25 +4405,25 @@
       <c r="AC3" s="65"/>
       <c r="AD3" s="66"/>
     </row>
-    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="103" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="102">
         <v>44648</v>
       </c>
       <c r="D4" s="120" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="E4" s="128" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F4" s="128" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G4" s="128" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H4" s="127">
         <v>15</v>
@@ -4352,16 +4435,24 @@
         <v>40000</v>
       </c>
       <c r="K4" s="114" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="L4" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="81"/>
+        <v>138</v>
+      </c>
+      <c r="M4" s="140" t="s">
+        <v>227</v>
+      </c>
+      <c r="N4" s="140" t="s">
+        <v>241</v>
+      </c>
+      <c r="O4" s="140" t="s">
+        <v>239</v>
+      </c>
+      <c r="P4" s="135" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q4" s="82"/>
       <c r="R4" s="109"/>
       <c r="S4" s="89"/>
       <c r="T4" s="90"/>
@@ -4376,25 +4467,25 @@
       <c r="AC4" s="65"/>
       <c r="AD4" s="66"/>
     </row>
-    <row r="5" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="91"/>
       <c r="C5" s="102">
         <v>44648</v>
       </c>
       <c r="D5" s="120" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="E5" s="128" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F5" s="128" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H5" s="127">
         <v>15</v>
@@ -4406,16 +4497,24 @@
         <v>40000</v>
       </c>
       <c r="K5" s="114" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="L5" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="134"/>
-      <c r="Q5" s="81"/>
+        <v>138</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="O5" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="P5" s="135" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q5" s="82"/>
       <c r="R5" s="109"/>
       <c r="S5" s="89"/>
       <c r="T5" s="90"/>
@@ -4430,24 +4529,46 @@
       <c r="AC5" s="65"/>
       <c r="AD5" s="66"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
+    <row r="6" spans="1:30" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="91" t="s">
+        <v>213</v>
+      </c>
       <c r="B6" s="91"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="81"/>
+      <c r="C6" s="102">
+        <v>44652</v>
+      </c>
+      <c r="D6" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="128" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="H6" s="128">
+        <v>20</v>
+      </c>
+      <c r="I6" s="128">
+        <v>40000</v>
+      </c>
+      <c r="J6" s="124">
+        <v>40000</v>
+      </c>
+      <c r="K6" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="82"/>
       <c r="R6" s="109"/>
       <c r="S6" s="89"/>
       <c r="T6" s="90"/>
@@ -4462,24 +4583,46 @@
       <c r="AC6" s="65"/>
       <c r="AD6" s="66"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
+    <row r="7" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="91" t="s">
+        <v>242</v>
+      </c>
       <c r="B7" s="91"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="134"/>
-      <c r="Q7" s="81"/>
+      <c r="C7" s="103">
+        <v>44652</v>
+      </c>
+      <c r="D7" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="E7" s="128" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="128">
+        <v>20</v>
+      </c>
+      <c r="I7" s="128">
+        <v>40000</v>
+      </c>
+      <c r="J7" s="124">
+        <v>40000</v>
+      </c>
+      <c r="K7" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="82"/>
       <c r="R7" s="109"/>
       <c r="S7" s="89"/>
       <c r="T7" s="90"/>
@@ -4494,24 +4637,46 @@
       <c r="AC7" s="65"/>
       <c r="AD7" s="66"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
+    <row r="8" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="91" t="s">
+        <v>221</v>
+      </c>
       <c r="B8" s="91"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="128"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="134"/>
-      <c r="Q8" s="81"/>
+      <c r="C8" s="102">
+        <v>44652</v>
+      </c>
+      <c r="D8" s="120" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="128" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="128">
+        <v>20</v>
+      </c>
+      <c r="I8" s="128">
+        <v>40000</v>
+      </c>
+      <c r="J8" s="124">
+        <v>40000</v>
+      </c>
+      <c r="K8" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="135"/>
+      <c r="Q8" s="82"/>
       <c r="R8" s="109"/>
       <c r="S8" s="89"/>
       <c r="T8" s="90"/>
@@ -4526,7 +4691,7 @@
       <c r="AC8" s="65"/>
       <c r="AD8" s="66"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="91"/>
       <c r="B9" s="91"/>
       <c r="C9" s="103"/>
@@ -4539,26 +4704,26 @@
       <c r="J9" s="124"/>
       <c r="K9" s="114"/>
       <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="134"/>
-      <c r="Q9" s="81"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="135"/>
+      <c r="Q9" s="82"/>
       <c r="R9" s="109"/>
       <c r="S9" s="89"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="90"/>
       <c r="X9" s="88"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="56"/>
-      <c r="AB9" s="57"/>
-      <c r="AC9" s="67"/>
-      <c r="AD9" s="68"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="54"/>
+      <c r="AB9" s="55"/>
+      <c r="AC9" s="65"/>
+      <c r="AD9" s="66"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="91"/>
       <c r="B10" s="91"/>
       <c r="C10" s="103"/>
@@ -4571,11 +4736,11 @@
       <c r="J10" s="124"/>
       <c r="K10" s="114"/>
       <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="134"/>
-      <c r="Q10" s="81"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="135"/>
+      <c r="Q10" s="82"/>
       <c r="R10" s="109"/>
       <c r="S10" s="89"/>
       <c r="T10" s="91"/>
@@ -4590,7 +4755,7 @@
       <c r="AC10" s="67"/>
       <c r="AD10" s="68"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="91"/>
       <c r="B11" s="91"/>
       <c r="C11" s="103"/>
@@ -4603,11 +4768,11 @@
       <c r="J11" s="124"/>
       <c r="K11" s="114"/>
       <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="81"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="135"/>
+      <c r="Q11" s="82"/>
       <c r="R11" s="109"/>
       <c r="S11" s="89"/>
       <c r="T11" s="91"/>
@@ -4622,8 +4787,8 @@
       <c r="AC11" s="67"/>
       <c r="AD11" s="68"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" s="91"/>
       <c r="B12" s="91"/>
       <c r="C12" s="103"/>
       <c r="D12" s="120"/>
@@ -4646,7 +4811,7 @@
       <c r="U12" s="91"/>
       <c r="V12" s="91"/>
       <c r="W12" s="91"/>
-      <c r="X12" s="92"/>
+      <c r="X12" s="88"/>
       <c r="Y12" s="76"/>
       <c r="Z12" s="47"/>
       <c r="AA12" s="56"/>
@@ -4654,7 +4819,7 @@
       <c r="AC12" s="67"/>
       <c r="AD12" s="68"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="90"/>
       <c r="B13" s="91"/>
       <c r="C13" s="103"/>
@@ -4665,8 +4830,8 @@
       <c r="H13" s="128"/>
       <c r="I13" s="128"/>
       <c r="J13" s="124"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="42"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
@@ -4686,7 +4851,7 @@
       <c r="AC13" s="67"/>
       <c r="AD13" s="68"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="90"/>
       <c r="B14" s="91"/>
       <c r="C14" s="103"/>
@@ -4711,14 +4876,14 @@
       <c r="V14" s="91"/>
       <c r="W14" s="91"/>
       <c r="X14" s="92"/>
-      <c r="Y14" s="77"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="58"/>
-      <c r="AB14" s="59"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="70"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y14" s="76"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="56"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="68"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="90"/>
       <c r="B15" s="91"/>
       <c r="C15" s="103"/>
@@ -4729,8 +4894,8 @@
       <c r="H15" s="128"/>
       <c r="I15" s="128"/>
       <c r="J15" s="124"/>
-      <c r="K15" s="114"/>
-      <c r="L15" s="41"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="42"/>
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
@@ -4743,14 +4908,14 @@
       <c r="V15" s="91"/>
       <c r="W15" s="91"/>
       <c r="X15" s="92"/>
-      <c r="Y15" s="76"/>
-      <c r="Z15" s="47"/>
-      <c r="AA15" s="56"/>
-      <c r="AB15" s="57"/>
-      <c r="AC15" s="67"/>
-      <c r="AD15" s="68"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y15" s="77"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="70"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="90"/>
       <c r="B16" s="91"/>
       <c r="C16" s="103"/>
@@ -4761,8 +4926,8 @@
       <c r="H16" s="128"/>
       <c r="I16" s="128"/>
       <c r="J16" s="124"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="42"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="41"/>
       <c r="M16" s="42"/>
       <c r="N16" s="42"/>
       <c r="O16" s="42"/>
@@ -4775,15 +4940,15 @@
       <c r="V16" s="91"/>
       <c r="W16" s="91"/>
       <c r="X16" s="92"/>
-      <c r="Y16" s="77"/>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="58"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="69"/>
-      <c r="AD16" s="70"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="56"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="67"/>
+      <c r="AD16" s="68"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" s="90"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
       <c r="D17" s="120"/>
@@ -4793,8 +4958,8 @@
       <c r="H17" s="128"/>
       <c r="I17" s="128"/>
       <c r="J17" s="124"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="83"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="42"/>
       <c r="M17" s="42"/>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
@@ -4814,7 +4979,7 @@
       <c r="AC17" s="69"/>
       <c r="AD17" s="70"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -4846,7 +5011,7 @@
       <c r="AC18" s="69"/>
       <c r="AD18" s="70"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -4878,7 +5043,7 @@
       <c r="AC19" s="69"/>
       <c r="AD19" s="70"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -4910,7 +5075,7 @@
       <c r="AC20" s="69"/>
       <c r="AD20" s="70"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -4942,7 +5107,7 @@
       <c r="AC21" s="69"/>
       <c r="AD21" s="70"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -4974,7 +5139,7 @@
       <c r="AC22" s="69"/>
       <c r="AD22" s="70"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -5006,7 +5171,7 @@
       <c r="AC23" s="69"/>
       <c r="AD23" s="70"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -5038,7 +5203,7 @@
       <c r="AC24" s="69"/>
       <c r="AD24" s="70"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -5070,7 +5235,7 @@
       <c r="AC25" s="69"/>
       <c r="AD25" s="70"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -5102,7 +5267,7 @@
       <c r="AC26" s="69"/>
       <c r="AD26" s="70"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -5134,7 +5299,7 @@
       <c r="AC27" s="69"/>
       <c r="AD27" s="70"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -5166,7 +5331,7 @@
       <c r="AC28" s="69"/>
       <c r="AD28" s="70"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -5198,7 +5363,7 @@
       <c r="AC29" s="69"/>
       <c r="AD29" s="70"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -5230,7 +5395,7 @@
       <c r="AC30" s="69"/>
       <c r="AD30" s="70"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -5262,7 +5427,7 @@
       <c r="AC31" s="69"/>
       <c r="AD31" s="70"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -5294,7 +5459,7 @@
       <c r="AC32" s="69"/>
       <c r="AD32" s="70"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -5326,7 +5491,7 @@
       <c r="AC33" s="69"/>
       <c r="AD33" s="70"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -5358,7 +5523,7 @@
       <c r="AC34" s="69"/>
       <c r="AD34" s="70"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -5390,7 +5555,7 @@
       <c r="AC35" s="69"/>
       <c r="AD35" s="70"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -5422,7 +5587,7 @@
       <c r="AC36" s="69"/>
       <c r="AD36" s="70"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -5454,7 +5619,7 @@
       <c r="AC37" s="69"/>
       <c r="AD37" s="70"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -5486,8 +5651,8 @@
       <c r="AC38" s="69"/>
       <c r="AD38" s="70"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39" s="104"/>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A39" s="91"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
       <c r="D39" s="120"/>
@@ -5518,7 +5683,7 @@
       <c r="AC39" s="69"/>
       <c r="AD39" s="70"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -5550,7 +5715,7 @@
       <c r="AC40" s="69"/>
       <c r="AD40" s="70"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -5582,7 +5747,7 @@
       <c r="AC41" s="69"/>
       <c r="AD41" s="70"/>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -5614,7 +5779,7 @@
       <c r="AC42" s="69"/>
       <c r="AD42" s="70"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="91"/>
       <c r="C43" s="103"/>
@@ -5646,47 +5811,156 @@
       <c r="AC43" s="69"/>
       <c r="AD43" s="70"/>
     </row>
-    <row r="44" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="105"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="129"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="129"/>
-      <c r="H44" s="129"/>
-      <c r="I44" s="129"/>
-      <c r="J44" s="125"/>
-      <c r="K44" s="117"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="130"/>
-      <c r="N44" s="130"/>
-      <c r="O44" s="130"/>
-      <c r="P44" s="136"/>
-      <c r="Q44" s="138"/>
-      <c r="R44" s="110"/>
-      <c r="S44" s="93"/>
-      <c r="T44" s="94"/>
-      <c r="U44" s="94"/>
-      <c r="V44" s="94"/>
-      <c r="W44" s="94"/>
-      <c r="X44" s="95"/>
-      <c r="Y44" s="78"/>
-      <c r="Z44" s="49"/>
-      <c r="AA44" s="60"/>
-      <c r="AB44" s="61"/>
-      <c r="AC44" s="71"/>
-      <c r="AD44" s="72"/>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A44" s="104"/>
+      <c r="B44" s="91"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="128"/>
+      <c r="F44" s="128"/>
+      <c r="G44" s="128"/>
+      <c r="H44" s="128"/>
+      <c r="I44" s="128"/>
+      <c r="J44" s="124"/>
+      <c r="K44" s="116"/>
+      <c r="L44" s="83"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="42"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="135"/>
+      <c r="Q44" s="82"/>
+      <c r="R44" s="109"/>
+      <c r="S44" s="89"/>
+      <c r="T44" s="91"/>
+      <c r="U44" s="91"/>
+      <c r="V44" s="91"/>
+      <c r="W44" s="91"/>
+      <c r="X44" s="92"/>
+      <c r="Y44" s="77"/>
+      <c r="Z44" s="48"/>
+      <c r="AA44" s="58"/>
+      <c r="AB44" s="59"/>
+      <c r="AC44" s="69"/>
+      <c r="AD44" s="70"/>
+    </row>
+    <row r="45" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="105"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="106"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="129"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="129"/>
+      <c r="H45" s="129"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="117"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="130"/>
+      <c r="N45" s="130"/>
+      <c r="O45" s="130"/>
+      <c r="P45" s="136"/>
+      <c r="Q45" s="138"/>
+      <c r="R45" s="110"/>
+      <c r="S45" s="93"/>
+      <c r="T45" s="94"/>
+      <c r="U45" s="94"/>
+      <c r="V45" s="94"/>
+      <c r="W45" s="94"/>
+      <c r="X45" s="95"/>
+      <c r="Y45" s="78"/>
+      <c r="Z45" s="49"/>
+      <c r="AA45" s="60"/>
+      <c r="AB45" s="61"/>
+      <c r="AC45" s="71"/>
+      <c r="AD45" s="72"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
+    </row>
+    <row r="49" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="39"/>
+    </row>
+    <row r="50" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="39"/>
+    </row>
+    <row r="51" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M51" s="39"/>
+      <c r="N51" s="39"/>
+      <c r="O51" s="39"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="39"/>
+    </row>
+    <row r="52" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="39"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="39"/>
+    </row>
+    <row r="53" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M53" s="39"/>
+      <c r="N53" s="39"/>
+      <c r="O53" s="39"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="39"/>
+    </row>
+    <row r="54" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M54" s="39"/>
+      <c r="N54" s="39"/>
+      <c r="O54" s="39"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="39"/>
+    </row>
+    <row r="55" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="39"/>
+    </row>
+    <row r="56" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M56" s="39"/>
+      <c r="N56" s="39"/>
+      <c r="O56" s="39"/>
+      <c r="P56" s="39"/>
+      <c r="Q56" s="39"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12:L44" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L45" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K44" xr:uid="{50F97EAA-3C25-42AF-880C-C780B18C2C28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K45" xr:uid="{50F97EAA-3C25-42AF-880C-C780B18C2C28}">
       <formula1>"yes, no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:P11" xr:uid="{A8837422-8676-43AE-8FBF-E37D051E89A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L12" xr:uid="{A8837422-8676-43AE-8FBF-E37D051E89A9}">
       <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5702,15 +5976,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="96.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="96.109375" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
@@ -5727,7 +6001,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="102">
         <v>44578</v>
       </c>
@@ -5741,7 +6015,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="103">
         <v>44582</v>
       </c>
@@ -5758,241 +6032,241 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="103"/>
       <c r="B4" s="120"/>
       <c r="C4" s="128"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="103"/>
       <c r="B5" s="120"/>
       <c r="C5" s="128"/>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="103"/>
       <c r="B6" s="120"/>
       <c r="C6" s="128"/>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="103"/>
       <c r="B7" s="120"/>
       <c r="C7" s="128"/>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="103"/>
       <c r="B8" s="120"/>
       <c r="C8" s="128"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="103"/>
       <c r="B9" s="120"/>
       <c r="C9" s="128"/>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="103"/>
       <c r="B10" s="120"/>
       <c r="C10" s="128"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="103"/>
       <c r="B11" s="120"/>
       <c r="C11" s="128"/>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="103"/>
       <c r="B12" s="120"/>
       <c r="C12" s="128"/>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="103"/>
       <c r="B13" s="120"/>
       <c r="C13" s="128"/>
       <c r="D13" s="42"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="103"/>
       <c r="B14" s="120"/>
       <c r="C14" s="128"/>
       <c r="D14" s="42"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="103"/>
       <c r="B15" s="120"/>
       <c r="C15" s="128"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="103"/>
       <c r="B16" s="120"/>
       <c r="C16" s="128"/>
       <c r="D16" s="42"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="103"/>
       <c r="B17" s="120"/>
       <c r="C17" s="128"/>
       <c r="D17" s="42"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="103"/>
       <c r="B18" s="120"/>
       <c r="C18" s="128"/>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="103"/>
       <c r="B19" s="120"/>
       <c r="C19" s="128"/>
       <c r="D19" s="42"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="103"/>
       <c r="B20" s="120"/>
       <c r="C20" s="128"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="103"/>
       <c r="B21" s="120"/>
       <c r="C21" s="128"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="103"/>
       <c r="B22" s="120"/>
       <c r="C22" s="128"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="103"/>
       <c r="B23" s="120"/>
       <c r="C23" s="128"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="103"/>
       <c r="B24" s="120"/>
       <c r="C24" s="128"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="103"/>
       <c r="B25" s="120"/>
       <c r="C25" s="128"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="103"/>
       <c r="B26" s="120"/>
       <c r="C26" s="128"/>
       <c r="D26" s="42"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="103"/>
       <c r="B27" s="120"/>
       <c r="C27" s="128"/>
       <c r="D27" s="42"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="103"/>
       <c r="B28" s="120"/>
       <c r="C28" s="128"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="103"/>
       <c r="B29" s="120"/>
       <c r="C29" s="128"/>
       <c r="D29" s="42"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="103"/>
       <c r="B30" s="120"/>
       <c r="C30" s="128"/>
       <c r="D30" s="42"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="103"/>
       <c r="B31" s="120"/>
       <c r="C31" s="128"/>
       <c r="D31" s="42"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="103"/>
       <c r="B32" s="120"/>
       <c r="C32" s="128"/>
       <c r="D32" s="42"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="103"/>
       <c r="B33" s="120"/>
       <c r="C33" s="128"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="103"/>
       <c r="B34" s="120"/>
       <c r="C34" s="128"/>
       <c r="D34" s="42"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="103"/>
       <c r="B35" s="120"/>
       <c r="C35" s="128"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="103"/>
       <c r="B36" s="120"/>
       <c r="C36" s="128"/>
       <c r="D36" s="42"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="103"/>
       <c r="B37" s="120"/>
       <c r="C37" s="128"/>
       <c r="D37" s="42"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="103"/>
       <c r="B38" s="120"/>
       <c r="C38" s="128"/>
       <c r="D38" s="42"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="103"/>
       <c r="B39" s="120"/>
       <c r="C39" s="128"/>
       <c r="D39" s="42"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="103"/>
       <c r="B40" s="120"/>
       <c r="C40" s="128"/>
       <c r="D40" s="42"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="103"/>
       <c r="B41" s="120"/>
       <c r="C41" s="128"/>
       <c r="D41" s="42"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="103"/>
       <c r="B42" s="120"/>
       <c r="C42" s="128"/>
       <c r="D42" s="42"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="106"/>
       <c r="B43" s="121"/>
       <c r="C43" s="129"/>
@@ -6012,13 +6286,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -6041,20 +6315,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.7109375" customWidth="1"/>
-    <col min="8" max="8" width="39.7109375" customWidth="1"/>
-    <col min="9" max="9" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.6640625" customWidth="1"/>
+    <col min="8" max="8" width="39.6640625" customWidth="1"/>
+    <col min="9" max="9" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
@@ -6083,7 +6357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="18" t="s">
@@ -6106,7 +6380,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="19" t="s">
@@ -6129,7 +6403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="19" t="s">
@@ -6150,7 +6424,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
@@ -6177,7 +6451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
@@ -6202,7 +6476,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
@@ -6227,7 +6501,7 @@
       </c>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>38</v>
       </c>
@@ -6256,7 +6530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
@@ -6283,7 +6557,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -6306,7 +6580,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>40</v>
       </c>
@@ -6329,7 +6603,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>38</v>
       </c>
@@ -6354,7 +6628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="29"/>
       <c r="C13" s="23"/>
@@ -6365,7 +6639,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>40</v>
       </c>
@@ -6390,7 +6664,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>40</v>
       </c>
@@ -6417,7 +6691,7 @@
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
@@ -6444,7 +6718,7 @@
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>40</v>
       </c>
@@ -6469,7 +6743,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
@@ -6496,7 +6770,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>40</v>
       </c>
@@ -6523,7 +6797,7 @@
       </c>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>40</v>
       </c>
@@ -6546,7 +6820,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>40</v>
       </c>
@@ -6571,7 +6845,7 @@
       </c>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -6594,7 +6868,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="31"/>
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
@@ -6605,7 +6879,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
@@ -6616,7 +6890,7 @@
       <c r="H24" s="37"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="30"/>
       <c r="C25" s="25"/>
@@ -6641,14 +6915,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="105.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="105.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -6659,7 +6933,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>93</v>
       </c>
@@ -6670,7 +6944,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -6678,7 +6952,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>64</v>
       </c>
@@ -6686,7 +6960,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -6694,19 +6968,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="39"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" s="39"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="39"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="39"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="39"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data analysis script and simulation log
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C14A67-C44E-41F8-956F-5E634E13DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CB4010-7D87-4060-8438-FB1C6FF6193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="265">
   <si>
     <t>Date run</t>
   </si>
@@ -926,6 +926,21 @@
   </si>
   <si>
     <t>Yup.</t>
+  </si>
+  <si>
+    <t>HS.PO_test.recaptures.R</t>
+  </si>
+  <si>
+    <t>test.recaptures</t>
+  </si>
+  <si>
+    <t>When removing individual recaptures, we have to decide whether to keep the first instance of capture or the second. I want to see how the choice affects parameter estimates. Only running for 50 iterations, and only using a sample size of 250 per year (1000 total) bc the odds of many recaptures with smaller sample sizes are minimal.</t>
+  </si>
+  <si>
+    <t>Which recapture instance is retained doesn't seem to matter much. There is a slight improvement in precision for each parameter when using the last capture occasion. The bias is slightly improved for survival and lambda with the last capture occasion, but made slightly worse for male and female abundance.</t>
+  </si>
+  <si>
+    <t>Date of analysis</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1998,6 +2013,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4189,11 +4208,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0949DA-C0C5-4F9C-B1C9-632432E72B29}">
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4201,27 +4220,28 @@
     <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5546875" customWidth="1"/>
-    <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="7" width="39.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="31.5546875" customWidth="1"/>
+    <col min="17" max="17" width="51" customWidth="1"/>
+    <col min="18" max="18" width="49.6640625" style="39" customWidth="1"/>
+    <col min="19" max="22" width="19.5546875" customWidth="1"/>
+    <col min="23" max="24" width="25.33203125" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -4231,86 +4251,89 @@
       <c r="C1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="142" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="118" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="F1" s="126" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="126" t="s">
+      <c r="G1" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="126" t="s">
+      <c r="H1" s="126" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="126" t="s">
+      <c r="I1" s="126" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="126" t="s">
+      <c r="J1" s="126" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="122" t="s">
+      <c r="K1" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="L1" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="M1" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="85" t="s">
+      <c r="N1" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="N1" s="85" t="s">
+      <c r="O1" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="O1" s="131" t="s">
+      <c r="P1" s="131" t="s">
         <v>160</v>
       </c>
-      <c r="P1" s="84" t="s">
+      <c r="Q1" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="Q1" s="107" t="s">
+      <c r="R1" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="98" t="s">
+      <c r="S1" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="99" t="s">
+      <c r="T1" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="99" t="s">
+      <c r="U1" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="U1" s="99" t="s">
+      <c r="V1" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="V1" s="99" t="s">
+      <c r="W1" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="W1" s="86" t="s">
+      <c r="X1" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="73" t="s">
+      <c r="Y1" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="44" t="s">
+      <c r="Z1" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="Z1" s="50" t="s">
+      <c r="AA1" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="AA1" s="51" t="s">
+      <c r="AB1" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AC1" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="AC1" s="79" t="s">
+      <c r="AD1" s="79" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="100" t="s">
         <v>213</v>
       </c>
@@ -4318,58 +4341,59 @@
       <c r="C2" s="102">
         <v>44648</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="143"/>
+      <c r="E2" s="119" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="127" t="s">
+      <c r="F2" s="127" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="127" t="s">
+      <c r="G2" s="127" t="s">
         <v>217</v>
       </c>
-      <c r="G2" s="127" t="s">
+      <c r="H2" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H2" s="127">
+      <c r="I2" s="127">
         <v>15</v>
       </c>
-      <c r="I2" s="127">
+      <c r="J2" s="127">
         <v>30000</v>
       </c>
-      <c r="J2" s="123">
+      <c r="K2" s="123">
         <v>40000</v>
       </c>
-      <c r="K2" s="80" t="s">
+      <c r="L2" s="80" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="139" t="s">
+      <c r="M2" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="M2" s="139" t="s">
+      <c r="N2" s="139" t="s">
         <v>228</v>
       </c>
-      <c r="N2" s="139" t="s">
+      <c r="O2" s="139" t="s">
         <v>229</v>
       </c>
-      <c r="O2" s="108" t="s">
+      <c r="P2" s="108" t="s">
         <v>230</v>
       </c>
-      <c r="P2" s="141"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="97"/>
+      <c r="Q2" s="141"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="96"/>
       <c r="T2" s="97"/>
       <c r="U2" s="97"/>
       <c r="V2" s="97"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="64"/>
-    </row>
-    <row r="3" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W2" s="97"/>
+      <c r="X2" s="87"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="64"/>
+    </row>
+    <row r="3" spans="1:30" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="103" t="s">
         <v>221</v>
       </c>
@@ -4377,58 +4401,59 @@
       <c r="C3" s="102">
         <v>44648</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="143"/>
+      <c r="E3" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="F3" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="G3" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="H3" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H3" s="127">
+      <c r="I3" s="127">
         <v>15</v>
       </c>
-      <c r="I3" s="127">
+      <c r="J3" s="127">
         <v>30000</v>
       </c>
-      <c r="J3" s="123">
+      <c r="K3" s="123">
         <v>40000</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="L3" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="L3" s="139" t="s">
+      <c r="M3" s="139" t="s">
         <v>231</v>
       </c>
-      <c r="M3" s="140" t="s">
+      <c r="N3" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="N3" s="140" t="s">
+      <c r="O3" s="140" t="s">
         <v>233</v>
       </c>
-      <c r="O3" s="109" t="s">
+      <c r="P3" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="90"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="89"/>
       <c r="T3" s="90"/>
       <c r="U3" s="90"/>
       <c r="V3" s="90"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="66"/>
-    </row>
-    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="90"/>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="55"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="66"/>
+    </row>
+    <row r="4" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="103" t="s">
         <v>220</v>
       </c>
@@ -4436,58 +4461,59 @@
       <c r="C4" s="102">
         <v>44648</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="143"/>
+      <c r="E4" s="120" t="s">
         <v>235</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="F4" s="128" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="128" t="s">
+      <c r="G4" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="128" t="s">
+      <c r="H4" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="H4" s="127">
+      <c r="I4" s="127">
         <v>15</v>
       </c>
-      <c r="I4" s="127">
+      <c r="J4" s="127">
         <v>30000</v>
       </c>
-      <c r="J4" s="123">
+      <c r="K4" s="123">
         <v>40000</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="L4" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="L4" s="140" t="s">
+      <c r="M4" s="140" t="s">
         <v>227</v>
       </c>
-      <c r="M4" s="140" t="s">
+      <c r="N4" s="140" t="s">
         <v>241</v>
       </c>
-      <c r="N4" s="140" t="s">
+      <c r="O4" s="140" t="s">
         <v>239</v>
       </c>
-      <c r="O4" s="135" t="s">
+      <c r="P4" s="135" t="s">
         <v>240</v>
       </c>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="90"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="89"/>
       <c r="T4" s="90"/>
       <c r="U4" s="90"/>
       <c r="V4" s="90"/>
-      <c r="W4" s="88"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="65"/>
-      <c r="AC4" s="66"/>
-    </row>
-    <row r="5" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="90"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="65"/>
+      <c r="AD4" s="66"/>
+    </row>
+    <row r="5" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="91" t="s">
         <v>219</v>
       </c>
@@ -4495,58 +4521,59 @@
       <c r="C5" s="102">
         <v>44648</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="143"/>
+      <c r="E5" s="120" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="128" t="s">
+      <c r="F5" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="128" t="s">
+      <c r="G5" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G5" s="127" t="s">
+      <c r="H5" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H5" s="127">
+      <c r="I5" s="127">
         <v>15</v>
       </c>
-      <c r="I5" s="127">
+      <c r="J5" s="127">
         <v>30000</v>
       </c>
-      <c r="J5" s="123">
+      <c r="K5" s="123">
         <v>40000</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="L5" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="M5" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="N5" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="O5" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="O5" s="135" t="s">
+      <c r="P5" s="135" t="s">
         <v>240</v>
       </c>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="109"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="89"/>
       <c r="T5" s="90"/>
       <c r="U5" s="90"/>
       <c r="V5" s="90"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="66"/>
-    </row>
-    <row r="6" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="W5" s="90"/>
+      <c r="X5" s="88"/>
+      <c r="Y5" s="75"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="65"/>
+      <c r="AD5" s="66"/>
+    </row>
+    <row r="6" spans="1:30" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="91" t="s">
         <v>213</v>
       </c>
@@ -4554,58 +4581,61 @@
       <c r="C6" s="102">
         <v>44652</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E6" s="120" t="s">
         <v>244</v>
       </c>
-      <c r="E6" s="128" t="s">
+      <c r="F6" s="128" t="s">
         <v>245</v>
       </c>
-      <c r="F6" s="128" t="s">
+      <c r="G6" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G6" s="127" t="s">
+      <c r="H6" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="H6" s="128">
+      <c r="I6" s="128">
         <v>20</v>
       </c>
-      <c r="I6" s="128">
+      <c r="J6" s="128">
         <v>40000</v>
       </c>
-      <c r="J6" s="124">
+      <c r="K6" s="124">
         <v>40000</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="L6" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="M6" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="N6" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="N6" s="42" t="s">
+      <c r="O6" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="O6" s="135" t="s">
+      <c r="P6" s="135" t="s">
         <v>252</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="89"/>
-      <c r="S6" s="90"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="89"/>
       <c r="T6" s="90"/>
       <c r="U6" s="90"/>
       <c r="V6" s="90"/>
-      <c r="W6" s="88"/>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="46"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="55"/>
-      <c r="AB6" s="65"/>
-      <c r="AC6" s="66"/>
-    </row>
-    <row r="7" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="W6" s="90"/>
+      <c r="X6" s="88"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="55"/>
+      <c r="AC6" s="65"/>
+      <c r="AD6" s="66"/>
+    </row>
+    <row r="7" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="91" t="s">
         <v>242</v>
       </c>
@@ -4613,58 +4643,61 @@
       <c r="C7" s="103">
         <v>44652</v>
       </c>
-      <c r="D7" s="120" t="s">
+      <c r="D7" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E7" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="E7" s="128" t="s">
+      <c r="F7" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="F7" s="128" t="s">
+      <c r="G7" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G7" s="127" t="s">
+      <c r="H7" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="H7" s="128">
+      <c r="I7" s="128">
         <v>20</v>
       </c>
-      <c r="I7" s="128">
+      <c r="J7" s="128">
         <v>40000</v>
       </c>
-      <c r="J7" s="124">
+      <c r="K7" s="124">
         <v>40000</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="L7" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="M7" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="M7" s="42" t="s">
+      <c r="N7" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="N7" s="42" t="s">
+      <c r="O7" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="O7" s="135" t="s">
+      <c r="P7" s="135" t="s">
         <v>259</v>
       </c>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="89"/>
-      <c r="S7" s="90"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="89"/>
       <c r="T7" s="90"/>
       <c r="U7" s="90"/>
       <c r="V7" s="90"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="75"/>
-      <c r="Y7" s="46"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="55"/>
-      <c r="AB7" s="65"/>
-      <c r="AC7" s="66"/>
-    </row>
-    <row r="8" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="W7" s="90"/>
+      <c r="X7" s="88"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="55"/>
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="66"/>
+    </row>
+    <row r="8" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="91" t="s">
         <v>221</v>
       </c>
@@ -4672,58 +4705,61 @@
       <c r="C8" s="102">
         <v>44652</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E8" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="E8" s="128" t="s">
+      <c r="F8" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="F8" s="128" t="s">
+      <c r="G8" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G8" s="127" t="s">
+      <c r="H8" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="H8" s="128">
+      <c r="I8" s="128">
         <v>20</v>
       </c>
-      <c r="I8" s="128">
+      <c r="J8" s="128">
         <v>40000</v>
       </c>
-      <c r="J8" s="124">
+      <c r="K8" s="124">
         <v>40000</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="L8" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="L8" s="42" t="s">
+      <c r="M8" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="N8" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="O8" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="O8" s="135" t="s">
+      <c r="P8" s="135" t="s">
         <v>258</v>
       </c>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="109"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="90"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="89"/>
       <c r="T8" s="90"/>
       <c r="U8" s="90"/>
       <c r="V8" s="90"/>
-      <c r="W8" s="88"/>
-      <c r="X8" s="75"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="55"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="66"/>
-    </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="W8" s="90"/>
+      <c r="X8" s="88"/>
+      <c r="Y8" s="75"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="54"/>
+      <c r="AB8" s="55"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="66"/>
+    </row>
+    <row r="9" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="91" t="s">
         <v>213</v>
       </c>
@@ -4731,50 +4767,53 @@
       <c r="C9" s="102">
         <v>44655</v>
       </c>
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E9" s="120" t="s">
         <v>244</v>
       </c>
-      <c r="E9" s="128" t="s">
+      <c r="F9" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="F9" s="128" t="s">
+      <c r="G9" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G9" s="127" t="s">
+      <c r="H9" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H9" s="128">
+      <c r="I9" s="128">
         <v>20</v>
       </c>
-      <c r="I9" s="128">
+      <c r="J9" s="128">
         <v>40000</v>
       </c>
-      <c r="J9" s="124">
-        <v>40000</v>
-      </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L9" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="L9" s="42"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
-      <c r="O9" s="135"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="109"/>
-      <c r="R9" s="89"/>
-      <c r="S9" s="90"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="135"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="89"/>
       <c r="T9" s="90"/>
       <c r="U9" s="90"/>
       <c r="V9" s="90"/>
-      <c r="W9" s="88"/>
-      <c r="X9" s="75"/>
-      <c r="Y9" s="46"/>
-      <c r="Z9" s="54"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="66"/>
-    </row>
-    <row r="10" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="W9" s="90"/>
+      <c r="X9" s="88"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="54"/>
+      <c r="AB9" s="55"/>
+      <c r="AC9" s="65"/>
+      <c r="AD9" s="66"/>
+    </row>
+    <row r="10" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="91" t="s">
         <v>242</v>
       </c>
@@ -4782,50 +4821,53 @@
       <c r="C10" s="102">
         <v>44655</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E10" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="E10" s="128" t="s">
+      <c r="F10" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="128" t="s">
+      <c r="G10" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G10" s="127" t="s">
+      <c r="H10" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H10" s="128">
+      <c r="I10" s="128">
         <v>20</v>
       </c>
-      <c r="I10" s="128">
+      <c r="J10" s="128">
         <v>40000</v>
       </c>
-      <c r="J10" s="124">
-        <v>40000</v>
-      </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L10" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="L10" s="42"/>
       <c r="M10" s="42"/>
       <c r="N10" s="42"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="89"/>
-      <c r="S10" s="90"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="135"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="89"/>
       <c r="T10" s="90"/>
       <c r="U10" s="90"/>
       <c r="V10" s="90"/>
-      <c r="W10" s="88"/>
-      <c r="X10" s="75"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="54"/>
-      <c r="AA10" s="55"/>
-      <c r="AB10" s="65"/>
-      <c r="AC10" s="66"/>
-    </row>
-    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="W10" s="90"/>
+      <c r="X10" s="88"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="55"/>
+      <c r="AC10" s="65"/>
+      <c r="AD10" s="66"/>
+    </row>
+    <row r="11" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="91" t="s">
         <v>221</v>
       </c>
@@ -4833,1186 +4875,1247 @@
       <c r="C11" s="102">
         <v>44655</v>
       </c>
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E11" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="E11" s="128" t="s">
+      <c r="F11" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="F11" s="128" t="s">
+      <c r="G11" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="127" t="s">
+      <c r="H11" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="H11" s="128">
+      <c r="I11" s="128">
         <v>20</v>
       </c>
-      <c r="I11" s="128">
+      <c r="J11" s="128">
         <v>40000</v>
       </c>
-      <c r="J11" s="124">
-        <v>40000</v>
-      </c>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L11" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="L11" s="42"/>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="135"/>
-      <c r="P11" s="82"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="90"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="135"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="89"/>
       <c r="T11" s="90"/>
       <c r="U11" s="90"/>
       <c r="V11" s="90"/>
-      <c r="W11" s="88"/>
-      <c r="X11" s="75"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="54"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="66"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="91"/>
+      <c r="W11" s="90"/>
+      <c r="X11" s="88"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="46"/>
+      <c r="AA11" s="54"/>
+      <c r="AB11" s="55"/>
+      <c r="AC11" s="65"/>
+      <c r="AD11" s="66"/>
+    </row>
+    <row r="12" spans="1:30" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="91" t="s">
+        <v>260</v>
+      </c>
       <c r="B12" s="91"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="42"/>
+      <c r="C12" s="103">
+        <v>44655</v>
+      </c>
+      <c r="D12" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E12" s="120" t="s">
+        <v>261</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="128" t="s">
+        <v>217</v>
+      </c>
+      <c r="H12" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I12" s="128">
+        <v>20</v>
+      </c>
+      <c r="J12" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K12" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L12" s="41" t="s">
+        <v>226</v>
+      </c>
       <c r="M12" s="42"/>
       <c r="N12" s="42"/>
-      <c r="O12" s="135"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="109"/>
-      <c r="R12" s="89"/>
-      <c r="S12" s="91"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="135"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="109" t="s">
+        <v>263</v>
+      </c>
+      <c r="S12" s="89"/>
       <c r="T12" s="91"/>
       <c r="U12" s="91"/>
       <c r="V12" s="91"/>
-      <c r="W12" s="88"/>
-      <c r="X12" s="76"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="56"/>
-      <c r="AA12" s="57"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="68"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W12" s="91"/>
+      <c r="X12" s="88"/>
+      <c r="Y12" s="76"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="56"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="68"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="90"/>
       <c r="B13" s="91"/>
       <c r="C13" s="103"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="128"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="120"/>
       <c r="F13" s="128"/>
       <c r="G13" s="128"/>
       <c r="H13" s="128"/>
       <c r="I13" s="128"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
-      <c r="O13" s="135"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="109"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="91"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="135"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="89"/>
       <c r="T13" s="91"/>
       <c r="U13" s="91"/>
       <c r="V13" s="91"/>
-      <c r="W13" s="92"/>
-      <c r="X13" s="76"/>
-      <c r="Y13" s="47"/>
-      <c r="Z13" s="56"/>
-      <c r="AA13" s="57"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="68"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W13" s="91"/>
+      <c r="X13" s="92"/>
+      <c r="Y13" s="76"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="56"/>
+      <c r="AB13" s="57"/>
+      <c r="AC13" s="67"/>
+      <c r="AD13" s="68"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="90"/>
       <c r="B14" s="91"/>
       <c r="C14" s="103"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="128"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="120"/>
       <c r="F14" s="128"/>
       <c r="G14" s="128"/>
       <c r="H14" s="128"/>
       <c r="I14" s="128"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="42"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="124"/>
       <c r="L14" s="42"/>
       <c r="M14" s="42"/>
       <c r="N14" s="42"/>
-      <c r="O14" s="135"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="109"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="91"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="135"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="109"/>
+      <c r="S14" s="89"/>
       <c r="T14" s="91"/>
       <c r="U14" s="91"/>
       <c r="V14" s="91"/>
-      <c r="W14" s="92"/>
-      <c r="X14" s="76"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W14" s="91"/>
+      <c r="X14" s="92"/>
+      <c r="Y14" s="76"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="56"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="68"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="90"/>
       <c r="B15" s="91"/>
       <c r="C15" s="103"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="128"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="120"/>
       <c r="F15" s="128"/>
       <c r="G15" s="128"/>
       <c r="H15" s="128"/>
       <c r="I15" s="128"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="42"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="124"/>
       <c r="L15" s="42"/>
       <c r="M15" s="42"/>
       <c r="N15" s="42"/>
-      <c r="O15" s="135"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="109"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="91"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="135"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="109"/>
+      <c r="S15" s="89"/>
       <c r="T15" s="91"/>
       <c r="U15" s="91"/>
       <c r="V15" s="91"/>
-      <c r="W15" s="92"/>
-      <c r="X15" s="77"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="58"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="69"/>
-      <c r="AC15" s="70"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W15" s="91"/>
+      <c r="X15" s="92"/>
+      <c r="Y15" s="77"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="70"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="90"/>
       <c r="B16" s="91"/>
       <c r="C16" s="103"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="128"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="120"/>
       <c r="F16" s="128"/>
       <c r="G16" s="128"/>
       <c r="H16" s="128"/>
       <c r="I16" s="128"/>
-      <c r="J16" s="124"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="41"/>
       <c r="M16" s="42"/>
       <c r="N16" s="42"/>
-      <c r="O16" s="135"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="109"/>
-      <c r="R16" s="89"/>
-      <c r="S16" s="91"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="135"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="109"/>
+      <c r="S16" s="89"/>
       <c r="T16" s="91"/>
       <c r="U16" s="91"/>
       <c r="V16" s="91"/>
-      <c r="W16" s="92"/>
-      <c r="X16" s="76"/>
-      <c r="Y16" s="47"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="57"/>
-      <c r="AB16" s="67"/>
-      <c r="AC16" s="68"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W16" s="91"/>
+      <c r="X16" s="92"/>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="56"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="67"/>
+      <c r="AD16" s="68"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="90"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="128"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="120"/>
       <c r="F17" s="128"/>
       <c r="G17" s="128"/>
       <c r="H17" s="128"/>
       <c r="I17" s="128"/>
-      <c r="J17" s="124"/>
-      <c r="K17" s="42"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="124"/>
       <c r="L17" s="42"/>
       <c r="M17" s="42"/>
       <c r="N17" s="42"/>
-      <c r="O17" s="135"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="109"/>
-      <c r="R17" s="89"/>
-      <c r="S17" s="91"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="135"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="109"/>
+      <c r="S17" s="89"/>
       <c r="T17" s="91"/>
       <c r="U17" s="91"/>
       <c r="V17" s="91"/>
-      <c r="W17" s="92"/>
-      <c r="X17" s="77"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="58"/>
-      <c r="AA17" s="59"/>
-      <c r="AB17" s="69"/>
-      <c r="AC17" s="70"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W17" s="91"/>
+      <c r="X17" s="92"/>
+      <c r="Y17" s="77"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="69"/>
+      <c r="AD17" s="70"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="128"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="120"/>
       <c r="F18" s="128"/>
       <c r="G18" s="128"/>
       <c r="H18" s="128"/>
       <c r="I18" s="128"/>
-      <c r="J18" s="124"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="42"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="83"/>
       <c r="M18" s="42"/>
       <c r="N18" s="42"/>
-      <c r="O18" s="135"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="109"/>
-      <c r="R18" s="89"/>
-      <c r="S18" s="91"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="135"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="109"/>
+      <c r="S18" s="89"/>
       <c r="T18" s="91"/>
       <c r="U18" s="91"/>
       <c r="V18" s="91"/>
-      <c r="W18" s="92"/>
-      <c r="X18" s="77"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="70"/>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W18" s="91"/>
+      <c r="X18" s="92"/>
+      <c r="Y18" s="77"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="59"/>
+      <c r="AC18" s="69"/>
+      <c r="AD18" s="70"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="128"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="120"/>
       <c r="F19" s="128"/>
       <c r="G19" s="128"/>
       <c r="H19" s="128"/>
       <c r="I19" s="128"/>
-      <c r="J19" s="124"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="42"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="83"/>
       <c r="M19" s="42"/>
       <c r="N19" s="42"/>
-      <c r="O19" s="135"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="109"/>
-      <c r="R19" s="89"/>
-      <c r="S19" s="91"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="135"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="89"/>
       <c r="T19" s="91"/>
       <c r="U19" s="91"/>
       <c r="V19" s="91"/>
-      <c r="W19" s="92"/>
-      <c r="X19" s="77"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="58"/>
-      <c r="AA19" s="59"/>
-      <c r="AB19" s="69"/>
-      <c r="AC19" s="70"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W19" s="91"/>
+      <c r="X19" s="92"/>
+      <c r="Y19" s="77"/>
+      <c r="Z19" s="48"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="59"/>
+      <c r="AC19" s="69"/>
+      <c r="AD19" s="70"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="128"/>
+      <c r="D20" s="144"/>
+      <c r="E20" s="120"/>
       <c r="F20" s="128"/>
       <c r="G20" s="128"/>
       <c r="H20" s="128"/>
       <c r="I20" s="128"/>
-      <c r="J20" s="124"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="42"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="124"/>
+      <c r="L20" s="83"/>
       <c r="M20" s="42"/>
       <c r="N20" s="42"/>
-      <c r="O20" s="135"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="109"/>
-      <c r="R20" s="89"/>
-      <c r="S20" s="91"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="109"/>
+      <c r="S20" s="89"/>
       <c r="T20" s="91"/>
       <c r="U20" s="91"/>
       <c r="V20" s="91"/>
-      <c r="W20" s="92"/>
-      <c r="X20" s="77"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="58"/>
-      <c r="AA20" s="59"/>
-      <c r="AB20" s="69"/>
-      <c r="AC20" s="70"/>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W20" s="91"/>
+      <c r="X20" s="92"/>
+      <c r="Y20" s="77"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="59"/>
+      <c r="AC20" s="69"/>
+      <c r="AD20" s="70"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="128"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="120"/>
       <c r="F21" s="128"/>
       <c r="G21" s="128"/>
       <c r="H21" s="128"/>
       <c r="I21" s="128"/>
-      <c r="J21" s="124"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="42"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="124"/>
+      <c r="L21" s="83"/>
       <c r="M21" s="42"/>
       <c r="N21" s="42"/>
-      <c r="O21" s="135"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="89"/>
-      <c r="S21" s="91"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="135"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="89"/>
       <c r="T21" s="91"/>
       <c r="U21" s="91"/>
       <c r="V21" s="91"/>
-      <c r="W21" s="92"/>
-      <c r="X21" s="77"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="58"/>
-      <c r="AA21" s="59"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="70"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W21" s="91"/>
+      <c r="X21" s="92"/>
+      <c r="Y21" s="77"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="59"/>
+      <c r="AC21" s="69"/>
+      <c r="AD21" s="70"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="128"/>
+      <c r="D22" s="144"/>
+      <c r="E22" s="120"/>
       <c r="F22" s="128"/>
       <c r="G22" s="128"/>
       <c r="H22" s="128"/>
       <c r="I22" s="128"/>
-      <c r="J22" s="124"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="42"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="124"/>
+      <c r="L22" s="83"/>
       <c r="M22" s="42"/>
       <c r="N22" s="42"/>
-      <c r="O22" s="135"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="109"/>
-      <c r="R22" s="89"/>
-      <c r="S22" s="91"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="135"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="89"/>
       <c r="T22" s="91"/>
       <c r="U22" s="91"/>
       <c r="V22" s="91"/>
-      <c r="W22" s="92"/>
-      <c r="X22" s="77"/>
-      <c r="Y22" s="48"/>
-      <c r="Z22" s="58"/>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="69"/>
-      <c r="AC22" s="70"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W22" s="91"/>
+      <c r="X22" s="92"/>
+      <c r="Y22" s="77"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="69"/>
+      <c r="AD22" s="70"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="128"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="120"/>
       <c r="F23" s="128"/>
       <c r="G23" s="128"/>
       <c r="H23" s="128"/>
       <c r="I23" s="128"/>
-      <c r="J23" s="124"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="42"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="124"/>
+      <c r="L23" s="83"/>
       <c r="M23" s="42"/>
       <c r="N23" s="42"/>
-      <c r="O23" s="135"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="89"/>
-      <c r="S23" s="91"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="135"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="109"/>
+      <c r="S23" s="89"/>
       <c r="T23" s="91"/>
       <c r="U23" s="91"/>
       <c r="V23" s="91"/>
-      <c r="W23" s="92"/>
-      <c r="X23" s="77"/>
-      <c r="Y23" s="48"/>
-      <c r="Z23" s="58"/>
-      <c r="AA23" s="59"/>
-      <c r="AB23" s="69"/>
-      <c r="AC23" s="70"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W23" s="91"/>
+      <c r="X23" s="92"/>
+      <c r="Y23" s="77"/>
+      <c r="Z23" s="48"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="59"/>
+      <c r="AC23" s="69"/>
+      <c r="AD23" s="70"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="128"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="120"/>
       <c r="F24" s="128"/>
       <c r="G24" s="128"/>
       <c r="H24" s="128"/>
       <c r="I24" s="128"/>
-      <c r="J24" s="124"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="42"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="124"/>
+      <c r="L24" s="83"/>
       <c r="M24" s="42"/>
       <c r="N24" s="42"/>
-      <c r="O24" s="135"/>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="109"/>
-      <c r="R24" s="89"/>
-      <c r="S24" s="91"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="135"/>
+      <c r="Q24" s="82"/>
+      <c r="R24" s="109"/>
+      <c r="S24" s="89"/>
       <c r="T24" s="91"/>
       <c r="U24" s="91"/>
       <c r="V24" s="91"/>
-      <c r="W24" s="92"/>
-      <c r="X24" s="77"/>
-      <c r="Y24" s="48"/>
-      <c r="Z24" s="58"/>
-      <c r="AA24" s="59"/>
-      <c r="AB24" s="69"/>
-      <c r="AC24" s="70"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W24" s="91"/>
+      <c r="X24" s="92"/>
+      <c r="Y24" s="77"/>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="59"/>
+      <c r="AC24" s="69"/>
+      <c r="AD24" s="70"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="128"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="120"/>
       <c r="F25" s="128"/>
       <c r="G25" s="128"/>
       <c r="H25" s="128"/>
       <c r="I25" s="128"/>
-      <c r="J25" s="124"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="42"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="124"/>
+      <c r="L25" s="83"/>
       <c r="M25" s="42"/>
       <c r="N25" s="42"/>
-      <c r="O25" s="135"/>
-      <c r="P25" s="82"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="89"/>
-      <c r="S25" s="91"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="135"/>
+      <c r="Q25" s="82"/>
+      <c r="R25" s="109"/>
+      <c r="S25" s="89"/>
       <c r="T25" s="91"/>
       <c r="U25" s="91"/>
       <c r="V25" s="91"/>
-      <c r="W25" s="92"/>
-      <c r="X25" s="77"/>
-      <c r="Y25" s="48"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="59"/>
-      <c r="AB25" s="69"/>
-      <c r="AC25" s="70"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W25" s="91"/>
+      <c r="X25" s="92"/>
+      <c r="Y25" s="77"/>
+      <c r="Z25" s="48"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="69"/>
+      <c r="AD25" s="70"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="128"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="120"/>
       <c r="F26" s="128"/>
       <c r="G26" s="128"/>
       <c r="H26" s="128"/>
       <c r="I26" s="128"/>
-      <c r="J26" s="124"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="42"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="83"/>
       <c r="M26" s="42"/>
       <c r="N26" s="42"/>
-      <c r="O26" s="135"/>
-      <c r="P26" s="82"/>
-      <c r="Q26" s="109"/>
-      <c r="R26" s="89"/>
-      <c r="S26" s="91"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="135"/>
+      <c r="Q26" s="82"/>
+      <c r="R26" s="109"/>
+      <c r="S26" s="89"/>
       <c r="T26" s="91"/>
       <c r="U26" s="91"/>
       <c r="V26" s="91"/>
-      <c r="W26" s="92"/>
-      <c r="X26" s="77"/>
-      <c r="Y26" s="48"/>
-      <c r="Z26" s="58"/>
-      <c r="AA26" s="59"/>
-      <c r="AB26" s="69"/>
-      <c r="AC26" s="70"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W26" s="91"/>
+      <c r="X26" s="92"/>
+      <c r="Y26" s="77"/>
+      <c r="Z26" s="48"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="59"/>
+      <c r="AC26" s="69"/>
+      <c r="AD26" s="70"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="128"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="120"/>
       <c r="F27" s="128"/>
       <c r="G27" s="128"/>
       <c r="H27" s="128"/>
       <c r="I27" s="128"/>
-      <c r="J27" s="124"/>
-      <c r="K27" s="83"/>
-      <c r="L27" s="42"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="124"/>
+      <c r="L27" s="83"/>
       <c r="M27" s="42"/>
       <c r="N27" s="42"/>
-      <c r="O27" s="135"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="109"/>
-      <c r="R27" s="89"/>
-      <c r="S27" s="91"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="135"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="109"/>
+      <c r="S27" s="89"/>
       <c r="T27" s="91"/>
       <c r="U27" s="91"/>
       <c r="V27" s="91"/>
-      <c r="W27" s="92"/>
-      <c r="X27" s="77"/>
-      <c r="Y27" s="48"/>
-      <c r="Z27" s="58"/>
-      <c r="AA27" s="59"/>
-      <c r="AB27" s="69"/>
-      <c r="AC27" s="70"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W27" s="91"/>
+      <c r="X27" s="92"/>
+      <c r="Y27" s="77"/>
+      <c r="Z27" s="48"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="59"/>
+      <c r="AC27" s="69"/>
+      <c r="AD27" s="70"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="128"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="120"/>
       <c r="F28" s="128"/>
       <c r="G28" s="128"/>
       <c r="H28" s="128"/>
       <c r="I28" s="128"/>
-      <c r="J28" s="124"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="42"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="83"/>
       <c r="M28" s="42"/>
       <c r="N28" s="42"/>
-      <c r="O28" s="135"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="109"/>
-      <c r="R28" s="89"/>
-      <c r="S28" s="91"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="135"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="109"/>
+      <c r="S28" s="89"/>
       <c r="T28" s="91"/>
       <c r="U28" s="91"/>
       <c r="V28" s="91"/>
-      <c r="W28" s="92"/>
-      <c r="X28" s="77"/>
-      <c r="Y28" s="48"/>
-      <c r="Z28" s="58"/>
-      <c r="AA28" s="59"/>
-      <c r="AB28" s="69"/>
-      <c r="AC28" s="70"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W28" s="91"/>
+      <c r="X28" s="92"/>
+      <c r="Y28" s="77"/>
+      <c r="Z28" s="48"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="59"/>
+      <c r="AC28" s="69"/>
+      <c r="AD28" s="70"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="128"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="120"/>
       <c r="F29" s="128"/>
       <c r="G29" s="128"/>
       <c r="H29" s="128"/>
       <c r="I29" s="128"/>
-      <c r="J29" s="124"/>
-      <c r="K29" s="83"/>
-      <c r="L29" s="42"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="124"/>
+      <c r="L29" s="83"/>
       <c r="M29" s="42"/>
       <c r="N29" s="42"/>
-      <c r="O29" s="135"/>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="109"/>
-      <c r="R29" s="89"/>
-      <c r="S29" s="91"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="135"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="109"/>
+      <c r="S29" s="89"/>
       <c r="T29" s="91"/>
       <c r="U29" s="91"/>
       <c r="V29" s="91"/>
-      <c r="W29" s="92"/>
-      <c r="X29" s="77"/>
-      <c r="Y29" s="48"/>
-      <c r="Z29" s="58"/>
-      <c r="AA29" s="59"/>
-      <c r="AB29" s="69"/>
-      <c r="AC29" s="70"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W29" s="91"/>
+      <c r="X29" s="92"/>
+      <c r="Y29" s="77"/>
+      <c r="Z29" s="48"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="59"/>
+      <c r="AC29" s="69"/>
+      <c r="AD29" s="70"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="128"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="120"/>
       <c r="F30" s="128"/>
       <c r="G30" s="128"/>
       <c r="H30" s="128"/>
       <c r="I30" s="128"/>
-      <c r="J30" s="124"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="42"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="124"/>
+      <c r="L30" s="83"/>
       <c r="M30" s="42"/>
       <c r="N30" s="42"/>
-      <c r="O30" s="135"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="109"/>
-      <c r="R30" s="89"/>
-      <c r="S30" s="91"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="135"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="109"/>
+      <c r="S30" s="89"/>
       <c r="T30" s="91"/>
       <c r="U30" s="91"/>
       <c r="V30" s="91"/>
-      <c r="W30" s="92"/>
-      <c r="X30" s="77"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="58"/>
-      <c r="AA30" s="59"/>
-      <c r="AB30" s="69"/>
-      <c r="AC30" s="70"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W30" s="91"/>
+      <c r="X30" s="92"/>
+      <c r="Y30" s="77"/>
+      <c r="Z30" s="48"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="59"/>
+      <c r="AC30" s="69"/>
+      <c r="AD30" s="70"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
-      <c r="D31" s="120"/>
-      <c r="E31" s="128"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="120"/>
       <c r="F31" s="128"/>
       <c r="G31" s="128"/>
       <c r="H31" s="128"/>
       <c r="I31" s="128"/>
-      <c r="J31" s="124"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="42"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="124"/>
+      <c r="L31" s="83"/>
       <c r="M31" s="42"/>
       <c r="N31" s="42"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="109"/>
-      <c r="R31" s="89"/>
-      <c r="S31" s="91"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="135"/>
+      <c r="Q31" s="82"/>
+      <c r="R31" s="109"/>
+      <c r="S31" s="89"/>
       <c r="T31" s="91"/>
       <c r="U31" s="91"/>
       <c r="V31" s="91"/>
-      <c r="W31" s="92"/>
-      <c r="X31" s="77"/>
-      <c r="Y31" s="48"/>
-      <c r="Z31" s="58"/>
-      <c r="AA31" s="59"/>
-      <c r="AB31" s="69"/>
-      <c r="AC31" s="70"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W31" s="91"/>
+      <c r="X31" s="92"/>
+      <c r="Y31" s="77"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="58"/>
+      <c r="AB31" s="59"/>
+      <c r="AC31" s="69"/>
+      <c r="AD31" s="70"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="128"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="120"/>
       <c r="F32" s="128"/>
       <c r="G32" s="128"/>
       <c r="H32" s="128"/>
       <c r="I32" s="128"/>
-      <c r="J32" s="124"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="42"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="124"/>
+      <c r="L32" s="83"/>
       <c r="M32" s="42"/>
       <c r="N32" s="42"/>
-      <c r="O32" s="135"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="109"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="91"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="135"/>
+      <c r="Q32" s="82"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="89"/>
       <c r="T32" s="91"/>
       <c r="U32" s="91"/>
       <c r="V32" s="91"/>
-      <c r="W32" s="92"/>
-      <c r="X32" s="77"/>
-      <c r="Y32" s="48"/>
-      <c r="Z32" s="58"/>
-      <c r="AA32" s="59"/>
-      <c r="AB32" s="69"/>
-      <c r="AC32" s="70"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W32" s="91"/>
+      <c r="X32" s="92"/>
+      <c r="Y32" s="77"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="58"/>
+      <c r="AB32" s="59"/>
+      <c r="AC32" s="69"/>
+      <c r="AD32" s="70"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
-      <c r="D33" s="120"/>
-      <c r="E33" s="128"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="120"/>
       <c r="F33" s="128"/>
       <c r="G33" s="128"/>
       <c r="H33" s="128"/>
       <c r="I33" s="128"/>
-      <c r="J33" s="124"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="42"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="124"/>
+      <c r="L33" s="83"/>
       <c r="M33" s="42"/>
       <c r="N33" s="42"/>
-      <c r="O33" s="135"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="109"/>
-      <c r="R33" s="89"/>
-      <c r="S33" s="91"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="135"/>
+      <c r="Q33" s="82"/>
+      <c r="R33" s="109"/>
+      <c r="S33" s="89"/>
       <c r="T33" s="91"/>
       <c r="U33" s="91"/>
       <c r="V33" s="91"/>
-      <c r="W33" s="92"/>
-      <c r="X33" s="77"/>
-      <c r="Y33" s="48"/>
-      <c r="Z33" s="58"/>
-      <c r="AA33" s="59"/>
-      <c r="AB33" s="69"/>
-      <c r="AC33" s="70"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W33" s="91"/>
+      <c r="X33" s="92"/>
+      <c r="Y33" s="77"/>
+      <c r="Z33" s="48"/>
+      <c r="AA33" s="58"/>
+      <c r="AB33" s="59"/>
+      <c r="AC33" s="69"/>
+      <c r="AD33" s="70"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="128"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="120"/>
       <c r="F34" s="128"/>
       <c r="G34" s="128"/>
       <c r="H34" s="128"/>
       <c r="I34" s="128"/>
-      <c r="J34" s="124"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="42"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="124"/>
+      <c r="L34" s="83"/>
       <c r="M34" s="42"/>
       <c r="N34" s="42"/>
-      <c r="O34" s="135"/>
-      <c r="P34" s="82"/>
-      <c r="Q34" s="109"/>
-      <c r="R34" s="89"/>
-      <c r="S34" s="91"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="135"/>
+      <c r="Q34" s="82"/>
+      <c r="R34" s="109"/>
+      <c r="S34" s="89"/>
       <c r="T34" s="91"/>
       <c r="U34" s="91"/>
       <c r="V34" s="91"/>
-      <c r="W34" s="92"/>
-      <c r="X34" s="77"/>
-      <c r="Y34" s="48"/>
-      <c r="Z34" s="58"/>
-      <c r="AA34" s="59"/>
-      <c r="AB34" s="69"/>
-      <c r="AC34" s="70"/>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W34" s="91"/>
+      <c r="X34" s="92"/>
+      <c r="Y34" s="77"/>
+      <c r="Z34" s="48"/>
+      <c r="AA34" s="58"/>
+      <c r="AB34" s="59"/>
+      <c r="AC34" s="69"/>
+      <c r="AD34" s="70"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
-      <c r="D35" s="120"/>
-      <c r="E35" s="128"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="120"/>
       <c r="F35" s="128"/>
       <c r="G35" s="128"/>
       <c r="H35" s="128"/>
       <c r="I35" s="128"/>
-      <c r="J35" s="124"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="42"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="83"/>
       <c r="M35" s="42"/>
       <c r="N35" s="42"/>
-      <c r="O35" s="135"/>
-      <c r="P35" s="82"/>
-      <c r="Q35" s="109"/>
-      <c r="R35" s="89"/>
-      <c r="S35" s="91"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="135"/>
+      <c r="Q35" s="82"/>
+      <c r="R35" s="109"/>
+      <c r="S35" s="89"/>
       <c r="T35" s="91"/>
       <c r="U35" s="91"/>
       <c r="V35" s="91"/>
-      <c r="W35" s="92"/>
-      <c r="X35" s="77"/>
-      <c r="Y35" s="48"/>
-      <c r="Z35" s="58"/>
-      <c r="AA35" s="59"/>
-      <c r="AB35" s="69"/>
-      <c r="AC35" s="70"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W35" s="91"/>
+      <c r="X35" s="92"/>
+      <c r="Y35" s="77"/>
+      <c r="Z35" s="48"/>
+      <c r="AA35" s="58"/>
+      <c r="AB35" s="59"/>
+      <c r="AC35" s="69"/>
+      <c r="AD35" s="70"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="128"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="120"/>
       <c r="F36" s="128"/>
       <c r="G36" s="128"/>
       <c r="H36" s="128"/>
       <c r="I36" s="128"/>
-      <c r="J36" s="124"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="42"/>
+      <c r="J36" s="128"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="83"/>
       <c r="M36" s="42"/>
       <c r="N36" s="42"/>
-      <c r="O36" s="135"/>
-      <c r="P36" s="82"/>
-      <c r="Q36" s="109"/>
-      <c r="R36" s="89"/>
-      <c r="S36" s="91"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="135"/>
+      <c r="Q36" s="82"/>
+      <c r="R36" s="109"/>
+      <c r="S36" s="89"/>
       <c r="T36" s="91"/>
       <c r="U36" s="91"/>
       <c r="V36" s="91"/>
-      <c r="W36" s="92"/>
-      <c r="X36" s="77"/>
-      <c r="Y36" s="48"/>
-      <c r="Z36" s="58"/>
-      <c r="AA36" s="59"/>
-      <c r="AB36" s="69"/>
-      <c r="AC36" s="70"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W36" s="91"/>
+      <c r="X36" s="92"/>
+      <c r="Y36" s="77"/>
+      <c r="Z36" s="48"/>
+      <c r="AA36" s="58"/>
+      <c r="AB36" s="59"/>
+      <c r="AC36" s="69"/>
+      <c r="AD36" s="70"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
-      <c r="D37" s="120"/>
-      <c r="E37" s="128"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="120"/>
       <c r="F37" s="128"/>
       <c r="G37" s="128"/>
       <c r="H37" s="128"/>
       <c r="I37" s="128"/>
-      <c r="J37" s="124"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="42"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="124"/>
+      <c r="L37" s="83"/>
       <c r="M37" s="42"/>
       <c r="N37" s="42"/>
-      <c r="O37" s="135"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="109"/>
-      <c r="R37" s="89"/>
-      <c r="S37" s="91"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="135"/>
+      <c r="Q37" s="82"/>
+      <c r="R37" s="109"/>
+      <c r="S37" s="89"/>
       <c r="T37" s="91"/>
       <c r="U37" s="91"/>
       <c r="V37" s="91"/>
-      <c r="W37" s="92"/>
-      <c r="X37" s="77"/>
-      <c r="Y37" s="48"/>
-      <c r="Z37" s="58"/>
-      <c r="AA37" s="59"/>
-      <c r="AB37" s="69"/>
-      <c r="AC37" s="70"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W37" s="91"/>
+      <c r="X37" s="92"/>
+      <c r="Y37" s="77"/>
+      <c r="Z37" s="48"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="59"/>
+      <c r="AC37" s="69"/>
+      <c r="AD37" s="70"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="128"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="120"/>
       <c r="F38" s="128"/>
       <c r="G38" s="128"/>
       <c r="H38" s="128"/>
       <c r="I38" s="128"/>
-      <c r="J38" s="124"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="42"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="124"/>
+      <c r="L38" s="83"/>
       <c r="M38" s="42"/>
       <c r="N38" s="42"/>
-      <c r="O38" s="135"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="109"/>
-      <c r="R38" s="89"/>
-      <c r="S38" s="91"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="135"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="109"/>
+      <c r="S38" s="89"/>
       <c r="T38" s="91"/>
       <c r="U38" s="91"/>
       <c r="V38" s="91"/>
-      <c r="W38" s="92"/>
-      <c r="X38" s="77"/>
-      <c r="Y38" s="48"/>
-      <c r="Z38" s="58"/>
-      <c r="AA38" s="59"/>
-      <c r="AB38" s="69"/>
-      <c r="AC38" s="70"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W38" s="91"/>
+      <c r="X38" s="92"/>
+      <c r="Y38" s="77"/>
+      <c r="Z38" s="48"/>
+      <c r="AA38" s="58"/>
+      <c r="AB38" s="59"/>
+      <c r="AC38" s="69"/>
+      <c r="AD38" s="70"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A39" s="91"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
-      <c r="D39" s="120"/>
-      <c r="E39" s="128"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="120"/>
       <c r="F39" s="128"/>
       <c r="G39" s="128"/>
       <c r="H39" s="128"/>
       <c r="I39" s="128"/>
-      <c r="J39" s="124"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="42"/>
+      <c r="J39" s="128"/>
+      <c r="K39" s="124"/>
+      <c r="L39" s="83"/>
       <c r="M39" s="42"/>
       <c r="N39" s="42"/>
-      <c r="O39" s="135"/>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="109"/>
-      <c r="R39" s="89"/>
-      <c r="S39" s="91"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="135"/>
+      <c r="Q39" s="82"/>
+      <c r="R39" s="109"/>
+      <c r="S39" s="89"/>
       <c r="T39" s="91"/>
       <c r="U39" s="91"/>
       <c r="V39" s="91"/>
-      <c r="W39" s="92"/>
-      <c r="X39" s="77"/>
-      <c r="Y39" s="48"/>
-      <c r="Z39" s="58"/>
-      <c r="AA39" s="59"/>
-      <c r="AB39" s="69"/>
-      <c r="AC39" s="70"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W39" s="91"/>
+      <c r="X39" s="92"/>
+      <c r="Y39" s="77"/>
+      <c r="Z39" s="48"/>
+      <c r="AA39" s="58"/>
+      <c r="AB39" s="59"/>
+      <c r="AC39" s="69"/>
+      <c r="AD39" s="70"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="128"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="120"/>
       <c r="F40" s="128"/>
       <c r="G40" s="128"/>
       <c r="H40" s="128"/>
       <c r="I40" s="128"/>
-      <c r="J40" s="124"/>
-      <c r="K40" s="83"/>
-      <c r="L40" s="42"/>
+      <c r="J40" s="128"/>
+      <c r="K40" s="124"/>
+      <c r="L40" s="83"/>
       <c r="M40" s="42"/>
       <c r="N40" s="42"/>
-      <c r="O40" s="135"/>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="109"/>
-      <c r="R40" s="89"/>
-      <c r="S40" s="91"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="135"/>
+      <c r="Q40" s="82"/>
+      <c r="R40" s="109"/>
+      <c r="S40" s="89"/>
       <c r="T40" s="91"/>
       <c r="U40" s="91"/>
       <c r="V40" s="91"/>
-      <c r="W40" s="92"/>
-      <c r="X40" s="77"/>
-      <c r="Y40" s="48"/>
-      <c r="Z40" s="58"/>
-      <c r="AA40" s="59"/>
-      <c r="AB40" s="69"/>
-      <c r="AC40" s="70"/>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W40" s="91"/>
+      <c r="X40" s="92"/>
+      <c r="Y40" s="77"/>
+      <c r="Z40" s="48"/>
+      <c r="AA40" s="58"/>
+      <c r="AB40" s="59"/>
+      <c r="AC40" s="69"/>
+      <c r="AD40" s="70"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="128"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="120"/>
       <c r="F41" s="128"/>
       <c r="G41" s="128"/>
       <c r="H41" s="128"/>
       <c r="I41" s="128"/>
-      <c r="J41" s="124"/>
-      <c r="K41" s="83"/>
-      <c r="L41" s="42"/>
+      <c r="J41" s="128"/>
+      <c r="K41" s="124"/>
+      <c r="L41" s="83"/>
       <c r="M41" s="42"/>
       <c r="N41" s="42"/>
-      <c r="O41" s="135"/>
-      <c r="P41" s="82"/>
-      <c r="Q41" s="109"/>
-      <c r="R41" s="89"/>
-      <c r="S41" s="91"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="135"/>
+      <c r="Q41" s="82"/>
+      <c r="R41" s="109"/>
+      <c r="S41" s="89"/>
       <c r="T41" s="91"/>
       <c r="U41" s="91"/>
       <c r="V41" s="91"/>
-      <c r="W41" s="92"/>
-      <c r="X41" s="77"/>
-      <c r="Y41" s="48"/>
-      <c r="Z41" s="58"/>
-      <c r="AA41" s="59"/>
-      <c r="AB41" s="69"/>
-      <c r="AC41" s="70"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W41" s="91"/>
+      <c r="X41" s="92"/>
+      <c r="Y41" s="77"/>
+      <c r="Z41" s="48"/>
+      <c r="AA41" s="58"/>
+      <c r="AB41" s="59"/>
+      <c r="AC41" s="69"/>
+      <c r="AD41" s="70"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="128"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="120"/>
       <c r="F42" s="128"/>
       <c r="G42" s="128"/>
       <c r="H42" s="128"/>
       <c r="I42" s="128"/>
-      <c r="J42" s="124"/>
-      <c r="K42" s="83"/>
-      <c r="L42" s="42"/>
+      <c r="J42" s="128"/>
+      <c r="K42" s="124"/>
+      <c r="L42" s="83"/>
       <c r="M42" s="42"/>
       <c r="N42" s="42"/>
-      <c r="O42" s="135"/>
-      <c r="P42" s="82"/>
-      <c r="Q42" s="109"/>
-      <c r="R42" s="89"/>
-      <c r="S42" s="91"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="135"/>
+      <c r="Q42" s="82"/>
+      <c r="R42" s="109"/>
+      <c r="S42" s="89"/>
       <c r="T42" s="91"/>
       <c r="U42" s="91"/>
       <c r="V42" s="91"/>
-      <c r="W42" s="92"/>
-      <c r="X42" s="77"/>
-      <c r="Y42" s="48"/>
-      <c r="Z42" s="58"/>
-      <c r="AA42" s="59"/>
-      <c r="AB42" s="69"/>
-      <c r="AC42" s="70"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W42" s="91"/>
+      <c r="X42" s="92"/>
+      <c r="Y42" s="77"/>
+      <c r="Z42" s="48"/>
+      <c r="AA42" s="58"/>
+      <c r="AB42" s="59"/>
+      <c r="AC42" s="69"/>
+      <c r="AD42" s="70"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="104"/>
       <c r="B43" s="91"/>
       <c r="C43" s="103"/>
-      <c r="D43" s="120"/>
-      <c r="E43" s="128"/>
+      <c r="D43" s="144"/>
+      <c r="E43" s="120"/>
       <c r="F43" s="128"/>
       <c r="G43" s="128"/>
       <c r="H43" s="128"/>
       <c r="I43" s="128"/>
-      <c r="J43" s="124"/>
-      <c r="K43" s="83"/>
-      <c r="L43" s="42"/>
+      <c r="J43" s="128"/>
+      <c r="K43" s="124"/>
+      <c r="L43" s="83"/>
       <c r="M43" s="42"/>
       <c r="N43" s="42"/>
-      <c r="O43" s="135"/>
-      <c r="P43" s="82"/>
-      <c r="Q43" s="109"/>
-      <c r="R43" s="89"/>
-      <c r="S43" s="91"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="135"/>
+      <c r="Q43" s="82"/>
+      <c r="R43" s="109"/>
+      <c r="S43" s="89"/>
       <c r="T43" s="91"/>
       <c r="U43" s="91"/>
       <c r="V43" s="91"/>
-      <c r="W43" s="92"/>
-      <c r="X43" s="77"/>
-      <c r="Y43" s="48"/>
-      <c r="Z43" s="58"/>
-      <c r="AA43" s="59"/>
-      <c r="AB43" s="69"/>
-      <c r="AC43" s="70"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="W43" s="91"/>
+      <c r="X43" s="92"/>
+      <c r="Y43" s="77"/>
+      <c r="Z43" s="48"/>
+      <c r="AA43" s="58"/>
+      <c r="AB43" s="59"/>
+      <c r="AC43" s="69"/>
+      <c r="AD43" s="70"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" s="104"/>
       <c r="B44" s="91"/>
       <c r="C44" s="103"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="128"/>
+      <c r="D44" s="144"/>
+      <c r="E44" s="120"/>
       <c r="F44" s="128"/>
       <c r="G44" s="128"/>
       <c r="H44" s="128"/>
       <c r="I44" s="128"/>
-      <c r="J44" s="124"/>
-      <c r="K44" s="83"/>
-      <c r="L44" s="42"/>
+      <c r="J44" s="128"/>
+      <c r="K44" s="124"/>
+      <c r="L44" s="83"/>
       <c r="M44" s="42"/>
       <c r="N44" s="42"/>
-      <c r="O44" s="135"/>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="109"/>
-      <c r="R44" s="89"/>
-      <c r="S44" s="91"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="135"/>
+      <c r="Q44" s="82"/>
+      <c r="R44" s="109"/>
+      <c r="S44" s="89"/>
       <c r="T44" s="91"/>
       <c r="U44" s="91"/>
       <c r="V44" s="91"/>
-      <c r="W44" s="92"/>
-      <c r="X44" s="77"/>
-      <c r="Y44" s="48"/>
-      <c r="Z44" s="58"/>
-      <c r="AA44" s="59"/>
-      <c r="AB44" s="69"/>
-      <c r="AC44" s="70"/>
-    </row>
-    <row r="45" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W44" s="91"/>
+      <c r="X44" s="92"/>
+      <c r="Y44" s="77"/>
+      <c r="Z44" s="48"/>
+      <c r="AA44" s="58"/>
+      <c r="AB44" s="59"/>
+      <c r="AC44" s="69"/>
+      <c r="AD44" s="70"/>
+    </row>
+    <row r="45" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="105"/>
       <c r="B45" s="94"/>
       <c r="C45" s="106"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="129"/>
+      <c r="D45" s="145"/>
+      <c r="E45" s="121"/>
       <c r="F45" s="129"/>
       <c r="G45" s="129"/>
       <c r="H45" s="129"/>
       <c r="I45" s="129"/>
-      <c r="J45" s="125"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="130"/>
+      <c r="J45" s="129"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="43"/>
       <c r="M45" s="130"/>
       <c r="N45" s="130"/>
-      <c r="O45" s="136"/>
-      <c r="P45" s="138"/>
-      <c r="Q45" s="110"/>
-      <c r="R45" s="93"/>
-      <c r="S45" s="94"/>
+      <c r="O45" s="130"/>
+      <c r="P45" s="136"/>
+      <c r="Q45" s="138"/>
+      <c r="R45" s="110"/>
+      <c r="S45" s="93"/>
       <c r="T45" s="94"/>
       <c r="U45" s="94"/>
       <c r="V45" s="94"/>
-      <c r="W45" s="95"/>
-      <c r="X45" s="78"/>
-      <c r="Y45" s="49"/>
-      <c r="Z45" s="60"/>
-      <c r="AA45" s="61"/>
-      <c r="AB45" s="71"/>
-      <c r="AC45" s="72"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="L46" s="39"/>
+      <c r="W45" s="94"/>
+      <c r="X45" s="95"/>
+      <c r="Y45" s="78"/>
+      <c r="Z45" s="49"/>
+      <c r="AA45" s="60"/>
+      <c r="AB45" s="61"/>
+      <c r="AC45" s="71"/>
+      <c r="AD45" s="72"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="M46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="L47" s="39"/>
+      <c r="Q46" s="39"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="M47" s="39"/>
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
       <c r="P47" s="39"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="L48" s="39"/>
+      <c r="Q47" s="39"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="M48" s="39"/>
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
       <c r="P48" s="39"/>
-    </row>
-    <row r="49" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L49" s="39"/>
+      <c r="Q48" s="39"/>
+    </row>
+    <row r="49" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M49" s="39"/>
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
       <c r="P49" s="39"/>
-    </row>
-    <row r="50" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L50" s="39"/>
+      <c r="Q49" s="39"/>
+    </row>
+    <row r="50" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
       <c r="P50" s="39"/>
-    </row>
-    <row r="51" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L51" s="39"/>
+      <c r="Q50" s="39"/>
+    </row>
+    <row r="51" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
-    </row>
-    <row r="52" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L52" s="39"/>
+      <c r="Q51" s="39"/>
+    </row>
+    <row r="52" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M52" s="39"/>
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
       <c r="P52" s="39"/>
-    </row>
-    <row r="53" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L53" s="39"/>
+      <c r="Q52" s="39"/>
+    </row>
+    <row r="53" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M53" s="39"/>
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
       <c r="P53" s="39"/>
-    </row>
-    <row r="54" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L54" s="39"/>
+      <c r="Q53" s="39"/>
+    </row>
+    <row r="54" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M54" s="39"/>
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
       <c r="P54" s="39"/>
-    </row>
-    <row r="55" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L55" s="39"/>
+      <c r="Q54" s="39"/>
+    </row>
+    <row r="55" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M55" s="39"/>
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
       <c r="P55" s="39"/>
-    </row>
-    <row r="56" spans="12:16" x14ac:dyDescent="0.3">
-      <c r="L56" s="39"/>
+      <c r="Q55" s="39"/>
+    </row>
+    <row r="56" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M56" s="39"/>
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
       <c r="P56" s="39"/>
+      <c r="Q56" s="39"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K45" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L45" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K12" xr:uid="{A8837422-8676-43AE-8FBF-E37D051E89A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L12" xr:uid="{A8837422-8676-43AE-8FBF-E37D051E89A9}">
       <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update everything before the weekend
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38772911-5807-4627-9172-DD9C63B8FE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2FA09F-A392-42D9-89AC-E48A40F5BE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="Reboot_03.22.2022" sheetId="6" r:id="rId2"/>
-    <sheet name="Prior_sensitivity" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="Notes" sheetId="4" r:id="rId4"/>
-    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId5"/>
-    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Archived_sims" sheetId="7" r:id="rId3"/>
+    <sheet name="Prior_sensitivity" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="Notes" sheetId="4" r:id="rId5"/>
+    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId6"/>
+    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="294">
   <si>
     <t>Date run</t>
   </si>
@@ -937,9 +938,6 @@
     <t>When removing individual recaptures, we have to decide whether to keep the first instance of capture or the second. I want to see how the choice affects parameter estimates. Only running for 50 iterations, and only using a sample size of 250 per year (1000 total) bc the odds of many recaptures with smaller sample sizes are minimal.</t>
   </si>
   <si>
-    <t>Which recapture instance is retained doesn't seem to matter much. There is a slight improvement in precision for each parameter when using the last capture occasion. The bias is slightly improved for survival and lambda with the last capture occasion, but made slightly worse for male and female abundance.</t>
-  </si>
-  <si>
     <t>Date of analysis</t>
   </si>
   <si>
@@ -971,6 +969,89 @@
   </si>
   <si>
     <t>Copied results from HS.PO_new.compsDF to compare to the above three simulations using different numbers of comparisons. Changed the date run (was actually run on 4/4) and the purpose so I could easily analyze with the above three runs</t>
+  </si>
+  <si>
+    <t>HS.PO_downsample.R</t>
+  </si>
+  <si>
+    <t>HS.only_downsample.R</t>
+  </si>
+  <si>
+    <t>HS.PO_downsample</t>
+  </si>
+  <si>
+    <t>HS.only_downsample</t>
+  </si>
+  <si>
+    <t>Want to see if I can fix the bias at high sample sizes by downsampling the HS pairwise comparison dataframe.</t>
+  </si>
+  <si>
+    <t>Same as above, but wondering if the PO comparisons increase or decrease the bias and precision.</t>
+  </si>
+  <si>
+    <t>Archived sims</t>
+  </si>
+  <si>
+    <t>This tab is for simulations where I got the result, but think it's unlikely that the results/figures will play into the manuscript. The simulations listed here should match the results in the archived_sims folder in the Model.results folder on Drive</t>
+  </si>
+  <si>
+    <t>Results: general notes</t>
+  </si>
+  <si>
+    <t>Downsampling does appear to improve both bias and precision of abundance and survival estimates.</t>
+  </si>
+  <si>
+    <t>Adding PO probabilities improves the CV, but doesn't affect the bias much, likely because this population is juvenile heavy.</t>
+  </si>
+  <si>
+    <t>Results are very similar to above.</t>
+  </si>
+  <si>
+    <t>Didn't help</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Performs just </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">slightly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>better than the original HS|PO model.</t>
+    </r>
+  </si>
+  <si>
+    <t>Definitely improved survival estimates (shocking!).</t>
+  </si>
+  <si>
+    <t>Performs similarly to HS|PO model</t>
+  </si>
+  <si>
+    <t>Which instance of recapture doesn't matter much. Slight improvements in precision from using the later capture. Slight increase in bias for abundance estimates with later capture, but decrease in bias for survival and lambda.</t>
+  </si>
+  <si>
+    <t>More biased than keeping all comparisons, except at high sample sizes</t>
+  </si>
+  <si>
+    <t>Very similar to using all the comparisons</t>
+  </si>
+  <si>
+    <t>Again, doesn't change much from the HS|PO model, prob because there are not many POs relative to half-sibs.</t>
   </si>
 </sst>
 </file>
@@ -4247,11 +4328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0949DA-C0C5-4F9C-B1C9-632432E72B29}">
-  <dimension ref="A1:AD56"/>
+  <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4266,21 +4346,20 @@
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="31.5546875" customWidth="1"/>
-    <col min="17" max="17" width="51" customWidth="1"/>
-    <col min="18" max="18" width="49.6640625" style="39" customWidth="1"/>
-    <col min="19" max="22" width="19.5546875" customWidth="1"/>
-    <col min="23" max="24" width="25.33203125" customWidth="1"/>
-    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5546875" customWidth="1"/>
+    <col min="18" max="21" width="19.5546875" customWidth="1"/>
+    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -4291,7 +4370,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="142" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E1" s="118" t="s">
         <v>149</v>
@@ -4314,138 +4393,126 @@
       <c r="K1" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="L1" s="84" t="s">
+        <v>282</v>
+      </c>
+      <c r="M1" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="85" t="s">
+      <c r="N1" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="N1" s="85" t="s">
+      <c r="O1" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="P1" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="P1" s="131" t="s">
+      <c r="Q1" s="131" t="s">
         <v>160</v>
       </c>
-      <c r="Q1" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="R1" s="107" t="s">
-        <v>170</v>
-      </c>
-      <c r="S1" s="98" t="s">
+      <c r="R1" s="98" t="s">
         <v>24</v>
       </c>
+      <c r="S1" s="99" t="s">
+        <v>94</v>
+      </c>
       <c r="T1" s="99" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="U1" s="99" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="V1" s="99" t="s">
-        <v>95</v>
-      </c>
-      <c r="W1" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="86" t="s">
+      <c r="W1" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" s="73" t="s">
+      <c r="X1" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" s="44" t="s">
+      <c r="Y1" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="AA1" s="50" t="s">
+      <c r="Z1" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="AB1" s="51" t="s">
+      <c r="AA1" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="AC1" s="62" t="s">
+      <c r="AB1" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" s="79" t="s">
+      <c r="AC1" s="79" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
-        <v>213</v>
-      </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102">
-        <v>44648</v>
-      </c>
-      <c r="D2" s="143"/>
-      <c r="E2" s="119" t="s">
-        <v>212</v>
-      </c>
-      <c r="F2" s="127" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="127" t="s">
-        <v>217</v>
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="90" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="103">
+        <v>44656</v>
+      </c>
+      <c r="D2" s="144">
+        <v>44657</v>
+      </c>
+      <c r="E2" s="120" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="128" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" s="128" t="s">
+        <v>218</v>
       </c>
       <c r="H2" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="I2" s="127">
-        <v>15</v>
-      </c>
-      <c r="J2" s="127">
-        <v>30000</v>
-      </c>
-      <c r="K2" s="123">
+      <c r="I2" s="128">
+        <v>20</v>
+      </c>
+      <c r="J2" s="128">
         <v>40000</v>
       </c>
-      <c r="L2" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="M2" s="139" t="s">
-        <v>227</v>
-      </c>
-      <c r="N2" s="139" t="s">
-        <v>228</v>
-      </c>
-      <c r="O2" s="139" t="s">
-        <v>229</v>
-      </c>
-      <c r="P2" s="108" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q2" s="141"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="64"/>
-    </row>
-    <row r="3" spans="1:30" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="103" t="s">
-        <v>221</v>
+      <c r="K2" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L2" s="82"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="68"/>
+    </row>
+    <row r="3" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="90" t="s">
+        <v>274</v>
       </c>
       <c r="B3" s="91"/>
-      <c r="C3" s="102">
-        <v>44648</v>
-      </c>
-      <c r="D3" s="143"/>
+      <c r="C3" s="103">
+        <v>44658</v>
+      </c>
+      <c r="D3" s="144"/>
       <c r="E3" s="120" t="s">
-        <v>222</v>
+        <v>276</v>
       </c>
       <c r="F3" s="128" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="G3" s="128" t="s">
         <v>218</v>
@@ -4453,779 +4520,441 @@
       <c r="H3" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="I3" s="127">
-        <v>15</v>
-      </c>
-      <c r="J3" s="127">
-        <v>30000</v>
-      </c>
-      <c r="K3" s="123">
+      <c r="I3" s="128">
+        <v>20</v>
+      </c>
+      <c r="J3" s="128">
         <v>40000</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="M3" s="139" t="s">
-        <v>231</v>
-      </c>
-      <c r="N3" s="140" t="s">
-        <v>232</v>
-      </c>
-      <c r="O3" s="140" t="s">
-        <v>233</v>
-      </c>
-      <c r="P3" s="109" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="88"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="66"/>
-    </row>
-    <row r="4" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103" t="s">
-        <v>220</v>
-      </c>
+      <c r="K3" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L3" s="82" t="s">
+        <v>283</v>
+      </c>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="91"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="70"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" s="91"/>
       <c r="B4" s="91"/>
-      <c r="C4" s="102">
-        <v>44648</v>
-      </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="120" t="s">
-        <v>235</v>
-      </c>
-      <c r="F4" s="128" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H4" s="128" t="s">
-        <v>215</v>
-      </c>
-      <c r="I4" s="127">
-        <v>15</v>
-      </c>
-      <c r="J4" s="127">
-        <v>30000</v>
-      </c>
-      <c r="K4" s="123">
-        <v>40000</v>
-      </c>
-      <c r="L4" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="M4" s="140" t="s">
-        <v>227</v>
-      </c>
-      <c r="N4" s="140" t="s">
-        <v>241</v>
-      </c>
-      <c r="O4" s="140" t="s">
-        <v>239</v>
-      </c>
-      <c r="P4" s="135" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="65"/>
-      <c r="AD4" s="66"/>
-    </row>
-    <row r="5" spans="1:30" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
-        <v>219</v>
-      </c>
+      <c r="C4" s="103"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="135"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="69"/>
+      <c r="AC4" s="70"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="91"/>
       <c r="B5" s="91"/>
-      <c r="C5" s="102">
-        <v>44648</v>
-      </c>
-      <c r="D5" s="143"/>
-      <c r="E5" s="120" t="s">
-        <v>236</v>
-      </c>
-      <c r="F5" s="128" t="s">
-        <v>225</v>
-      </c>
-      <c r="G5" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H5" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I5" s="127">
-        <v>15</v>
-      </c>
-      <c r="J5" s="127">
-        <v>30000</v>
-      </c>
-      <c r="K5" s="123">
-        <v>40000</v>
-      </c>
-      <c r="L5" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>237</v>
-      </c>
-      <c r="N5" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="O5" s="42" t="s">
-        <v>239</v>
-      </c>
-      <c r="P5" s="135" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="109"/>
-      <c r="S5" s="89"/>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="88"/>
-      <c r="Y5" s="75"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="66"/>
-    </row>
-    <row r="6" spans="1:30" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="91" t="s">
-        <v>213</v>
-      </c>
+      <c r="C5" s="103"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="89"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="77"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="70"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="91"/>
       <c r="B6" s="91"/>
-      <c r="C6" s="102">
-        <v>44652</v>
-      </c>
-      <c r="D6" s="143">
-        <v>44655</v>
-      </c>
-      <c r="E6" s="120" t="s">
-        <v>244</v>
-      </c>
-      <c r="F6" s="128" t="s">
-        <v>245</v>
-      </c>
-      <c r="G6" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H6" s="127" t="s">
-        <v>253</v>
-      </c>
-      <c r="I6" s="128">
-        <v>20</v>
-      </c>
-      <c r="J6" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K6" s="124">
-        <v>40000</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="M6" s="42" t="s">
-        <v>249</v>
-      </c>
-      <c r="N6" s="42" t="s">
-        <v>250</v>
-      </c>
-      <c r="O6" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="P6" s="135" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="88"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="55"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="66"/>
-    </row>
-    <row r="7" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="91" t="s">
-        <v>242</v>
-      </c>
+      <c r="C6" s="103"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
+      <c r="U6" s="91"/>
+      <c r="V6" s="91"/>
+      <c r="W6" s="92"/>
+      <c r="X6" s="77"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="70"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" s="91"/>
       <c r="B7" s="91"/>
-      <c r="C7" s="103">
-        <v>44652</v>
-      </c>
-      <c r="D7" s="143">
-        <v>44655</v>
-      </c>
-      <c r="E7" s="120" t="s">
-        <v>243</v>
-      </c>
-      <c r="F7" s="128" t="s">
-        <v>246</v>
-      </c>
-      <c r="G7" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" s="127" t="s">
-        <v>253</v>
-      </c>
-      <c r="I7" s="128">
-        <v>20</v>
-      </c>
-      <c r="J7" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K7" s="124">
-        <v>40000</v>
-      </c>
-      <c r="L7" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="N7" s="42" t="s">
-        <v>257</v>
-      </c>
-      <c r="O7" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="P7" s="135" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="109"/>
-      <c r="S7" s="89"/>
-      <c r="T7" s="90"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="88"/>
-      <c r="Y7" s="75"/>
-      <c r="Z7" s="46"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="65"/>
-      <c r="AD7" s="66"/>
-    </row>
-    <row r="8" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="91" t="s">
-        <v>221</v>
-      </c>
+      <c r="C7" s="103"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="89"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="91"/>
+      <c r="U7" s="91"/>
+      <c r="V7" s="91"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="77"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="70"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" s="91"/>
       <c r="B8" s="91"/>
-      <c r="C8" s="102">
-        <v>44652</v>
-      </c>
-      <c r="D8" s="143">
-        <v>44655</v>
-      </c>
-      <c r="E8" s="120" t="s">
-        <v>247</v>
-      </c>
-      <c r="F8" s="128" t="s">
-        <v>248</v>
-      </c>
-      <c r="G8" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H8" s="127" t="s">
-        <v>253</v>
-      </c>
-      <c r="I8" s="128">
-        <v>20</v>
-      </c>
-      <c r="J8" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K8" s="124">
-        <v>40000</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="N8" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="O8" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="P8" s="135" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q8" s="82"/>
-      <c r="R8" s="109"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="90"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="90"/>
-      <c r="X8" s="88"/>
-      <c r="Y8" s="75"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="55"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="66"/>
-    </row>
-    <row r="9" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="91" t="s">
-        <v>213</v>
-      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="135"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="91"/>
+      <c r="T8" s="91"/>
+      <c r="U8" s="91"/>
+      <c r="V8" s="91"/>
+      <c r="W8" s="92"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="70"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" s="91"/>
       <c r="B9" s="91"/>
-      <c r="C9" s="102">
-        <v>44655</v>
-      </c>
-      <c r="D9" s="144">
-        <v>44656</v>
-      </c>
-      <c r="E9" s="120" t="s">
-        <v>244</v>
-      </c>
-      <c r="F9" s="128" t="s">
-        <v>254</v>
-      </c>
-      <c r="G9" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H9" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I9" s="128">
-        <v>20</v>
-      </c>
-      <c r="J9" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K9" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="M9" s="42"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="83"/>
       <c r="N9" s="42"/>
       <c r="O9" s="42"/>
-      <c r="P9" s="135"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="109"/>
-      <c r="S9" s="89"/>
-      <c r="T9" s="90"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="88"/>
-      <c r="Y9" s="75"/>
-      <c r="Z9" s="46"/>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="55"/>
-      <c r="AC9" s="65"/>
-      <c r="AD9" s="66"/>
-    </row>
-    <row r="10" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="91" t="s">
-        <v>242</v>
-      </c>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="135"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="91"/>
+      <c r="T9" s="91"/>
+      <c r="U9" s="91"/>
+      <c r="V9" s="91"/>
+      <c r="W9" s="92"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="70"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" s="91"/>
       <c r="B10" s="91"/>
-      <c r="C10" s="102">
-        <v>44655</v>
-      </c>
-      <c r="D10" s="144">
-        <v>44656</v>
-      </c>
-      <c r="E10" s="120" t="s">
-        <v>243</v>
-      </c>
-      <c r="F10" s="128" t="s">
-        <v>254</v>
-      </c>
-      <c r="G10" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H10" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I10" s="128">
-        <v>20</v>
-      </c>
-      <c r="J10" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K10" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="M10" s="42"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
       <c r="N10" s="42"/>
       <c r="O10" s="42"/>
-      <c r="P10" s="135"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="109"/>
-      <c r="S10" s="89"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="88"/>
-      <c r="Y10" s="75"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="54"/>
-      <c r="AB10" s="55"/>
-      <c r="AC10" s="65"/>
-      <c r="AD10" s="66"/>
-    </row>
-    <row r="11" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="91" t="s">
-        <v>221</v>
-      </c>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="135"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="92"/>
+      <c r="X10" s="77"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="58"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="70"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="91"/>
       <c r="B11" s="91"/>
-      <c r="C11" s="102">
-        <v>44655</v>
-      </c>
-      <c r="D11" s="144">
-        <v>44656</v>
-      </c>
-      <c r="E11" s="120" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="128" t="s">
-        <v>254</v>
-      </c>
-      <c r="G11" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H11" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I11" s="128">
-        <v>20</v>
-      </c>
-      <c r="J11" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K11" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="M11" s="42"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="83"/>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
-      <c r="P11" s="135"/>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="89"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="88"/>
-      <c r="Y11" s="75"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="55"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="66"/>
-    </row>
-    <row r="12" spans="1:30" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="91" t="s">
-        <v>260</v>
-      </c>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="135"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="91"/>
+      <c r="T11" s="91"/>
+      <c r="U11" s="91"/>
+      <c r="V11" s="91"/>
+      <c r="W11" s="92"/>
+      <c r="X11" s="77"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="70"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="91"/>
       <c r="B12" s="91"/>
-      <c r="C12" s="103">
-        <v>44655</v>
-      </c>
-      <c r="D12" s="144">
-        <v>44656</v>
-      </c>
-      <c r="E12" s="120" t="s">
-        <v>261</v>
-      </c>
-      <c r="F12" s="128" t="s">
-        <v>262</v>
-      </c>
-      <c r="G12" s="128" t="s">
-        <v>217</v>
-      </c>
-      <c r="H12" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I12" s="128">
-        <v>20</v>
-      </c>
-      <c r="J12" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K12" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="M12" s="42"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="83"/>
       <c r="N12" s="42"/>
       <c r="O12" s="42"/>
-      <c r="P12" s="135"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="109" t="s">
-        <v>263</v>
-      </c>
-      <c r="S12" s="89"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="135"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="91"/>
       <c r="T12" s="91"/>
       <c r="U12" s="91"/>
       <c r="V12" s="91"/>
-      <c r="W12" s="91"/>
-      <c r="X12" s="88"/>
-      <c r="Y12" s="76"/>
-      <c r="Z12" s="47"/>
-      <c r="AA12" s="56"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="68"/>
-    </row>
-    <row r="13" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="90" t="s">
-        <v>269</v>
-      </c>
+      <c r="W12" s="92"/>
+      <c r="X12" s="77"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="70"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="91"/>
       <c r="B13" s="91"/>
-      <c r="C13" s="103">
-        <v>44656</v>
-      </c>
-      <c r="D13" s="144">
-        <v>44657</v>
-      </c>
-      <c r="E13" s="120" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="128" t="s">
-        <v>268</v>
-      </c>
-      <c r="G13" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H13" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I13" s="128">
-        <v>20</v>
-      </c>
-      <c r="J13" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K13" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="83"/>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
-      <c r="P13" s="135"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="109"/>
-      <c r="S13" s="89"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="135"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="91"/>
       <c r="T13" s="91"/>
       <c r="U13" s="91"/>
       <c r="V13" s="91"/>
-      <c r="W13" s="91"/>
-      <c r="X13" s="92"/>
-      <c r="Y13" s="76"/>
-      <c r="Z13" s="47"/>
-      <c r="AA13" s="56"/>
-      <c r="AB13" s="57"/>
-      <c r="AC13" s="67"/>
-      <c r="AD13" s="68"/>
-    </row>
-    <row r="14" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="90" t="s">
-        <v>270</v>
-      </c>
+      <c r="W13" s="92"/>
+      <c r="X13" s="77"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="70"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="91"/>
       <c r="B14" s="91"/>
-      <c r="C14" s="103">
-        <v>44656</v>
-      </c>
-      <c r="D14" s="144">
-        <v>44657</v>
-      </c>
-      <c r="E14" s="120" t="s">
-        <v>266</v>
-      </c>
-      <c r="F14" s="128" t="s">
-        <v>268</v>
-      </c>
-      <c r="G14" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H14" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I14" s="128">
-        <v>20</v>
-      </c>
-      <c r="J14" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K14" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="83"/>
       <c r="N14" s="42"/>
       <c r="O14" s="42"/>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="82"/>
-      <c r="R14" s="109"/>
-      <c r="S14" s="89"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="135"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="91"/>
       <c r="T14" s="91"/>
       <c r="U14" s="91"/>
       <c r="V14" s="91"/>
-      <c r="W14" s="91"/>
-      <c r="X14" s="92"/>
-      <c r="Y14" s="76"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="67"/>
-      <c r="AD14" s="68"/>
-    </row>
-    <row r="15" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="90" t="s">
-        <v>271</v>
-      </c>
+      <c r="W14" s="92"/>
+      <c r="X14" s="77"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="70"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="91"/>
       <c r="B15" s="91"/>
-      <c r="C15" s="103">
-        <v>44656</v>
-      </c>
-      <c r="D15" s="144">
-        <v>44657</v>
-      </c>
-      <c r="E15" s="120" t="s">
-        <v>267</v>
-      </c>
-      <c r="F15" s="128" t="s">
-        <v>268</v>
-      </c>
-      <c r="G15" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H15" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I15" s="128">
-        <v>20</v>
-      </c>
-      <c r="J15" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K15" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="83"/>
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
-      <c r="P15" s="135"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="109"/>
-      <c r="S15" s="89"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="135"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="91"/>
       <c r="T15" s="91"/>
       <c r="U15" s="91"/>
       <c r="V15" s="91"/>
-      <c r="W15" s="91"/>
-      <c r="X15" s="92"/>
-      <c r="Y15" s="77"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="58"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="69"/>
-      <c r="AD15" s="70"/>
-    </row>
-    <row r="16" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
-        <v>272</v>
-      </c>
+      <c r="W15" s="92"/>
+      <c r="X15" s="77"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="59"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="70"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="91"/>
       <c r="B16" s="91"/>
-      <c r="C16" s="103">
-        <v>44656</v>
-      </c>
-      <c r="D16" s="144">
-        <v>44657</v>
-      </c>
-      <c r="E16" s="120" t="s">
-        <v>273</v>
-      </c>
-      <c r="F16" s="146" t="s">
-        <v>274</v>
-      </c>
-      <c r="G16" s="128" t="s">
-        <v>218</v>
-      </c>
-      <c r="H16" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="I16" s="128">
-        <v>20</v>
-      </c>
-      <c r="J16" s="128">
-        <v>40000</v>
-      </c>
-      <c r="K16" s="124">
-        <v>50000</v>
-      </c>
-      <c r="L16" s="41"/>
-      <c r="M16" s="42"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="82"/>
+      <c r="M16" s="83"/>
       <c r="N16" s="42"/>
       <c r="O16" s="42"/>
-      <c r="P16" s="135"/>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="109"/>
-      <c r="S16" s="89"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="135"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="91"/>
       <c r="T16" s="91"/>
       <c r="U16" s="91"/>
       <c r="V16" s="91"/>
-      <c r="W16" s="91"/>
-      <c r="X16" s="92"/>
-      <c r="Y16" s="76"/>
-      <c r="Z16" s="47"/>
-      <c r="AA16" s="56"/>
-      <c r="AB16" s="57"/>
-      <c r="AC16" s="67"/>
-      <c r="AD16" s="68"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="90"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="77"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
       <c r="D17" s="144"/>
@@ -5236,27 +4965,26 @@
       <c r="I17" s="128"/>
       <c r="J17" s="128"/>
       <c r="K17" s="124"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
-      <c r="P17" s="135"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="109"/>
-      <c r="S17" s="89"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="135"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="91"/>
       <c r="T17" s="91"/>
       <c r="U17" s="91"/>
       <c r="V17" s="91"/>
-      <c r="W17" s="91"/>
-      <c r="X17" s="92"/>
-      <c r="Y17" s="77"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="58"/>
-      <c r="AB17" s="59"/>
-      <c r="AC17" s="69"/>
-      <c r="AD17" s="70"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W17" s="92"/>
+      <c r="X17" s="77"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="70"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -5268,27 +4996,26 @@
       <c r="I18" s="128"/>
       <c r="J18" s="128"/>
       <c r="K18" s="124"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="42"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="83"/>
       <c r="N18" s="42"/>
       <c r="O18" s="42"/>
-      <c r="P18" s="135"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="109"/>
-      <c r="S18" s="89"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="135"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="91"/>
       <c r="T18" s="91"/>
       <c r="U18" s="91"/>
       <c r="V18" s="91"/>
-      <c r="W18" s="91"/>
-      <c r="X18" s="92"/>
-      <c r="Y18" s="77"/>
-      <c r="Z18" s="48"/>
-      <c r="AA18" s="58"/>
-      <c r="AB18" s="59"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="70"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W18" s="92"/>
+      <c r="X18" s="77"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="69"/>
+      <c r="AC18" s="70"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -5300,27 +5027,26 @@
       <c r="I19" s="128"/>
       <c r="J19" s="128"/>
       <c r="K19" s="124"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="42"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="83"/>
       <c r="N19" s="42"/>
       <c r="O19" s="42"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="109"/>
-      <c r="S19" s="89"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="135"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="91"/>
       <c r="T19" s="91"/>
       <c r="U19" s="91"/>
       <c r="V19" s="91"/>
-      <c r="W19" s="91"/>
-      <c r="X19" s="92"/>
-      <c r="Y19" s="77"/>
-      <c r="Z19" s="48"/>
-      <c r="AA19" s="58"/>
-      <c r="AB19" s="59"/>
-      <c r="AC19" s="69"/>
-      <c r="AD19" s="70"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W19" s="92"/>
+      <c r="X19" s="77"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="70"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -5332,27 +5058,26 @@
       <c r="I20" s="128"/>
       <c r="J20" s="128"/>
       <c r="K20" s="124"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="42"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="83"/>
       <c r="N20" s="42"/>
       <c r="O20" s="42"/>
-      <c r="P20" s="135"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="109"/>
-      <c r="S20" s="89"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="135"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="91"/>
       <c r="T20" s="91"/>
       <c r="U20" s="91"/>
       <c r="V20" s="91"/>
-      <c r="W20" s="91"/>
-      <c r="X20" s="92"/>
-      <c r="Y20" s="77"/>
-      <c r="Z20" s="48"/>
-      <c r="AA20" s="58"/>
-      <c r="AB20" s="59"/>
-      <c r="AC20" s="69"/>
-      <c r="AD20" s="70"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W20" s="92"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="70"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -5364,27 +5089,26 @@
       <c r="I21" s="128"/>
       <c r="J21" s="128"/>
       <c r="K21" s="124"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="42"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
       <c r="N21" s="42"/>
       <c r="O21" s="42"/>
-      <c r="P21" s="135"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="109"/>
-      <c r="S21" s="89"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="135"/>
+      <c r="R21" s="89"/>
+      <c r="S21" s="91"/>
       <c r="T21" s="91"/>
       <c r="U21" s="91"/>
       <c r="V21" s="91"/>
-      <c r="W21" s="91"/>
-      <c r="X21" s="92"/>
-      <c r="Y21" s="77"/>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="59"/>
-      <c r="AC21" s="69"/>
-      <c r="AD21" s="70"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W21" s="92"/>
+      <c r="X21" s="77"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="70"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -5396,27 +5120,26 @@
       <c r="I22" s="128"/>
       <c r="J22" s="128"/>
       <c r="K22" s="124"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="42"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="83"/>
       <c r="N22" s="42"/>
       <c r="O22" s="42"/>
-      <c r="P22" s="135"/>
-      <c r="Q22" s="82"/>
-      <c r="R22" s="109"/>
-      <c r="S22" s="89"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="135"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="91"/>
       <c r="T22" s="91"/>
       <c r="U22" s="91"/>
       <c r="V22" s="91"/>
-      <c r="W22" s="91"/>
-      <c r="X22" s="92"/>
-      <c r="Y22" s="77"/>
-      <c r="Z22" s="48"/>
-      <c r="AA22" s="58"/>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="69"/>
-      <c r="AD22" s="70"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W22" s="92"/>
+      <c r="X22" s="77"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="58"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="69"/>
+      <c r="AC22" s="70"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -5428,27 +5151,26 @@
       <c r="I23" s="128"/>
       <c r="J23" s="128"/>
       <c r="K23" s="124"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="42"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="83"/>
       <c r="N23" s="42"/>
       <c r="O23" s="42"/>
-      <c r="P23" s="135"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="89"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="135"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="91"/>
       <c r="T23" s="91"/>
       <c r="U23" s="91"/>
       <c r="V23" s="91"/>
-      <c r="W23" s="91"/>
-      <c r="X23" s="92"/>
-      <c r="Y23" s="77"/>
-      <c r="Z23" s="48"/>
-      <c r="AA23" s="58"/>
-      <c r="AB23" s="59"/>
-      <c r="AC23" s="69"/>
-      <c r="AD23" s="70"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W23" s="92"/>
+      <c r="X23" s="77"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="59"/>
+      <c r="AB23" s="69"/>
+      <c r="AC23" s="70"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -5460,27 +5182,1527 @@
       <c r="I24" s="128"/>
       <c r="J24" s="128"/>
       <c r="K24" s="124"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="42"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="83"/>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
-      <c r="P24" s="135"/>
-      <c r="Q24" s="82"/>
-      <c r="R24" s="109"/>
-      <c r="S24" s="89"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="135"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="91"/>
       <c r="T24" s="91"/>
       <c r="U24" s="91"/>
       <c r="V24" s="91"/>
-      <c r="W24" s="91"/>
-      <c r="X24" s="92"/>
-      <c r="Y24" s="77"/>
-      <c r="Z24" s="48"/>
-      <c r="AA24" s="58"/>
-      <c r="AB24" s="59"/>
-      <c r="AC24" s="69"/>
-      <c r="AD24" s="70"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W24" s="92"/>
+      <c r="X24" s="77"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="58"/>
+      <c r="AA24" s="59"/>
+      <c r="AB24" s="69"/>
+      <c r="AC24" s="70"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A25" s="104"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="124"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="135"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="91"/>
+      <c r="T25" s="91"/>
+      <c r="U25" s="91"/>
+      <c r="V25" s="91"/>
+      <c r="W25" s="92"/>
+      <c r="X25" s="77"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="69"/>
+      <c r="AC25" s="70"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A26" s="104"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="83"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="135"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="91"/>
+      <c r="T26" s="91"/>
+      <c r="U26" s="91"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="92"/>
+      <c r="X26" s="77"/>
+      <c r="Y26" s="48"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="59"/>
+      <c r="AB26" s="69"/>
+      <c r="AC26" s="70"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A27" s="104"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="124"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="135"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="92"/>
+      <c r="X27" s="77"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="59"/>
+      <c r="AB27" s="69"/>
+      <c r="AC27" s="70"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" s="104"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="120"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="83"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="135"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="91"/>
+      <c r="T28" s="91"/>
+      <c r="U28" s="91"/>
+      <c r="V28" s="91"/>
+      <c r="W28" s="92"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="59"/>
+      <c r="AB28" s="69"/>
+      <c r="AC28" s="70"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A29" s="104"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="124"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="83"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="135"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="91"/>
+      <c r="T29" s="91"/>
+      <c r="U29" s="91"/>
+      <c r="V29" s="91"/>
+      <c r="W29" s="92"/>
+      <c r="X29" s="77"/>
+      <c r="Y29" s="48"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="59"/>
+      <c r="AB29" s="69"/>
+      <c r="AC29" s="70"/>
+    </row>
+    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="105"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="129"/>
+      <c r="G30" s="129"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
+      <c r="J30" s="129"/>
+      <c r="K30" s="125"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="130"/>
+      <c r="O30" s="130"/>
+      <c r="P30" s="130"/>
+      <c r="Q30" s="136"/>
+      <c r="R30" s="93"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="95"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="49"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="61"/>
+      <c r="AB30" s="71"/>
+      <c r="AC30" s="72"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+    </row>
+    <row r="33" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+    </row>
+    <row r="34" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+    </row>
+    <row r="35" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+    </row>
+    <row r="36" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+    </row>
+    <row r="37" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+    </row>
+    <row r="38" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
+    </row>
+    <row r="39" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="39"/>
+      <c r="Q39" s="39"/>
+    </row>
+    <row r="40" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+      <c r="P40" s="39"/>
+      <c r="Q40" s="39"/>
+    </row>
+    <row r="41" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="39"/>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M30" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
+      <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B018C518-579D-41AF-A4D3-5ADE8EC7F546}">
+  <dimension ref="A1:AC54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="20.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5546875" customWidth="1"/>
+    <col min="7" max="7" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="51" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5546875" customWidth="1"/>
+    <col min="18" max="21" width="19.5546875" customWidth="1"/>
+    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="142" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" s="118" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="126" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="126" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="126" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="126" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="126" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="122" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" s="84" t="s">
+        <v>282</v>
+      </c>
+      <c r="M1" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="85" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q1" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" s="98" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" s="79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="100" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="101"/>
+      <c r="C2" s="102">
+        <v>44648</v>
+      </c>
+      <c r="D2" s="143"/>
+      <c r="E2" s="119" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="H2" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2" s="127">
+        <v>15</v>
+      </c>
+      <c r="J2" s="127">
+        <v>30000</v>
+      </c>
+      <c r="K2" s="123">
+        <v>40000</v>
+      </c>
+      <c r="L2" s="141" t="s">
+        <v>284</v>
+      </c>
+      <c r="M2" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="139" t="s">
+        <v>227</v>
+      </c>
+      <c r="O2" s="139" t="s">
+        <v>228</v>
+      </c>
+      <c r="P2" s="139" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="108" t="s">
+        <v>230</v>
+      </c>
+      <c r="R2" s="96"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="87"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="64"/>
+    </row>
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="103" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="91"/>
+      <c r="C3" s="102">
+        <v>44648</v>
+      </c>
+      <c r="D3" s="143"/>
+      <c r="E3" s="120" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="128" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H3" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I3" s="127">
+        <v>15</v>
+      </c>
+      <c r="J3" s="127">
+        <v>30000</v>
+      </c>
+      <c r="K3" s="123">
+        <v>40000</v>
+      </c>
+      <c r="L3" s="82" t="s">
+        <v>285</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="N3" s="139" t="s">
+        <v>231</v>
+      </c>
+      <c r="O3" s="140" t="s">
+        <v>232</v>
+      </c>
+      <c r="P3" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q3" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="R3" s="89"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="90"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="66"/>
+    </row>
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="91"/>
+      <c r="C4" s="102">
+        <v>44648</v>
+      </c>
+      <c r="D4" s="143"/>
+      <c r="E4" s="120" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="128" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="128" t="s">
+        <v>215</v>
+      </c>
+      <c r="I4" s="127">
+        <v>15</v>
+      </c>
+      <c r="J4" s="127">
+        <v>30000</v>
+      </c>
+      <c r="K4" s="123">
+        <v>40000</v>
+      </c>
+      <c r="L4" s="82" t="s">
+        <v>286</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="N4" s="140" t="s">
+        <v>227</v>
+      </c>
+      <c r="O4" s="140" t="s">
+        <v>241</v>
+      </c>
+      <c r="P4" s="140" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q4" s="135" t="s">
+        <v>240</v>
+      </c>
+      <c r="R4" s="89"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="66"/>
+    </row>
+    <row r="5" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="91" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="102">
+        <v>44648</v>
+      </c>
+      <c r="D5" s="143"/>
+      <c r="E5" s="120" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H5" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="127">
+        <v>15</v>
+      </c>
+      <c r="J5" s="127">
+        <v>30000</v>
+      </c>
+      <c r="K5" s="123">
+        <v>40000</v>
+      </c>
+      <c r="L5" s="82" t="s">
+        <v>286</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="O5" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="P5" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q5" s="135" t="s">
+        <v>240</v>
+      </c>
+      <c r="R5" s="89"/>
+      <c r="S5" s="90"/>
+      <c r="T5" s="90"/>
+      <c r="U5" s="90"/>
+      <c r="V5" s="90"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="66"/>
+    </row>
+    <row r="6" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="91" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="91"/>
+      <c r="C6" s="102">
+        <v>44652</v>
+      </c>
+      <c r="D6" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E6" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" s="128" t="s">
+        <v>245</v>
+      </c>
+      <c r="G6" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H6" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="I6" s="128">
+        <v>20</v>
+      </c>
+      <c r="J6" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K6" s="124">
+        <v>40000</v>
+      </c>
+      <c r="L6" s="82" t="s">
+        <v>287</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="N6" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="O6" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="P6" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q6" s="135" t="s">
+        <v>252</v>
+      </c>
+      <c r="R6" s="89"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="88"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="66"/>
+    </row>
+    <row r="7" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="91"/>
+      <c r="C7" s="103">
+        <v>44652</v>
+      </c>
+      <c r="D7" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E7" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" s="128" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7" s="128">
+        <v>20</v>
+      </c>
+      <c r="J7" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K7" s="124">
+        <v>40000</v>
+      </c>
+      <c r="L7" s="82" t="s">
+        <v>288</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="O7" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="P7" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q7" s="135" t="s">
+        <v>259</v>
+      </c>
+      <c r="R7" s="89"/>
+      <c r="S7" s="90"/>
+      <c r="T7" s="90"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="90"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="66"/>
+    </row>
+    <row r="8" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="91" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="91"/>
+      <c r="C8" s="102">
+        <v>44652</v>
+      </c>
+      <c r="D8" s="143">
+        <v>44655</v>
+      </c>
+      <c r="E8" s="120" t="s">
+        <v>247</v>
+      </c>
+      <c r="F8" s="128" t="s">
+        <v>248</v>
+      </c>
+      <c r="G8" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="128">
+        <v>20</v>
+      </c>
+      <c r="J8" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K8" s="124">
+        <v>40000</v>
+      </c>
+      <c r="L8" s="82" t="s">
+        <v>289</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="N8" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="O8" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="P8" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q8" s="135" t="s">
+        <v>258</v>
+      </c>
+      <c r="R8" s="89"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="88"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="66"/>
+    </row>
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="91" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="91"/>
+      <c r="C9" s="102">
+        <v>44655</v>
+      </c>
+      <c r="D9" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E9" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H9" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I9" s="128">
+        <v>20</v>
+      </c>
+      <c r="J9" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K9" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L9" s="82"/>
+      <c r="M9" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="135"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="88"/>
+      <c r="X9" s="75"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="65"/>
+      <c r="AC9" s="66"/>
+    </row>
+    <row r="10" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="91"/>
+      <c r="C10" s="102">
+        <v>44655</v>
+      </c>
+      <c r="D10" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E10" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="G10" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I10" s="128">
+        <v>20</v>
+      </c>
+      <c r="J10" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K10" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L10" s="82"/>
+      <c r="M10" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="135"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="88"/>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="65"/>
+      <c r="AC10" s="66"/>
+    </row>
+    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="91" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="91"/>
+      <c r="C11" s="102">
+        <v>44655</v>
+      </c>
+      <c r="D11" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E11" s="120" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="G11" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H11" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I11" s="128">
+        <v>20</v>
+      </c>
+      <c r="J11" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K11" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L11" s="82"/>
+      <c r="M11" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="135"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="90"/>
+      <c r="T11" s="90"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="88"/>
+      <c r="X11" s="75"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="55"/>
+      <c r="AB11" s="65"/>
+      <c r="AC11" s="66"/>
+    </row>
+    <row r="12" spans="1:29" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="91" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="91"/>
+      <c r="C12" s="103">
+        <v>44655</v>
+      </c>
+      <c r="D12" s="144">
+        <v>44656</v>
+      </c>
+      <c r="E12" s="120" t="s">
+        <v>261</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="128" t="s">
+        <v>217</v>
+      </c>
+      <c r="H12" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I12" s="128">
+        <v>20</v>
+      </c>
+      <c r="J12" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K12" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L12" s="82" t="s">
+        <v>290</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="135"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="91"/>
+      <c r="T12" s="91"/>
+      <c r="U12" s="91"/>
+      <c r="V12" s="91"/>
+      <c r="W12" s="88"/>
+      <c r="X12" s="76"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="68"/>
+    </row>
+    <row r="13" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="90" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="91"/>
+      <c r="C13" s="103">
+        <v>44656</v>
+      </c>
+      <c r="D13" s="144">
+        <v>44657</v>
+      </c>
+      <c r="E13" s="120" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13" s="128" t="s">
+        <v>267</v>
+      </c>
+      <c r="G13" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I13" s="128">
+        <v>20</v>
+      </c>
+      <c r="J13" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K13" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L13" s="82" t="s">
+        <v>291</v>
+      </c>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="135"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="91"/>
+      <c r="T13" s="91"/>
+      <c r="U13" s="91"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="92"/>
+      <c r="X13" s="76"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="57"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="68"/>
+    </row>
+    <row r="14" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="90" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" s="91"/>
+      <c r="C14" s="103">
+        <v>44656</v>
+      </c>
+      <c r="D14" s="144">
+        <v>44657</v>
+      </c>
+      <c r="E14" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" s="128" t="s">
+        <v>267</v>
+      </c>
+      <c r="G14" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I14" s="128">
+        <v>20</v>
+      </c>
+      <c r="J14" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K14" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L14" s="82" t="s">
+        <v>291</v>
+      </c>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="135"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="91"/>
+      <c r="V14" s="91"/>
+      <c r="W14" s="92"/>
+      <c r="X14" s="77"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="70"/>
+    </row>
+    <row r="15" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15" s="91"/>
+      <c r="C15" s="103">
+        <v>44656</v>
+      </c>
+      <c r="D15" s="144">
+        <v>44657</v>
+      </c>
+      <c r="E15" s="120" t="s">
+        <v>272</v>
+      </c>
+      <c r="F15" s="146" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I15" s="128">
+        <v>20</v>
+      </c>
+      <c r="J15" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K15" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L15" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="M15" s="41"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="135"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="76"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="57"/>
+      <c r="AB15" s="67"/>
+      <c r="AC15" s="68"/>
+    </row>
+    <row r="16" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="91" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="91"/>
+      <c r="C16" s="103">
+        <v>44658</v>
+      </c>
+      <c r="D16" s="144"/>
+      <c r="E16" s="120" t="s">
+        <v>277</v>
+      </c>
+      <c r="F16" s="128" t="s">
+        <v>279</v>
+      </c>
+      <c r="G16" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I16" s="128">
+        <v>20</v>
+      </c>
+      <c r="J16" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K16" s="124">
+        <v>50000</v>
+      </c>
+      <c r="L16" s="82" t="s">
+        <v>293</v>
+      </c>
+      <c r="M16" s="83"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="135"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="91"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="91"/>
+      <c r="V16" s="91"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="77"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="128"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="135"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="91"/>
+      <c r="T17" s="91"/>
+      <c r="U17" s="91"/>
+      <c r="V17" s="91"/>
+      <c r="W17" s="92"/>
+      <c r="X17" s="77"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="70"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="135"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="91"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="92"/>
+      <c r="X18" s="77"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="69"/>
+      <c r="AC18" s="70"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="135"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="91"/>
+      <c r="T19" s="91"/>
+      <c r="U19" s="91"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="92"/>
+      <c r="X19" s="77"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="70"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="144"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="124"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="135"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="91"/>
+      <c r="U20" s="91"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="70"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="124"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="135"/>
+      <c r="R21" s="89"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="91"/>
+      <c r="U21" s="91"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="77"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="70"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="144"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="124"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="135"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="91"/>
+      <c r="T22" s="91"/>
+      <c r="U22" s="91"/>
+      <c r="V22" s="91"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="77"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="58"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="69"/>
+      <c r="AC22" s="70"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="124"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="135"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="91"/>
+      <c r="T23" s="91"/>
+      <c r="U23" s="91"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="92"/>
+      <c r="X23" s="77"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="59"/>
+      <c r="AB23" s="69"/>
+      <c r="AC23" s="70"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="124"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="135"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="91"/>
+      <c r="T24" s="91"/>
+      <c r="U24" s="91"/>
+      <c r="V24" s="91"/>
+      <c r="W24" s="92"/>
+      <c r="X24" s="77"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="58"/>
+      <c r="AA24" s="59"/>
+      <c r="AB24" s="69"/>
+      <c r="AC24" s="70"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -5492,27 +6714,26 @@
       <c r="I25" s="128"/>
       <c r="J25" s="128"/>
       <c r="K25" s="124"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="42"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="83"/>
       <c r="N25" s="42"/>
       <c r="O25" s="42"/>
-      <c r="P25" s="135"/>
-      <c r="Q25" s="82"/>
-      <c r="R25" s="109"/>
-      <c r="S25" s="89"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="135"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="91"/>
       <c r="T25" s="91"/>
       <c r="U25" s="91"/>
       <c r="V25" s="91"/>
-      <c r="W25" s="91"/>
-      <c r="X25" s="92"/>
-      <c r="Y25" s="77"/>
-      <c r="Z25" s="48"/>
-      <c r="AA25" s="58"/>
-      <c r="AB25" s="59"/>
-      <c r="AC25" s="69"/>
-      <c r="AD25" s="70"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W25" s="92"/>
+      <c r="X25" s="77"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="69"/>
+      <c r="AC25" s="70"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -5524,27 +6745,26 @@
       <c r="I26" s="128"/>
       <c r="J26" s="128"/>
       <c r="K26" s="124"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="42"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="83"/>
       <c r="N26" s="42"/>
       <c r="O26" s="42"/>
-      <c r="P26" s="135"/>
-      <c r="Q26" s="82"/>
-      <c r="R26" s="109"/>
-      <c r="S26" s="89"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="135"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="91"/>
       <c r="T26" s="91"/>
       <c r="U26" s="91"/>
       <c r="V26" s="91"/>
-      <c r="W26" s="91"/>
-      <c r="X26" s="92"/>
-      <c r="Y26" s="77"/>
-      <c r="Z26" s="48"/>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="59"/>
-      <c r="AC26" s="69"/>
-      <c r="AD26" s="70"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W26" s="92"/>
+      <c r="X26" s="77"/>
+      <c r="Y26" s="48"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="59"/>
+      <c r="AB26" s="69"/>
+      <c r="AC26" s="70"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -5556,27 +6776,26 @@
       <c r="I27" s="128"/>
       <c r="J27" s="128"/>
       <c r="K27" s="124"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="42"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="83"/>
       <c r="N27" s="42"/>
       <c r="O27" s="42"/>
-      <c r="P27" s="135"/>
-      <c r="Q27" s="82"/>
-      <c r="R27" s="109"/>
-      <c r="S27" s="89"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="135"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="91"/>
       <c r="T27" s="91"/>
       <c r="U27" s="91"/>
       <c r="V27" s="91"/>
-      <c r="W27" s="91"/>
-      <c r="X27" s="92"/>
-      <c r="Y27" s="77"/>
-      <c r="Z27" s="48"/>
-      <c r="AA27" s="58"/>
-      <c r="AB27" s="59"/>
-      <c r="AC27" s="69"/>
-      <c r="AD27" s="70"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W27" s="92"/>
+      <c r="X27" s="77"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="59"/>
+      <c r="AB27" s="69"/>
+      <c r="AC27" s="70"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -5588,27 +6807,26 @@
       <c r="I28" s="128"/>
       <c r="J28" s="128"/>
       <c r="K28" s="124"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="42"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="83"/>
       <c r="N28" s="42"/>
       <c r="O28" s="42"/>
-      <c r="P28" s="135"/>
-      <c r="Q28" s="82"/>
-      <c r="R28" s="109"/>
-      <c r="S28" s="89"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="135"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="91"/>
       <c r="T28" s="91"/>
       <c r="U28" s="91"/>
       <c r="V28" s="91"/>
-      <c r="W28" s="91"/>
-      <c r="X28" s="92"/>
-      <c r="Y28" s="77"/>
-      <c r="Z28" s="48"/>
-      <c r="AA28" s="58"/>
-      <c r="AB28" s="59"/>
-      <c r="AC28" s="69"/>
-      <c r="AD28" s="70"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W28" s="92"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="59"/>
+      <c r="AB28" s="69"/>
+      <c r="AC28" s="70"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -5620,27 +6838,26 @@
       <c r="I29" s="128"/>
       <c r="J29" s="128"/>
       <c r="K29" s="124"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="42"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="83"/>
       <c r="N29" s="42"/>
       <c r="O29" s="42"/>
-      <c r="P29" s="135"/>
-      <c r="Q29" s="82"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="89"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="135"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="91"/>
       <c r="T29" s="91"/>
       <c r="U29" s="91"/>
       <c r="V29" s="91"/>
-      <c r="W29" s="91"/>
-      <c r="X29" s="92"/>
-      <c r="Y29" s="77"/>
-      <c r="Z29" s="48"/>
-      <c r="AA29" s="58"/>
-      <c r="AB29" s="59"/>
-      <c r="AC29" s="69"/>
-      <c r="AD29" s="70"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W29" s="92"/>
+      <c r="X29" s="77"/>
+      <c r="Y29" s="48"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="59"/>
+      <c r="AB29" s="69"/>
+      <c r="AC29" s="70"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -5652,27 +6869,26 @@
       <c r="I30" s="128"/>
       <c r="J30" s="128"/>
       <c r="K30" s="124"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="42"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="83"/>
       <c r="N30" s="42"/>
       <c r="O30" s="42"/>
-      <c r="P30" s="135"/>
-      <c r="Q30" s="82"/>
-      <c r="R30" s="109"/>
-      <c r="S30" s="89"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="135"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="91"/>
       <c r="T30" s="91"/>
       <c r="U30" s="91"/>
       <c r="V30" s="91"/>
-      <c r="W30" s="91"/>
-      <c r="X30" s="92"/>
-      <c r="Y30" s="77"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="58"/>
-      <c r="AB30" s="59"/>
-      <c r="AC30" s="69"/>
-      <c r="AD30" s="70"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W30" s="92"/>
+      <c r="X30" s="77"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="69"/>
+      <c r="AC30" s="70"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -5684,27 +6900,26 @@
       <c r="I31" s="128"/>
       <c r="J31" s="128"/>
       <c r="K31" s="124"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="42"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
       <c r="N31" s="42"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="135"/>
-      <c r="Q31" s="82"/>
-      <c r="R31" s="109"/>
-      <c r="S31" s="89"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="135"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="91"/>
       <c r="T31" s="91"/>
       <c r="U31" s="91"/>
       <c r="V31" s="91"/>
-      <c r="W31" s="91"/>
-      <c r="X31" s="92"/>
-      <c r="Y31" s="77"/>
-      <c r="Z31" s="48"/>
-      <c r="AA31" s="58"/>
-      <c r="AB31" s="59"/>
-      <c r="AC31" s="69"/>
-      <c r="AD31" s="70"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W31" s="92"/>
+      <c r="X31" s="77"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="59"/>
+      <c r="AB31" s="69"/>
+      <c r="AC31" s="70"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -5716,27 +6931,26 @@
       <c r="I32" s="128"/>
       <c r="J32" s="128"/>
       <c r="K32" s="124"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="42"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="83"/>
       <c r="N32" s="42"/>
       <c r="O32" s="42"/>
-      <c r="P32" s="135"/>
-      <c r="Q32" s="82"/>
-      <c r="R32" s="109"/>
-      <c r="S32" s="89"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="135"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="91"/>
       <c r="T32" s="91"/>
       <c r="U32" s="91"/>
       <c r="V32" s="91"/>
-      <c r="W32" s="91"/>
-      <c r="X32" s="92"/>
-      <c r="Y32" s="77"/>
-      <c r="Z32" s="48"/>
-      <c r="AA32" s="58"/>
-      <c r="AB32" s="59"/>
-      <c r="AC32" s="69"/>
-      <c r="AD32" s="70"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W32" s="92"/>
+      <c r="X32" s="77"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="58"/>
+      <c r="AA32" s="59"/>
+      <c r="AB32" s="69"/>
+      <c r="AC32" s="70"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -5748,27 +6962,26 @@
       <c r="I33" s="128"/>
       <c r="J33" s="128"/>
       <c r="K33" s="124"/>
-      <c r="L33" s="83"/>
-      <c r="M33" s="42"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="83"/>
       <c r="N33" s="42"/>
       <c r="O33" s="42"/>
-      <c r="P33" s="135"/>
-      <c r="Q33" s="82"/>
-      <c r="R33" s="109"/>
-      <c r="S33" s="89"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="135"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="91"/>
       <c r="T33" s="91"/>
       <c r="U33" s="91"/>
       <c r="V33" s="91"/>
-      <c r="W33" s="91"/>
-      <c r="X33" s="92"/>
-      <c r="Y33" s="77"/>
-      <c r="Z33" s="48"/>
-      <c r="AA33" s="58"/>
-      <c r="AB33" s="59"/>
-      <c r="AC33" s="69"/>
-      <c r="AD33" s="70"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W33" s="92"/>
+      <c r="X33" s="77"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="58"/>
+      <c r="AA33" s="59"/>
+      <c r="AB33" s="69"/>
+      <c r="AC33" s="70"/>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -5780,27 +6993,26 @@
       <c r="I34" s="128"/>
       <c r="J34" s="128"/>
       <c r="K34" s="124"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="42"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="83"/>
       <c r="N34" s="42"/>
       <c r="O34" s="42"/>
-      <c r="P34" s="135"/>
-      <c r="Q34" s="82"/>
-      <c r="R34" s="109"/>
-      <c r="S34" s="89"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="135"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="91"/>
       <c r="T34" s="91"/>
       <c r="U34" s="91"/>
       <c r="V34" s="91"/>
-      <c r="W34" s="91"/>
-      <c r="X34" s="92"/>
-      <c r="Y34" s="77"/>
-      <c r="Z34" s="48"/>
-      <c r="AA34" s="58"/>
-      <c r="AB34" s="59"/>
-      <c r="AC34" s="69"/>
-      <c r="AD34" s="70"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W34" s="92"/>
+      <c r="X34" s="77"/>
+      <c r="Y34" s="48"/>
+      <c r="Z34" s="58"/>
+      <c r="AA34" s="59"/>
+      <c r="AB34" s="69"/>
+      <c r="AC34" s="70"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -5812,27 +7024,26 @@
       <c r="I35" s="128"/>
       <c r="J35" s="128"/>
       <c r="K35" s="124"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="42"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="83"/>
       <c r="N35" s="42"/>
       <c r="O35" s="42"/>
-      <c r="P35" s="135"/>
-      <c r="Q35" s="82"/>
-      <c r="R35" s="109"/>
-      <c r="S35" s="89"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="135"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="91"/>
       <c r="T35" s="91"/>
       <c r="U35" s="91"/>
       <c r="V35" s="91"/>
-      <c r="W35" s="91"/>
-      <c r="X35" s="92"/>
-      <c r="Y35" s="77"/>
-      <c r="Z35" s="48"/>
-      <c r="AA35" s="58"/>
-      <c r="AB35" s="59"/>
-      <c r="AC35" s="69"/>
-      <c r="AD35" s="70"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W35" s="92"/>
+      <c r="X35" s="77"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="58"/>
+      <c r="AA35" s="59"/>
+      <c r="AB35" s="69"/>
+      <c r="AC35" s="70"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -5844,27 +7055,26 @@
       <c r="I36" s="128"/>
       <c r="J36" s="128"/>
       <c r="K36" s="124"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="42"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="83"/>
       <c r="N36" s="42"/>
       <c r="O36" s="42"/>
-      <c r="P36" s="135"/>
-      <c r="Q36" s="82"/>
-      <c r="R36" s="109"/>
-      <c r="S36" s="89"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="135"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="91"/>
       <c r="T36" s="91"/>
       <c r="U36" s="91"/>
       <c r="V36" s="91"/>
-      <c r="W36" s="91"/>
-      <c r="X36" s="92"/>
-      <c r="Y36" s="77"/>
-      <c r="Z36" s="48"/>
-      <c r="AA36" s="58"/>
-      <c r="AB36" s="59"/>
-      <c r="AC36" s="69"/>
-      <c r="AD36" s="70"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W36" s="92"/>
+      <c r="X36" s="77"/>
+      <c r="Y36" s="48"/>
+      <c r="Z36" s="58"/>
+      <c r="AA36" s="59"/>
+      <c r="AB36" s="69"/>
+      <c r="AC36" s="70"/>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -5876,28 +7086,27 @@
       <c r="I37" s="128"/>
       <c r="J37" s="128"/>
       <c r="K37" s="124"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="42"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="83"/>
       <c r="N37" s="42"/>
       <c r="O37" s="42"/>
-      <c r="P37" s="135"/>
-      <c r="Q37" s="82"/>
-      <c r="R37" s="109"/>
-      <c r="S37" s="89"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="135"/>
+      <c r="R37" s="89"/>
+      <c r="S37" s="91"/>
       <c r="T37" s="91"/>
       <c r="U37" s="91"/>
       <c r="V37" s="91"/>
-      <c r="W37" s="91"/>
-      <c r="X37" s="92"/>
-      <c r="Y37" s="77"/>
-      <c r="Z37" s="48"/>
-      <c r="AA37" s="58"/>
-      <c r="AB37" s="59"/>
-      <c r="AC37" s="69"/>
-      <c r="AD37" s="70"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A38" s="91"/>
+      <c r="W37" s="92"/>
+      <c r="X37" s="77"/>
+      <c r="Y37" s="48"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="59"/>
+      <c r="AB37" s="69"/>
+      <c r="AC37" s="70"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" s="104"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
       <c r="D38" s="144"/>
@@ -5908,28 +7117,27 @@
       <c r="I38" s="128"/>
       <c r="J38" s="128"/>
       <c r="K38" s="124"/>
-      <c r="L38" s="83"/>
-      <c r="M38" s="42"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
       <c r="N38" s="42"/>
       <c r="O38" s="42"/>
-      <c r="P38" s="135"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="109"/>
-      <c r="S38" s="89"/>
+      <c r="P38" s="42"/>
+      <c r="Q38" s="135"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="91"/>
       <c r="T38" s="91"/>
       <c r="U38" s="91"/>
       <c r="V38" s="91"/>
-      <c r="W38" s="91"/>
-      <c r="X38" s="92"/>
-      <c r="Y38" s="77"/>
-      <c r="Z38" s="48"/>
-      <c r="AA38" s="58"/>
-      <c r="AB38" s="59"/>
-      <c r="AC38" s="69"/>
-      <c r="AD38" s="70"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A39" s="91"/>
+      <c r="W38" s="92"/>
+      <c r="X38" s="77"/>
+      <c r="Y38" s="48"/>
+      <c r="Z38" s="58"/>
+      <c r="AA38" s="59"/>
+      <c r="AB38" s="69"/>
+      <c r="AC38" s="70"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
       <c r="D39" s="144"/>
@@ -5940,27 +7148,26 @@
       <c r="I39" s="128"/>
       <c r="J39" s="128"/>
       <c r="K39" s="124"/>
-      <c r="L39" s="83"/>
-      <c r="M39" s="42"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="83"/>
       <c r="N39" s="42"/>
       <c r="O39" s="42"/>
-      <c r="P39" s="135"/>
-      <c r="Q39" s="82"/>
-      <c r="R39" s="109"/>
-      <c r="S39" s="89"/>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="135"/>
+      <c r="R39" s="89"/>
+      <c r="S39" s="91"/>
       <c r="T39" s="91"/>
       <c r="U39" s="91"/>
       <c r="V39" s="91"/>
-      <c r="W39" s="91"/>
-      <c r="X39" s="92"/>
-      <c r="Y39" s="77"/>
-      <c r="Z39" s="48"/>
-      <c r="AA39" s="58"/>
-      <c r="AB39" s="59"/>
-      <c r="AC39" s="69"/>
-      <c r="AD39" s="70"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W39" s="92"/>
+      <c r="X39" s="77"/>
+      <c r="Y39" s="48"/>
+      <c r="Z39" s="58"/>
+      <c r="AA39" s="59"/>
+      <c r="AB39" s="69"/>
+      <c r="AC39" s="70"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -5972,27 +7179,26 @@
       <c r="I40" s="128"/>
       <c r="J40" s="128"/>
       <c r="K40" s="124"/>
-      <c r="L40" s="83"/>
-      <c r="M40" s="42"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="83"/>
       <c r="N40" s="42"/>
       <c r="O40" s="42"/>
-      <c r="P40" s="135"/>
-      <c r="Q40" s="82"/>
-      <c r="R40" s="109"/>
-      <c r="S40" s="89"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="135"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="91"/>
       <c r="T40" s="91"/>
       <c r="U40" s="91"/>
       <c r="V40" s="91"/>
-      <c r="W40" s="91"/>
-      <c r="X40" s="92"/>
-      <c r="Y40" s="77"/>
-      <c r="Z40" s="48"/>
-      <c r="AA40" s="58"/>
-      <c r="AB40" s="59"/>
-      <c r="AC40" s="69"/>
-      <c r="AD40" s="70"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W40" s="92"/>
+      <c r="X40" s="77"/>
+      <c r="Y40" s="48"/>
+      <c r="Z40" s="58"/>
+      <c r="AA40" s="59"/>
+      <c r="AB40" s="69"/>
+      <c r="AC40" s="70"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -6004,27 +7210,26 @@
       <c r="I41" s="128"/>
       <c r="J41" s="128"/>
       <c r="K41" s="124"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="42"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="83"/>
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
-      <c r="P41" s="135"/>
-      <c r="Q41" s="82"/>
-      <c r="R41" s="109"/>
-      <c r="S41" s="89"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="135"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="91"/>
       <c r="T41" s="91"/>
       <c r="U41" s="91"/>
       <c r="V41" s="91"/>
-      <c r="W41" s="91"/>
-      <c r="X41" s="92"/>
-      <c r="Y41" s="77"/>
-      <c r="Z41" s="48"/>
-      <c r="AA41" s="58"/>
-      <c r="AB41" s="59"/>
-      <c r="AC41" s="69"/>
-      <c r="AD41" s="70"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W41" s="92"/>
+      <c r="X41" s="77"/>
+      <c r="Y41" s="48"/>
+      <c r="Z41" s="58"/>
+      <c r="AA41" s="59"/>
+      <c r="AB41" s="69"/>
+      <c r="AC41" s="70"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -6036,214 +7241,147 @@
       <c r="I42" s="128"/>
       <c r="J42" s="128"/>
       <c r="K42" s="124"/>
-      <c r="L42" s="83"/>
-      <c r="M42" s="42"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="83"/>
       <c r="N42" s="42"/>
       <c r="O42" s="42"/>
-      <c r="P42" s="135"/>
-      <c r="Q42" s="82"/>
-      <c r="R42" s="109"/>
-      <c r="S42" s="89"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="135"/>
+      <c r="R42" s="89"/>
+      <c r="S42" s="91"/>
       <c r="T42" s="91"/>
       <c r="U42" s="91"/>
       <c r="V42" s="91"/>
-      <c r="W42" s="91"/>
-      <c r="X42" s="92"/>
-      <c r="Y42" s="77"/>
-      <c r="Z42" s="48"/>
-      <c r="AA42" s="58"/>
-      <c r="AB42" s="59"/>
-      <c r="AC42" s="69"/>
-      <c r="AD42" s="70"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A43" s="104"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="103"/>
-      <c r="D43" s="144"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="128"/>
-      <c r="G43" s="128"/>
-      <c r="H43" s="128"/>
-      <c r="I43" s="128"/>
-      <c r="J43" s="128"/>
-      <c r="K43" s="124"/>
-      <c r="L43" s="83"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="135"/>
-      <c r="Q43" s="82"/>
-      <c r="R43" s="109"/>
-      <c r="S43" s="89"/>
-      <c r="T43" s="91"/>
-      <c r="U43" s="91"/>
-      <c r="V43" s="91"/>
-      <c r="W43" s="91"/>
-      <c r="X43" s="92"/>
-      <c r="Y43" s="77"/>
-      <c r="Z43" s="48"/>
-      <c r="AA43" s="58"/>
-      <c r="AB43" s="59"/>
-      <c r="AC43" s="69"/>
-      <c r="AD43" s="70"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A44" s="104"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="103"/>
-      <c r="D44" s="144"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="128"/>
-      <c r="G44" s="128"/>
-      <c r="H44" s="128"/>
-      <c r="I44" s="128"/>
-      <c r="J44" s="128"/>
-      <c r="K44" s="124"/>
-      <c r="L44" s="83"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="42"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="135"/>
-      <c r="Q44" s="82"/>
-      <c r="R44" s="109"/>
-      <c r="S44" s="89"/>
-      <c r="T44" s="91"/>
-      <c r="U44" s="91"/>
-      <c r="V44" s="91"/>
-      <c r="W44" s="91"/>
-      <c r="X44" s="92"/>
-      <c r="Y44" s="77"/>
-      <c r="Z44" s="48"/>
-      <c r="AA44" s="58"/>
-      <c r="AB44" s="59"/>
-      <c r="AC44" s="69"/>
-      <c r="AD44" s="70"/>
-    </row>
-    <row r="45" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="105"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="106"/>
-      <c r="D45" s="145"/>
-      <c r="E45" s="121"/>
-      <c r="F45" s="129"/>
-      <c r="G45" s="129"/>
-      <c r="H45" s="129"/>
-      <c r="I45" s="129"/>
-      <c r="J45" s="129"/>
-      <c r="K45" s="125"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="130"/>
-      <c r="N45" s="130"/>
-      <c r="O45" s="130"/>
-      <c r="P45" s="136"/>
-      <c r="Q45" s="138"/>
-      <c r="R45" s="110"/>
-      <c r="S45" s="93"/>
-      <c r="T45" s="94"/>
-      <c r="U45" s="94"/>
-      <c r="V45" s="94"/>
-      <c r="W45" s="94"/>
-      <c r="X45" s="95"/>
-      <c r="Y45" s="78"/>
-      <c r="Z45" s="49"/>
-      <c r="AA45" s="60"/>
-      <c r="AB45" s="61"/>
-      <c r="AC45" s="71"/>
-      <c r="AD45" s="72"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M46" s="39"/>
+      <c r="W42" s="92"/>
+      <c r="X42" s="77"/>
+      <c r="Y42" s="48"/>
+      <c r="Z42" s="58"/>
+      <c r="AA42" s="59"/>
+      <c r="AB42" s="69"/>
+      <c r="AC42" s="70"/>
+    </row>
+    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="105"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="129"/>
+      <c r="K43" s="125"/>
+      <c r="L43" s="138"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="130"/>
+      <c r="O43" s="130"/>
+      <c r="P43" s="130"/>
+      <c r="Q43" s="136"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="94"/>
+      <c r="T43" s="94"/>
+      <c r="U43" s="94"/>
+      <c r="V43" s="94"/>
+      <c r="W43" s="95"/>
+      <c r="X43" s="78"/>
+      <c r="Y43" s="49"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="61"/>
+      <c r="AB43" s="71"/>
+      <c r="AC43" s="72"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M47" s="39"/>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L47" s="39"/>
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M48" s="39"/>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L48" s="39"/>
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
     </row>
-    <row r="49" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M49" s="39"/>
+    <row r="49" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L49" s="39"/>
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
     </row>
-    <row r="50" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M50" s="39"/>
+    <row r="50" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
     </row>
-    <row r="51" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M51" s="39"/>
+    <row r="51" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
       <c r="Q51" s="39"/>
     </row>
-    <row r="52" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M52" s="39"/>
+    <row r="52" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L52" s="39"/>
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
       <c r="P52" s="39"/>
       <c r="Q52" s="39"/>
     </row>
-    <row r="53" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M53" s="39"/>
+    <row r="53" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L53" s="39"/>
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
       <c r="P53" s="39"/>
       <c r="Q53" s="39"/>
     </row>
-    <row r="54" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M54" s="39"/>
+    <row r="54" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L54" s="39"/>
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
       <c r="P54" s="39"/>
       <c r="Q54" s="39"/>
     </row>
-    <row r="55" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="39"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
-    </row>
-    <row r="56" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="39"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="39"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L45" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M12" xr:uid="{23831FAC-6AA8-4ACF-9F2C-5A870A089751}">
+      <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:M43" xr:uid="{E21FAC0E-4177-47D6-A1D7-9A22A467BEDB}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L12" xr:uid="{A8837422-8676-43AE-8FBF-E37D051E89A9}">
-      <formula1>"not run, running, run but not analyzed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD7D549-C187-4DCD-8DD0-20217DC34E3E}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -6553,12 +7691,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E03EF-3489-4384-AA19-0C78DA3254C7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6575,12 +7713,36 @@
         <v>162</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="39"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="39"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="39"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="39"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="39"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -7182,7 +8344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update sampling and add expected kin pairs
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2FA09F-A392-42D9-89AC-E48A40F5BE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79613192-CD3A-4C0B-896D-0A5C333B3FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="306">
   <si>
     <t>Date run</t>
   </si>
@@ -1052,6 +1052,50 @@
   </si>
   <si>
     <t>Again, doesn't change much from the HS|PO model, prob because there are not many POs relative to half-sibs.</t>
+  </si>
+  <si>
+    <t>HS.only_all.comps_refined.samples.R</t>
+  </si>
+  <si>
+    <t>HS.only_refined.samples_all.comps</t>
+  </si>
+  <si>
+    <t>HS.only_downsample_refined.samples.R</t>
+  </si>
+  <si>
+    <t>HS.only_refined.samples_downsample</t>
+  </si>
+  <si>
+    <t>HS.PO_all.comps_refined.samples.R</t>
+  </si>
+  <si>
+    <t>HS.PO_downsample_refined.samples.R</t>
+  </si>
+  <si>
+    <t>HS.PO_refined.samples_downsample</t>
+  </si>
+  <si>
+    <t>HS.PO_refined.samples_all.comps</t>
+  </si>
+  <si>
+    <t>Focused on sampling only YOY for four years. Also added expected kin pairs.
+Down-samples if &gt; 150 HSPs.
+HS.PO model</t>
+  </si>
+  <si>
+    <t>Focused on sampling only YOY for four years. Also added expected kin pairs.
+Includes all comparisons, no down-sampling.
+HS.PO model</t>
+  </si>
+  <si>
+    <t>Focused on sampling only YOY for four years. Also added expected kin pairs.
+Includes all comparisons, no down-sampling.
+HS.only model</t>
+  </si>
+  <si>
+    <t>Focused on sampling only YOY for four years. Also added expected kin pairs.
+Down-samples if &gt; 150 HSPs.
+HS.only model</t>
   </si>
 </sst>
 </file>
@@ -4328,10 +4372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0949DA-C0C5-4F9C-B1C9-632432E72B29}">
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4550,18 +4594,36 @@
       <c r="AB3" s="69"/>
       <c r="AC3" s="70"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="91"/>
+    <row r="4" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="91" t="s">
+        <v>298</v>
+      </c>
       <c r="B4" s="91"/>
-      <c r="C4" s="103"/>
+      <c r="C4" s="103">
+        <v>44662</v>
+      </c>
       <c r="D4" s="144"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="124"/>
+      <c r="E4" s="120" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" s="128" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I4" s="128">
+        <v>20</v>
+      </c>
+      <c r="J4" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K4" s="124">
+        <v>50000</v>
+      </c>
       <c r="L4" s="82"/>
       <c r="M4" s="83"/>
       <c r="N4" s="42"/>
@@ -4581,18 +4643,36 @@
       <c r="AB4" s="69"/>
       <c r="AC4" s="70"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
+    <row r="5" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="91" t="s">
+        <v>299</v>
+      </c>
       <c r="B5" s="91"/>
-      <c r="C5" s="103"/>
+      <c r="C5" s="103">
+        <v>44662</v>
+      </c>
       <c r="D5" s="144"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="124"/>
+      <c r="E5" s="120" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" s="128" t="s">
+        <v>302</v>
+      </c>
+      <c r="G5" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H5" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="128">
+        <v>20</v>
+      </c>
+      <c r="J5" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K5" s="124">
+        <v>50000</v>
+      </c>
       <c r="L5" s="82"/>
       <c r="M5" s="83"/>
       <c r="N5" s="42"/>
@@ -4612,18 +4692,36 @@
       <c r="AB5" s="69"/>
       <c r="AC5" s="70"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A6" s="91"/>
+    <row r="6" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="91" t="s">
+        <v>294</v>
+      </c>
       <c r="B6" s="91"/>
-      <c r="C6" s="103"/>
+      <c r="C6" s="103">
+        <v>44662</v>
+      </c>
       <c r="D6" s="144"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="124"/>
+      <c r="E6" s="120" t="s">
+        <v>295</v>
+      </c>
+      <c r="F6" s="128" t="s">
+        <v>304</v>
+      </c>
+      <c r="G6" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H6" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I6" s="128">
+        <v>20</v>
+      </c>
+      <c r="J6" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K6" s="124">
+        <v>50000</v>
+      </c>
       <c r="L6" s="82"/>
       <c r="M6" s="83"/>
       <c r="N6" s="42"/>
@@ -4643,18 +4741,36 @@
       <c r="AB6" s="69"/>
       <c r="AC6" s="70"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" s="91"/>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="91" t="s">
+        <v>296</v>
+      </c>
       <c r="B7" s="91"/>
-      <c r="C7" s="103"/>
+      <c r="C7" s="103">
+        <v>44662</v>
+      </c>
       <c r="D7" s="144"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
-      <c r="K7" s="124"/>
+      <c r="E7" s="120" t="s">
+        <v>297</v>
+      </c>
+      <c r="F7" s="128" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="127" t="s">
+        <v>215</v>
+      </c>
+      <c r="I7" s="128">
+        <v>20</v>
+      </c>
+      <c r="J7" s="128">
+        <v>40000</v>
+      </c>
+      <c r="K7" s="124">
+        <v>50000</v>
+      </c>
       <c r="L7" s="82"/>
       <c r="M7" s="83"/>
       <c r="N7" s="42"/>
@@ -5202,7 +5318,7 @@
       <c r="AC24" s="70"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A25" s="104"/>
+      <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
       <c r="D25" s="144"/>
@@ -5356,43 +5472,67 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="105"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="129"/>
-      <c r="G30" s="129"/>
-      <c r="H30" s="129"/>
-      <c r="I30" s="129"/>
-      <c r="J30" s="129"/>
-      <c r="K30" s="125"/>
-      <c r="L30" s="138"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="130"/>
-      <c r="P30" s="130"/>
-      <c r="Q30" s="136"/>
-      <c r="R30" s="93"/>
-      <c r="S30" s="94"/>
-      <c r="T30" s="94"/>
-      <c r="U30" s="94"/>
-      <c r="V30" s="94"/>
-      <c r="W30" s="95"/>
-      <c r="X30" s="78"/>
-      <c r="Y30" s="49"/>
-      <c r="Z30" s="60"/>
-      <c r="AA30" s="61"/>
-      <c r="AB30" s="71"/>
-      <c r="AC30" s="72"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="L31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" s="104"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="124"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="83"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="135"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="92"/>
+      <c r="X30" s="77"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="69"/>
+      <c r="AC30" s="70"/>
+    </row>
+    <row r="31" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="105"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="145"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="129"/>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
+      <c r="K31" s="125"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="130"/>
+      <c r="O31" s="130"/>
+      <c r="P31" s="130"/>
+      <c r="Q31" s="136"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="95"/>
+      <c r="X31" s="78"/>
+      <c r="Y31" s="49"/>
+      <c r="Z31" s="60"/>
+      <c r="AA31" s="61"/>
+      <c r="AB31" s="71"/>
+      <c r="AC31" s="72"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="L32" s="39"/>
@@ -5464,9 +5604,16 @@
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
     </row>
+    <row r="42" spans="12:17" x14ac:dyDescent="0.3">
+      <c r="L42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M30" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M31" xr:uid="{5B23D7C0-0889-4670-BBB0-CA4613C826A2}">
       <formula1>"not run, running, run but not analyzed, convergence assessed, analysis complete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5479,8 +5626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B018C518-579D-41AF-A4D3-5ADE8EC7F546}">
   <dimension ref="A1:AC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update on HP; transfer to other computer
</commit_message>
<xml_diff>
--- a/Simulation_log.xlsx
+++ b/Simulation_log.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79613192-CD3A-4C0B-896D-0A5C333B3FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065D2A5-725E-476D-A77C-EBEA81310FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{24E2991C-2C0C-4843-9426-0DC9EB9B25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayesian_model_validation" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="Reboot_03.22.2022" sheetId="6" r:id="rId2"/>
-    <sheet name="Archived_sims" sheetId="7" r:id="rId3"/>
-    <sheet name="Prior_sensitivity" sheetId="5" state="hidden" r:id="rId4"/>
-    <sheet name="Notes" sheetId="4" r:id="rId5"/>
-    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId6"/>
-    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId7"/>
+    <sheet name="Figures" sheetId="8" r:id="rId3"/>
+    <sheet name="Archived_sims" sheetId="7" r:id="rId4"/>
+    <sheet name="Prior_sensitivity" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Notes" sheetId="4" r:id="rId6"/>
+    <sheet name="Frequentist_scripts" sheetId="1" state="hidden" r:id="rId7"/>
+    <sheet name="Frequentist_notes" sheetId="2" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="320">
   <si>
     <t>Date run</t>
   </si>
@@ -1096,6 +1097,54 @@
     <t>Focused on sampling only YOY for four years. Also added expected kin pairs.
 Down-samples if &gt; 150 HSPs.
 HS.only model</t>
+  </si>
+  <si>
+    <t>Fig number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date generated</t>
+  </si>
+  <si>
+    <t>Figures</t>
+  </si>
+  <si>
+    <t>This tab is a key for file names for figures. The naming convention I am using for figures is "FigX.X_[year.mo.day]"</t>
+  </si>
+  <si>
+    <t>Compares bias and precision of indiscriminate sampling across age classes versus targeted sampling of YOY and supplementary sampling of adults (i.e. no juveniles). Simulations were run over four years of sampling. Sample size was 50 samples per year (200 samples total)</t>
+  </si>
+  <si>
+    <t>all.comps,
+HS.PO_refined.samples_all.comps</t>
+  </si>
+  <si>
+    <t>Associated scripts (purpose)</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Larger sample size (250 individuals per year over 4 years): 
+A and B: Compares precision and accuracy of parameter estimates when sampling is indiscriminate (across age classes) vs targeted (YOY and supplemental adults only) and when all samples are included vs downsampling to ~150 kin pairs total.</t>
+  </si>
+  <si>
+    <t>Larger sample size (250 individuals per year over 4 years): 
+C and D: Compares bias of posterior median of indiscriminate vs targeted sampling and all samples vs downsampling.</t>
+  </si>
+  <si>
+    <t>all.comps,
+HS.PO_downsample,
+HS.PO_refined.samples_all.comps,
+HS.PO_refined.samples_downsample</t>
+  </si>
+  <si>
+    <t>Shows how downsampling reduces the number of kin pairs.</t>
+  </si>
+  <si>
+    <t>Shows how bias accrues as the number of observed kin pairs deviates from expectations at low, moderate, and high sample sizes.</t>
   </si>
 </sst>
 </file>
@@ -1917,7 +1966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2180,6 +2229,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2502,33 +2563,33 @@
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="31.5703125" customWidth="1"/>
     <col min="16" max="16" width="51" customWidth="1"/>
-    <col min="17" max="17" width="49.6640625" style="39" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="17" max="17" width="49.7109375" style="39" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -2617,7 +2678,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>106</v>
       </c>
@@ -2668,7 +2729,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>107</v>
       </c>
@@ -2719,7 +2780,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
         <v>108</v>
       </c>
@@ -2770,7 +2831,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
@@ -2819,7 +2880,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
@@ -2872,7 +2933,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
@@ -2919,7 +2980,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91" t="s">
         <v>128</v>
       </c>
@@ -2952,7 +3013,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>129</v>
       </c>
@@ -2999,7 +3060,7 @@
       <c r="AB9" s="67"/>
       <c r="AC9" s="68"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
         <v>131</v>
       </c>
@@ -3056,7 +3117,7 @@
       <c r="AB10" s="67"/>
       <c r="AC10" s="68"/>
     </row>
-    <row r="11" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>144</v>
       </c>
@@ -3109,7 +3170,7 @@
       <c r="AB11" s="67"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="90" t="s">
         <v>146</v>
       </c>
@@ -3168,7 +3229,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
         <v>152</v>
       </c>
@@ -3229,7 +3290,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>178</v>
       </c>
@@ -3288,7 +3349,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>134</v>
       </c>
@@ -3349,7 +3410,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="90" t="s">
         <v>134</v>
       </c>
@@ -3410,7 +3471,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="91" t="s">
         <v>193</v>
       </c>
@@ -3473,7 +3534,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
         <v>202</v>
       </c>
@@ -3522,7 +3583,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="91" t="s">
         <v>202</v>
       </c>
@@ -3571,7 +3632,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
         <v>205</v>
       </c>
@@ -3606,7 +3667,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -3637,7 +3698,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -3668,7 +3729,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -3699,7 +3760,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -3730,7 +3791,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -3761,7 +3822,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -3792,7 +3853,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -3823,7 +3884,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -3854,7 +3915,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -3885,7 +3946,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -3916,7 +3977,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -3947,7 +4008,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -3978,7 +4039,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -4009,7 +4070,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -4040,7 +4101,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -4071,7 +4132,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -4102,7 +4163,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -4133,7 +4194,7 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="91"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -4164,7 +4225,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -4195,7 +4256,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -4226,7 +4287,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -4257,7 +4318,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -4288,7 +4349,7 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="104"/>
       <c r="B43" s="91"/>
       <c r="C43" s="103"/>
@@ -4319,7 +4380,7 @@
       <c r="AB43" s="69"/>
       <c r="AC43" s="70"/>
     </row>
-    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="105"/>
       <c r="B44" s="94"/>
       <c r="C44" s="106"/>
@@ -4374,36 +4435,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0949DA-C0C5-4F9C-B1C9-632432E72B29}">
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="7" width="39.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="7" width="39.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="31.5546875" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5703125" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -4492,7 +4553,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
         <v>268</v>
       </c>
@@ -4543,7 +4604,7 @@
       <c r="AB2" s="67"/>
       <c r="AC2" s="68"/>
     </row>
-    <row r="3" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
         <v>274</v>
       </c>
@@ -4551,7 +4612,9 @@
       <c r="C3" s="103">
         <v>44658</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="144">
+        <v>44657</v>
+      </c>
       <c r="E3" s="120" t="s">
         <v>276</v>
       </c>
@@ -4594,7 +4657,7 @@
       <c r="AB3" s="69"/>
       <c r="AC3" s="70"/>
     </row>
-    <row r="4" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="91" t="s">
         <v>298</v>
       </c>
@@ -4602,7 +4665,9 @@
       <c r="C4" s="103">
         <v>44662</v>
       </c>
-      <c r="D4" s="144"/>
+      <c r="D4" s="144">
+        <v>44663</v>
+      </c>
       <c r="E4" s="120" t="s">
         <v>301</v>
       </c>
@@ -4643,7 +4708,7 @@
       <c r="AB4" s="69"/>
       <c r="AC4" s="70"/>
     </row>
-    <row r="5" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>299</v>
       </c>
@@ -4651,7 +4716,9 @@
       <c r="C5" s="103">
         <v>44662</v>
       </c>
-      <c r="D5" s="144"/>
+      <c r="D5" s="144">
+        <v>44663</v>
+      </c>
       <c r="E5" s="120" t="s">
         <v>300</v>
       </c>
@@ -4692,7 +4759,7 @@
       <c r="AB5" s="69"/>
       <c r="AC5" s="70"/>
     </row>
-    <row r="6" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>294</v>
       </c>
@@ -4700,7 +4767,9 @@
       <c r="C6" s="103">
         <v>44662</v>
       </c>
-      <c r="D6" s="144"/>
+      <c r="D6" s="144">
+        <v>44663</v>
+      </c>
       <c r="E6" s="120" t="s">
         <v>295</v>
       </c>
@@ -4741,7 +4810,7 @@
       <c r="AB6" s="69"/>
       <c r="AC6" s="70"/>
     </row>
-    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>296</v>
       </c>
@@ -4749,7 +4818,9 @@
       <c r="C7" s="103">
         <v>44662</v>
       </c>
-      <c r="D7" s="144"/>
+      <c r="D7" s="144">
+        <v>44663</v>
+      </c>
       <c r="E7" s="120" t="s">
         <v>297</v>
       </c>
@@ -4790,7 +4861,7 @@
       <c r="AB7" s="69"/>
       <c r="AC7" s="70"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="91"/>
       <c r="B8" s="91"/>
       <c r="C8" s="103"/>
@@ -4821,7 +4892,7 @@
       <c r="AB8" s="69"/>
       <c r="AC8" s="70"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="91"/>
       <c r="B9" s="91"/>
       <c r="C9" s="103"/>
@@ -4852,7 +4923,7 @@
       <c r="AB9" s="69"/>
       <c r="AC9" s="70"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="91"/>
       <c r="B10" s="91"/>
       <c r="C10" s="103"/>
@@ -4883,7 +4954,7 @@
       <c r="AB10" s="69"/>
       <c r="AC10" s="70"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="91"/>
       <c r="B11" s="91"/>
       <c r="C11" s="103"/>
@@ -4914,7 +4985,7 @@
       <c r="AB11" s="69"/>
       <c r="AC11" s="70"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="91"/>
       <c r="B12" s="91"/>
       <c r="C12" s="103"/>
@@ -4945,7 +5016,7 @@
       <c r="AB12" s="69"/>
       <c r="AC12" s="70"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="91"/>
       <c r="B13" s="91"/>
       <c r="C13" s="103"/>
@@ -4976,7 +5047,7 @@
       <c r="AB13" s="69"/>
       <c r="AC13" s="70"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="91"/>
       <c r="B14" s="91"/>
       <c r="C14" s="103"/>
@@ -5007,7 +5078,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="91"/>
       <c r="B15" s="91"/>
       <c r="C15" s="103"/>
@@ -5038,7 +5109,7 @@
       <c r="AB15" s="69"/>
       <c r="AC15" s="70"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="91"/>
       <c r="B16" s="91"/>
       <c r="C16" s="103"/>
@@ -5069,7 +5140,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
@@ -5100,7 +5171,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -5131,7 +5202,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -5162,7 +5233,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -5193,7 +5264,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -5224,7 +5295,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -5255,7 +5326,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -5286,7 +5357,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -5317,7 +5388,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -5348,7 +5419,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -5379,7 +5450,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="104"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -5410,7 +5481,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="104"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -5441,7 +5512,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="104"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -5472,7 +5543,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="104"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -5503,7 +5574,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="105"/>
       <c r="B31" s="94"/>
       <c r="C31" s="106"/>
@@ -5534,77 +5605,77 @@
       <c r="AB31" s="71"/>
       <c r="AC31" s="72"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
     </row>
-    <row r="33" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L33" s="39"/>
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
     </row>
-    <row r="34" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
     </row>
-    <row r="35" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L35" s="39"/>
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="39"/>
     </row>
-    <row r="36" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
     </row>
-    <row r="37" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L37" s="39"/>
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
     </row>
-    <row r="38" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L38" s="39"/>
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
     </row>
-    <row r="39" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L39" s="39"/>
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
     </row>
-    <row r="40" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L40" s="39"/>
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
       <c r="P40" s="39"/>
       <c r="Q40" s="39"/>
     </row>
-    <row r="41" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L41" s="39"/>
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
     </row>
-    <row r="42" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L42" s="39"/>
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
@@ -5623,6 +5694,310 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062A0465-36AA-48A3-BB7A-61F0737D9C02}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="4" width="73.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="149" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="149" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" s="149" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="149" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" s="149" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="147">
+        <v>1</v>
+      </c>
+      <c r="B2" s="148">
+        <v>44664</v>
+      </c>
+      <c r="C2" s="150" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" s="150"/>
+      <c r="E2" s="39" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="147">
+        <v>2.1</v>
+      </c>
+      <c r="B3" s="148">
+        <v>44664</v>
+      </c>
+      <c r="C3" s="150" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="150"/>
+      <c r="E3" s="39" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="147">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B4" s="148">
+        <v>44664</v>
+      </c>
+      <c r="C4" s="150" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="150"/>
+      <c r="E4" s="39" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="147">
+        <v>3</v>
+      </c>
+      <c r="B5" s="148">
+        <v>44659</v>
+      </c>
+      <c r="C5" s="150" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" s="150"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="147">
+        <v>4</v>
+      </c>
+      <c r="B6" s="148">
+        <v>44665</v>
+      </c>
+      <c r="C6" s="150" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="150"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="147"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="147"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="150"/>
+      <c r="D8" s="150"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="147"/>
+      <c r="B9" s="147"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="150"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="147"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="150"/>
+      <c r="D10" s="150"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="147"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="147"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="147"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="150"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="147"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="147"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="147"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="150"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="147"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="150"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="147"/>
+      <c r="B18" s="147"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="150"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="147"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="147"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="147"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="150"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="147"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="147"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="150"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="147"/>
+      <c r="B24" s="147"/>
+      <c r="C24" s="150"/>
+      <c r="D24" s="150"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B018C518-579D-41AF-A4D3-5ADE8EC7F546}">
   <dimension ref="A1:AC54"/>
   <sheetViews>
@@ -5630,32 +6005,32 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="31.5546875" customWidth="1"/>
-    <col min="18" max="21" width="19.5546875" customWidth="1"/>
-    <col min="22" max="23" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="31.5703125" customWidth="1"/>
+    <col min="18" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="25.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>105</v>
       </c>
@@ -5744,7 +6119,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>213</v>
       </c>
@@ -5805,7 +6180,7 @@
       <c r="AB2" s="63"/>
       <c r="AC2" s="64"/>
     </row>
-    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>221</v>
       </c>
@@ -5866,7 +6241,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="66"/>
     </row>
-    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
         <v>220</v>
       </c>
@@ -5927,7 +6302,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="66"/>
     </row>
-    <row r="5" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>219</v>
       </c>
@@ -5988,7 +6363,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="66"/>
     </row>
-    <row r="6" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="91" t="s">
         <v>213</v>
       </c>
@@ -6051,7 +6426,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="66"/>
     </row>
-    <row r="7" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="91" t="s">
         <v>242</v>
       </c>
@@ -6114,7 +6489,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="91" t="s">
         <v>221</v>
       </c>
@@ -6177,7 +6552,7 @@
       <c r="AB8" s="65"/>
       <c r="AC8" s="66"/>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>213</v>
       </c>
@@ -6230,7 +6605,7 @@
       <c r="AB9" s="65"/>
       <c r="AC9" s="66"/>
     </row>
-    <row r="10" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
         <v>242</v>
       </c>
@@ -6283,7 +6658,7 @@
       <c r="AB10" s="65"/>
       <c r="AC10" s="66"/>
     </row>
-    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>221</v>
       </c>
@@ -6336,7 +6711,7 @@
       <c r="AB11" s="65"/>
       <c r="AC11" s="66"/>
     </row>
-    <row r="12" spans="1:29" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="91" t="s">
         <v>260</v>
       </c>
@@ -6391,7 +6766,7 @@
       <c r="AB12" s="67"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
         <v>269</v>
       </c>
@@ -6444,7 +6819,7 @@
       <c r="AB13" s="67"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>270</v>
       </c>
@@ -6497,7 +6872,7 @@
       <c r="AB14" s="69"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="91" t="s">
         <v>271</v>
       </c>
@@ -6550,7 +6925,7 @@
       <c r="AB15" s="67"/>
       <c r="AC15" s="68"/>
     </row>
-    <row r="16" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="91" t="s">
         <v>275</v>
       </c>
@@ -6601,7 +6976,7 @@
       <c r="AB16" s="69"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="91"/>
       <c r="C17" s="103"/>
@@ -6632,7 +7007,7 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="91"/>
       <c r="C18" s="103"/>
@@ -6663,7 +7038,7 @@
       <c r="AB18" s="69"/>
       <c r="AC18" s="70"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="91"/>
       <c r="B19" s="91"/>
       <c r="C19" s="103"/>
@@ -6694,7 +7069,7 @@
       <c r="AB19" s="69"/>
       <c r="AC19" s="70"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="91"/>
       <c r="B20" s="91"/>
       <c r="C20" s="103"/>
@@ -6725,7 +7100,7 @@
       <c r="AB20" s="69"/>
       <c r="AC20" s="70"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="91"/>
       <c r="B21" s="91"/>
       <c r="C21" s="103"/>
@@ -6756,7 +7131,7 @@
       <c r="AB21" s="69"/>
       <c r="AC21" s="70"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
       <c r="B22" s="91"/>
       <c r="C22" s="103"/>
@@ -6787,7 +7162,7 @@
       <c r="AB22" s="69"/>
       <c r="AC22" s="70"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="91"/>
       <c r="B23" s="91"/>
       <c r="C23" s="103"/>
@@ -6818,7 +7193,7 @@
       <c r="AB23" s="69"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="91"/>
       <c r="B24" s="91"/>
       <c r="C24" s="103"/>
@@ -6849,7 +7224,7 @@
       <c r="AB24" s="69"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="91"/>
       <c r="B25" s="91"/>
       <c r="C25" s="103"/>
@@ -6880,7 +7255,7 @@
       <c r="AB25" s="69"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="91"/>
       <c r="B26" s="91"/>
       <c r="C26" s="103"/>
@@ -6911,7 +7286,7 @@
       <c r="AB26" s="69"/>
       <c r="AC26" s="70"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="91"/>
       <c r="C27" s="103"/>
@@ -6942,7 +7317,7 @@
       <c r="AB27" s="69"/>
       <c r="AC27" s="70"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="91"/>
       <c r="B28" s="91"/>
       <c r="C28" s="103"/>
@@ -6973,7 +7348,7 @@
       <c r="AB28" s="69"/>
       <c r="AC28" s="70"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="91"/>
       <c r="C29" s="103"/>
@@ -7004,7 +7379,7 @@
       <c r="AB29" s="69"/>
       <c r="AC29" s="70"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="91"/>
       <c r="B30" s="91"/>
       <c r="C30" s="103"/>
@@ -7035,7 +7410,7 @@
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="91"/>
       <c r="C31" s="103"/>
@@ -7066,7 +7441,7 @@
       <c r="AB31" s="69"/>
       <c r="AC31" s="70"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="91"/>
       <c r="C32" s="103"/>
@@ -7097,7 +7472,7 @@
       <c r="AB32" s="69"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="91"/>
       <c r="C33" s="103"/>
@@ -7128,7 +7503,7 @@
       <c r="AB33" s="69"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
       <c r="C34" s="103"/>
@@ -7159,7 +7534,7 @@
       <c r="AB34" s="69"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="91"/>
       <c r="B35" s="91"/>
       <c r="C35" s="103"/>
@@ -7190,7 +7565,7 @@
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="91"/>
       <c r="B36" s="91"/>
       <c r="C36" s="103"/>
@@ -7221,7 +7596,7 @@
       <c r="AB36" s="69"/>
       <c r="AC36" s="70"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="91"/>
       <c r="B37" s="91"/>
       <c r="C37" s="103"/>
@@ -7252,7 +7627,7 @@
       <c r="AB37" s="69"/>
       <c r="AC37" s="70"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="104"/>
       <c r="B38" s="91"/>
       <c r="C38" s="103"/>
@@ -7283,7 +7658,7 @@
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="104"/>
       <c r="B39" s="91"/>
       <c r="C39" s="103"/>
@@ -7314,7 +7689,7 @@
       <c r="AB39" s="69"/>
       <c r="AC39" s="70"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="104"/>
       <c r="B40" s="91"/>
       <c r="C40" s="103"/>
@@ -7345,7 +7720,7 @@
       <c r="AB40" s="69"/>
       <c r="AC40" s="70"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="104"/>
       <c r="B41" s="91"/>
       <c r="C41" s="103"/>
@@ -7376,7 +7751,7 @@
       <c r="AB41" s="69"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="104"/>
       <c r="B42" s="91"/>
       <c r="C42" s="103"/>
@@ -7407,7 +7782,7 @@
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="105"/>
       <c r="B43" s="94"/>
       <c r="C43" s="106"/>
@@ -7438,77 +7813,77 @@
       <c r="AB43" s="71"/>
       <c r="AC43" s="72"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L44" s="39"/>
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L45" s="39"/>
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L47" s="39"/>
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L48" s="39"/>
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
     </row>
-    <row r="49" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L49" s="39"/>
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
     </row>
-    <row r="50" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
     </row>
-    <row r="51" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
       <c r="Q51" s="39"/>
     </row>
-    <row r="52" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L52" s="39"/>
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
       <c r="P52" s="39"/>
       <c r="Q52" s="39"/>
     </row>
-    <row r="53" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L53" s="39"/>
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
       <c r="P53" s="39"/>
       <c r="Q53" s="39"/>
     </row>
-    <row r="54" spans="12:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L54" s="39"/>
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
@@ -7528,7 +7903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD7D549-C187-4DCD-8DD0-20217DC34E3E}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -7536,15 +7911,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
@@ -7561,7 +7936,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="102">
         <v>44578</v>
       </c>
@@ -7575,7 +7950,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="103">
         <v>44582</v>
       </c>
@@ -7592,241 +7967,241 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="103"/>
       <c r="B4" s="120"/>
       <c r="C4" s="128"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="103"/>
       <c r="B5" s="120"/>
       <c r="C5" s="128"/>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="103"/>
       <c r="B6" s="120"/>
       <c r="C6" s="128"/>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="103"/>
       <c r="B7" s="120"/>
       <c r="C7" s="128"/>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="103"/>
       <c r="B8" s="120"/>
       <c r="C8" s="128"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="103"/>
       <c r="B9" s="120"/>
       <c r="C9" s="128"/>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="103"/>
       <c r="B10" s="120"/>
       <c r="C10" s="128"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="103"/>
       <c r="B11" s="120"/>
       <c r="C11" s="128"/>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="103"/>
       <c r="B12" s="120"/>
       <c r="C12" s="128"/>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="103"/>
       <c r="B13" s="120"/>
       <c r="C13" s="128"/>
       <c r="D13" s="42"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="103"/>
       <c r="B14" s="120"/>
       <c r="C14" s="128"/>
       <c r="D14" s="42"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="103"/>
       <c r="B15" s="120"/>
       <c r="C15" s="128"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="103"/>
       <c r="B16" s="120"/>
       <c r="C16" s="128"/>
       <c r="D16" s="42"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="103"/>
       <c r="B17" s="120"/>
       <c r="C17" s="128"/>
       <c r="D17" s="42"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="103"/>
       <c r="B18" s="120"/>
       <c r="C18" s="128"/>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="103"/>
       <c r="B19" s="120"/>
       <c r="C19" s="128"/>
       <c r="D19" s="42"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="103"/>
       <c r="B20" s="120"/>
       <c r="C20" s="128"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="103"/>
       <c r="B21" s="120"/>
       <c r="C21" s="128"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="103"/>
       <c r="B22" s="120"/>
       <c r="C22" s="128"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="103"/>
       <c r="B23" s="120"/>
       <c r="C23" s="128"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="103"/>
       <c r="B24" s="120"/>
       <c r="C24" s="128"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="103"/>
       <c r="B25" s="120"/>
       <c r="C25" s="128"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="103"/>
       <c r="B26" s="120"/>
       <c r="C26" s="128"/>
       <c r="D26" s="42"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="103"/>
       <c r="B27" s="120"/>
       <c r="C27" s="128"/>
       <c r="D27" s="42"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="103"/>
       <c r="B28" s="120"/>
       <c r="C28" s="128"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="103"/>
       <c r="B29" s="120"/>
       <c r="C29" s="128"/>
       <c r="D29" s="42"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="103"/>
       <c r="B30" s="120"/>
       <c r="C30" s="128"/>
       <c r="D30" s="42"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="103"/>
       <c r="B31" s="120"/>
       <c r="C31" s="128"/>
       <c r="D31" s="42"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="103"/>
       <c r="B32" s="120"/>
       <c r="C32" s="128"/>
       <c r="D32" s="42"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="103"/>
       <c r="B33" s="120"/>
       <c r="C33" s="128"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="103"/>
       <c r="B34" s="120"/>
       <c r="C34" s="128"/>
       <c r="D34" s="42"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="103"/>
       <c r="B35" s="120"/>
       <c r="C35" s="128"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="103"/>
       <c r="B36" s="120"/>
       <c r="C36" s="128"/>
       <c r="D36" s="42"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="103"/>
       <c r="B37" s="120"/>
       <c r="C37" s="128"/>
       <c r="D37" s="42"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="103"/>
       <c r="B38" s="120"/>
       <c r="C38" s="128"/>
       <c r="D38" s="42"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="103"/>
       <c r="B39" s="120"/>
       <c r="C39" s="128"/>
       <c r="D39" s="42"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="103"/>
       <c r="B40" s="120"/>
       <c r="C40" s="128"/>
       <c r="D40" s="42"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="103"/>
       <c r="B41" s="120"/>
       <c r="C41" s="128"/>
       <c r="D41" s="42"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="103"/>
       <c r="B42" s="120"/>
       <c r="C42" s="128"/>
       <c r="D42" s="42"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="106"/>
       <c r="B43" s="121"/>
       <c r="C43" s="129"/>
@@ -7838,21 +8213,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E03EF-3489-4384-AA19-0C78DA3254C7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -7860,7 +8235,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>280</v>
       </c>
@@ -7868,19 +8243,24 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="39"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="39"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="39"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
     </row>
   </sheetData>
@@ -7889,7 +8269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63293731-8B9D-4FB7-AC7D-84F6C37DDC98}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -7899,20 +8279,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
@@ -7941,7 +8321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="18" t="s">
@@ -7964,7 +8344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="19" t="s">
@@ -7987,7 +8367,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="19" t="s">
@@ -8008,7 +8388,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
@@ -8035,7 +8415,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
@@ -8060,7 +8440,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
@@ -8085,7 +8465,7 @@
       </c>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>38</v>
       </c>
@@ -8114,7 +8494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
@@ -8141,7 +8521,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8164,7 +8544,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>40</v>
       </c>
@@ -8187,7 +8567,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>38</v>
       </c>
@@ -8212,7 +8592,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="29"/>
       <c r="C13" s="23"/>
@@ -8223,7 +8603,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>40</v>
       </c>
@@ -8248,7 +8628,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>40</v>
       </c>
@@ -8275,7 +8655,7 @@
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
@@ -8302,7 +8682,7 @@
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>40</v>
       </c>
@@ -8327,7 +8707,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
@@ -8354,7 +8734,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>40</v>
       </c>
@@ -8381,7 +8761,7 @@
       </c>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>40</v>
       </c>
@@ -8404,7 +8784,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>40</v>
       </c>
@@ -8429,7 +8809,7 @@
       </c>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -8452,7 +8832,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
@@ -8463,7 +8843,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
@@ -8474,7 +8854,7 @@
       <c r="H24" s="37"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="30"/>
       <c r="C25" s="25"/>
@@ -8491,7 +8871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEF7D91-85A6-4DB4-B86B-47EAF5CFDDD0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -8499,14 +8879,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="1" max="1" width="105.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -8517,7 +8897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>93</v>
       </c>
@@ -8528,7 +8908,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -8536,7 +8916,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>64</v>
       </c>
@@ -8544,7 +8924,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -8552,19 +8932,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="39"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="39"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="39"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="39"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="39"/>
     </row>
   </sheetData>

</xml_diff>